<commit_message>
Consider elastic deviatoric strain, relate characteristic a: q/p with b: dev^e/dev^q using elastic dilation ratio when plastic deformation first introduced
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\My Paper\Geotexile and Geomembrane\anal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t># avgT</t>
   </si>
@@ -104,19 +103,56 @@
   </si>
   <si>
     <t>ev</t>
-  </si>
-  <si>
-    <t>eq</t>
   </si>
   <si>
     <t>K_phi</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>ev_ela</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev_pla</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>er_from_ev</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev_pla</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>D/E</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dratio</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>K_p</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -137,63 +173,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ds_r_pred</t>
+    <t>dev/deq_pred</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ds_a_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>s_r_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>s_a_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_ela</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_pla</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>er_from_ev</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev_pla</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev/deq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ratio^4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dratio</t>
+    <t>eq_pla</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -240,9 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY22"/>
+  <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3:AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -547,16 +534,18 @@
     <col min="19" max="26" width="13.77734375"/>
     <col min="27" max="27" width="12.77734375"/>
     <col min="28" max="28" width="11.5546875"/>
-    <col min="31" max="31" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.109375" customWidth="1"/>
+    <col min="36" max="36" width="12.88671875" customWidth="1"/>
+    <col min="39" max="39" width="8.88671875" style="2"/>
     <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="12.77734375" customWidth="1"/>
     <col min="44" max="44" width="12.44140625" customWidth="1"/>
     <col min="45" max="45" width="11.21875" customWidth="1"/>
-    <col min="52" max="1031" width="11.5546875"/>
+    <col min="48" max="1027" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,76 +631,64 @@
         <v>27</v>
       </c>
       <c r="AC1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.17366852143</v>
       </c>
@@ -805,17 +782,17 @@
         <f>AB2-AC2</f>
         <v>2.4003572443069832E-3</v>
       </c>
-      <c r="AE2">
-        <f>P2-AB2/3</f>
-        <v>9.588996263687477E-10</v>
+      <c r="AE2" s="3">
+        <f>P2-AB2/3-2*(1.35*(AK2/3255000)^-0.0723)*(1+0.33)/(9*(1-2*0.33))</f>
+        <v>-1.9678144869574707</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF18" si="1">AB2-P2/2</f>
         <v>-2.8766988791062431E-9</v>
       </c>
-      <c r="AJ2">
-        <f>(1.35*(AK2/3255000)^-0.0723)^4</f>
-        <v>26.260063640534618</v>
+      <c r="AJ2" s="2" t="e">
+        <f>(( 1.588*EXP(-0.0005387*0.5*232))^2-AP2^2)/(2*AP2)+0.4</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="AK2">
         <f t="shared" ref="AK2:AK18" si="2">(X2+Y2+Z2)/3</f>
@@ -825,9 +802,17 @@
         <f t="shared" ref="AL2:AL18" si="3">Z2-(Y2+X2)/2</f>
         <v>3423.5295013549999</v>
       </c>
-      <c r="AO2">
-        <f t="shared" ref="AO2" si="4">(3*(1-2*0.33))/(0.0762*0.2606*(AK2)^(0.2606-1))</f>
-        <v>16991.336586725814</v>
+      <c r="AM2" s="3" t="e">
+        <f t="shared" ref="AM2:AM18" si="4">(-2*AJ2-3)/(-2*AJ2+6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AN2" t="e">
+        <f t="shared" ref="AN2:AN18" si="5">1/(2+AM2*AQ2-2*0.33*(1+AM2+AQ2))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AO2" s="1" t="e">
+        <f>3*(1-2*0.33)*(AK2-AK1)/(AC2-AC1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="AS2">
         <v>0</v>
@@ -836,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.3863060409200001</v>
       </c>
@@ -923,36 +908,36 @@
         <v>0.42455699990888718</v>
       </c>
       <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC18" si="5">0.0762*AK3^0.2606-0.5912</f>
+        <f t="shared" ref="AC3:AC18" si="6">0.0762*AK3^0.2606-0.5912</f>
         <v>0.41458661901056004</v>
       </c>
       <c r="AD3" s="1">
-        <f t="shared" ref="AD3:AD18" si="6">AB3-AC3</f>
+        <f t="shared" ref="AD3:AD18" si="7">AB3-AC3</f>
         <v>9.9703808983271358E-3</v>
       </c>
-      <c r="AE3" s="1">
-        <f t="shared" ref="AE3:AE18" si="7">P3-AB3/3</f>
-        <v>0.86439544855037098</v>
+      <c r="AE3" s="3">
+        <f t="shared" ref="AE3:AE18" si="8">P3-AB3/3-2*(1.35*(AK3/3255000)^-0.0723)*(1+0.33)/(9*(1-2*0.33))</f>
+        <v>-0.83177500520751779</v>
       </c>
       <c r="AF3" s="1">
         <f t="shared" si="1"/>
         <v>-7.8400224351112824E-2</v>
       </c>
       <c r="AG3" s="1">
-        <f t="shared" ref="AG3:AH18" si="8">AD3-AD2</f>
+        <f t="shared" ref="AG3:AH18" si="9">AD3-AD2</f>
         <v>7.5700236540201526E-3</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="8"/>
-        <v>0.86439544759147136</v>
+        <f t="shared" si="9"/>
+        <v>1.1360394817499531</v>
       </c>
       <c r="AI3" s="1">
         <f>-AG3/AH3</f>
-        <v>-8.7575931538198936E-3</v>
-      </c>
-      <c r="AJ3" s="1">
-        <f>(1.35*(AK3/3255000)^-0.0723)^4</f>
-        <v>14.495631316908813</v>
+        <v>-6.6635216254626135E-3</v>
+      </c>
+      <c r="AJ3" s="2">
+        <f t="shared" ref="AJ3:AJ18" si="10">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
+        <v>3.1368433750215918E-2</v>
       </c>
       <c r="AK3" s="1">
         <f t="shared" si="2"/>
@@ -962,15 +947,16 @@
         <f t="shared" si="3"/>
         <v>26990.528974650002</v>
       </c>
-      <c r="AM3" s="1">
-        <v>-0.49972129302590063</v>
+      <c r="AM3" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.51584994620425884</v>
       </c>
       <c r="AN3" s="1">
-        <f t="shared" ref="AN3:AN18" si="9">1/(2+AM3*AQ3-2*0.33*(1+AM3+AQ3))</f>
-        <v>-0.18033086574903387</v>
+        <f t="shared" si="5"/>
+        <v>-0.17746035224544451</v>
       </c>
       <c r="AO3" s="1">
-        <v>77626.17248935283</v>
+        <v>42530.539337002985</v>
       </c>
       <c r="AP3" s="1">
         <f>(AK3*1.35*(AK3/3255000)^-0.0723-AK2*1.35*(AK2/3255000)^-0.0723)/(AK3-AK2)</f>
@@ -981,39 +967,23 @@
         <v>6.221476214165274</v>
       </c>
       <c r="AR3" s="1">
-        <f>(1+2*AM3)*(AK3-AK2)*(1-AP3/3)/(2*AN3*AO3*AM3)</f>
-        <v>2.5284172742607702E-4</v>
+        <f>(1+2*AM3)*(AK3-AK2)*(1-AP3/3)/(3*AN3*AO3*AM3)</f>
+        <v>-1.7223361727561365E-2</v>
       </c>
       <c r="AS3" s="1">
         <f>(AS2+AR3)</f>
-        <v>2.5284172742607702E-4</v>
+        <v>-1.7223361727561365E-2</v>
       </c>
       <c r="AT3" s="1">
-        <f>(1-AM3)*(AK3-AK2)*(1-AP3/3)/(3*AN3*AO3*AM3)</f>
-        <v>0.45351349580406258</v>
+        <f>2*(1-AM3)*(AK3-AK2)*(1-AP3/3)/(9*AN3*AO3*AM3)</f>
+        <v>0.54906667845482926</v>
       </c>
       <c r="AU3" s="1">
         <f>AU2+AT3</f>
-        <v>0.45351349580406258</v>
-      </c>
-      <c r="AV3" s="1">
-        <f t="shared" ref="AV3:AV18" si="10">AN3*AO3*(AM3*0.01*((AD3-AD2)/3+(AE3-AE2))-2*0.01*((AD3-AD2)/3-(AE3-AE2)/2))</f>
-        <v>-59.651498316853015</v>
-      </c>
-      <c r="AW3" s="1">
-        <f t="shared" ref="AW3:AW18" si="11">AN3*AO3*(AM3*AQ3*0.01*((AD3-AD2)/3+(AE3-AE2))-2*AQ3*0.01*((AD3-AD2)/3-(AE3-AE2)/2))</f>
-        <v>-371.12037791762077</v>
-      </c>
-      <c r="AX3" s="1">
-        <f t="shared" ref="AX3:AX18" si="12">AV3+(AK2-1.35*(AK2/3255000)^-0.0723*AK2/3)</f>
-        <v>567.66580673469991</v>
-      </c>
-      <c r="AY3" s="1">
-        <f t="shared" ref="AY3:AY18" si="13">AW3+(AK2+2*1.35*(AK2/3255000)^-0.0723*AK2/3)</f>
-        <v>6042.3945419292722</v>
+        <v>0.54906667845482926</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.4615371024499999</v>
       </c>
@@ -1100,36 +1070,36 @@
         <v>0.53723081921390747</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.69544295971520387</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.15821214050129639</v>
       </c>
-      <c r="AE4">
-        <f t="shared" si="7"/>
-        <v>1.8270880839220307</v>
+      <c r="AE4" s="3">
+        <f t="shared" si="8"/>
+        <v>0.24293542161306259</v>
       </c>
       <c r="AF4">
         <f t="shared" si="1"/>
         <v>-0.46585169261609249</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.16818252139962353</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="8"/>
-        <v>0.96269263537165972</v>
+        <f t="shared" si="9"/>
+        <v>1.0747104268205803</v>
       </c>
       <c r="AI4">
-        <f t="shared" ref="AI4:AI18" si="14">-AG4/AH4</f>
-        <v>0.17470012257307291</v>
-      </c>
-      <c r="AJ4">
-        <f t="shared" ref="AJ4:AJ18" si="15">(1.35*(AK4/3255000)^-0.0723)^4</f>
-        <v>11.029283131660142</v>
+        <f t="shared" ref="AI4:AI18" si="11">-AG4/AH4</f>
+        <v>0.15649101116211753</v>
+      </c>
+      <c r="AJ4" s="2">
+        <f t="shared" si="10"/>
+        <v>0.16912422089899823</v>
       </c>
       <c r="AK4">
         <f t="shared" si="2"/>
@@ -1139,59 +1109,43 @@
         <f t="shared" si="3"/>
         <v>72940.740784349997</v>
       </c>
-      <c r="AM4">
-        <f t="shared" ref="AM4:AM18" si="16">(-2*AI4-3)/(-2*AI4+6)</f>
-        <v>-0.59275128136071176</v>
+      <c r="AM4" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.58961408099265322</v>
       </c>
       <c r="AN4">
-        <f t="shared" si="9"/>
-        <v>-0.21210580576908009</v>
-      </c>
-      <c r="AO4" s="1">
-        <v>77626.17248935283</v>
+        <f t="shared" si="5"/>
+        <v>-0.21274075919304949</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>42530.539337002985</v>
       </c>
       <c r="AP4">
-        <f t="shared" ref="AP4:AP18" si="17">(AK4*1.35*(AK4/3255000)^-0.0723-AK3*1.35*(AK3/3255000)^-0.0723)/(AK4-AK3)</f>
+        <f t="shared" ref="AP4:AP18" si="12">(AK4*1.35*(AK4/3255000)^-0.0723-AK3*1.35*(AK3/3255000)^-0.0723)/(AK4-AK3)</f>
         <v>1.7404396115775711</v>
       </c>
       <c r="AQ4">
-        <f t="shared" ref="AQ4:AQ18" si="18">(2*AP4+3)/(3-AP4)</f>
+        <f t="shared" ref="AQ4:AQ18" si="13">(2*AP4+3)/(3-AP4)</f>
         <v>5.1453501417842284</v>
       </c>
-      <c r="AR4">
-        <f t="shared" ref="AR4:AR18" si="19">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(2*AN4*AO4*AM4)</f>
-        <v>-0.12518393613015869</v>
+      <c r="AR4" s="1">
+        <f t="shared" ref="AR4:AR18" si="14">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
+        <v>-0.14751204037394886</v>
       </c>
       <c r="AS4">
-        <f t="shared" ref="AS4:AS18" si="20">AS3+AR4</f>
-        <v>-0.1249310944027326</v>
-      </c>
-      <c r="AT4">
-        <f t="shared" ref="AT4:AT18" si="21">(1-AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
-        <v>0.71656467257369683</v>
+        <f t="shared" ref="AS4:AS18" si="15">AS3+AR4</f>
+        <v>-0.16473540210151022</v>
+      </c>
+      <c r="AT4" s="1">
+        <f t="shared" ref="AT4:AT18" si="16">2*(1-AM4)*(AK4-AK3)*(1-AP4/3)/(9*AN4*AO4*AM4)</f>
+        <v>0.87221120422511</v>
       </c>
       <c r="AU4">
         <f>AU3+AT4</f>
-        <v>1.1700781683777595</v>
-      </c>
-      <c r="AV4">
-        <f t="shared" si="10"/>
-        <v>-88.483883647546293</v>
-      </c>
-      <c r="AW4">
-        <f t="shared" si="11"/>
-        <v>-455.28056327152149</v>
-      </c>
-      <c r="AX4">
-        <f t="shared" si="12"/>
-        <v>6884.9348379544481</v>
-      </c>
-      <c r="AY4">
-        <f t="shared" si="13"/>
-        <v>45440.353372324491</v>
+        <v>1.4212778826799393</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.0730406484000001</v>
       </c>
@@ -1278,36 +1232,36 @@
         <v>0.57836850681094454</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.90101321517751964</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.32264470836657511</v>
       </c>
-      <c r="AE5">
-        <f t="shared" si="7"/>
-        <v>2.8131835652496848</v>
+      <c r="AE5" s="3">
+        <f t="shared" si="8"/>
+        <v>1.292854333240729</v>
       </c>
       <c r="AF5">
         <f t="shared" si="1"/>
         <v>-0.92461802694905537</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.16443256786527871</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="8"/>
-        <v>0.98609548132765412</v>
+        <f t="shared" si="9"/>
+        <v>1.0499189116276664</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="14"/>
-        <v>0.16675116251814767</v>
-      </c>
-      <c r="AJ5">
-        <f t="shared" si="15"/>
-        <v>9.3564207450334393</v>
+        <f t="shared" si="11"/>
+        <v>0.15661454046042708</v>
+      </c>
+      <c r="AJ5" s="2">
+        <f t="shared" si="10"/>
+        <v>0.2465601787796606</v>
       </c>
       <c r="AK5">
         <f t="shared" si="2"/>
@@ -1317,59 +1271,43 @@
         <f t="shared" si="3"/>
         <v>131416.95121849998</v>
       </c>
-      <c r="AM5">
+      <c r="AM5" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.63431935767006364</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="5"/>
+        <v>-0.23247936597521568</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="12"/>
+        <v>1.6531141584289157</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="13"/>
+        <v>4.6820807838486802</v>
+      </c>
+      <c r="AR5" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.25202903888975065</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" si="15"/>
+        <v>-0.41676444099126086</v>
+      </c>
+      <c r="AT5" s="1">
         <f t="shared" si="16"/>
-        <v>-0.58828265998673457</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" si="9"/>
-        <v>-0.24293698967854016</v>
-      </c>
-      <c r="AO5" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP5">
-        <f t="shared" si="17"/>
-        <v>1.6531141584289157</v>
-      </c>
-      <c r="AQ5">
-        <f t="shared" si="18"/>
-        <v>4.6820807838486802</v>
-      </c>
-      <c r="AR5">
-        <f t="shared" si="19"/>
-        <v>-0.14047015051070563</v>
-      </c>
-      <c r="AS5">
-        <f t="shared" si="20"/>
-        <v>-0.26540124491343825</v>
-      </c>
-      <c r="AT5">
-        <f t="shared" si="21"/>
-        <v>0.84239383036036253</v>
+        <v>1.0221806300480394</v>
       </c>
       <c r="AU5">
         <f>AU4+AT5</f>
-        <v>2.0124719987381221</v>
-      </c>
-      <c r="AV5">
-        <f t="shared" si="10"/>
-        <v>-103.31664605376587</v>
-      </c>
-      <c r="AW5">
-        <f t="shared" si="11"/>
-        <v>-483.73688314003272</v>
-      </c>
-      <c r="AX5">
-        <f t="shared" si="12"/>
-        <v>20042.411239308476</v>
-      </c>
-      <c r="AY5">
-        <f t="shared" si="13"/>
-        <v>113188.03987583549</v>
+        <v>2.4434585127279789</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.0101377271699992</v>
       </c>
@@ -1456,36 +1394,36 @@
         <v>0.35070042781746302</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0667382212772831</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.7160377934598201</v>
       </c>
-      <c r="AE6">
-        <f t="shared" si="7"/>
-        <v>3.8888826306841788</v>
+      <c r="AE6" s="3">
+        <f t="shared" si="8"/>
+        <v>2.4123318207388968</v>
       </c>
       <c r="AF6">
         <f t="shared" si="1"/>
         <v>-1.652190958827537</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.393393085093245</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="8"/>
-        <v>1.075699065434494</v>
+        <f t="shared" si="9"/>
+        <v>1.1194774874981679</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="14"/>
-        <v>0.36570923758713736</v>
-      </c>
-      <c r="AJ6">
-        <f t="shared" si="15"/>
-        <v>8.3243962342418119</v>
+        <f t="shared" si="11"/>
+        <v>0.35140776789751105</v>
+      </c>
+      <c r="AJ6" s="2">
+        <f t="shared" si="10"/>
+        <v>0.29783972053186508</v>
       </c>
       <c r="AK6">
         <f t="shared" si="2"/>
@@ -1495,59 +1433,43 @@
         <f t="shared" si="3"/>
         <v>199552.3578074</v>
       </c>
-      <c r="AM6">
+      <c r="AM6" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.66533422691185917</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="5"/>
+        <v>-0.24541223655052344</v>
+      </c>
+      <c r="AO6" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="12"/>
+        <v>1.5974582636996595</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="13"/>
+        <v>4.4169213414927846</v>
+      </c>
+      <c r="AR6" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.33493566012632725</v>
+      </c>
+      <c r="AS6">
+        <f t="shared" si="15"/>
+        <v>-0.75170010111758812</v>
+      </c>
+      <c r="AT6" s="1">
         <f t="shared" si="16"/>
-        <v>-0.70823967657930531</v>
-      </c>
-      <c r="AN6">
-        <f t="shared" si="9"/>
-        <v>-0.23607350230472132</v>
-      </c>
-      <c r="AO6" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP6">
-        <f t="shared" si="17"/>
-        <v>1.5974582636996595</v>
-      </c>
-      <c r="AQ6">
-        <f t="shared" si="18"/>
-        <v>4.4169213414927846</v>
-      </c>
-      <c r="AR6">
-        <f t="shared" si="19"/>
-        <v>-0.33857482246520254</v>
-      </c>
-      <c r="AS6">
-        <f t="shared" si="20"/>
-        <v>-0.60397606737864074</v>
-      </c>
-      <c r="AT6">
-        <f t="shared" si="21"/>
-        <v>0.92580330947896949</v>
+        <v>1.1245500080654742</v>
       </c>
       <c r="AU6">
-        <f t="shared" ref="AU6:AU18" si="22">AU5+AT6</f>
-        <v>2.9382753082170918</v>
-      </c>
-      <c r="AV6">
-        <f t="shared" si="10"/>
-        <v>-122.59391504782049</v>
-      </c>
-      <c r="AW6">
-        <f t="shared" si="11"/>
-        <v>-541.48767971187181</v>
-      </c>
-      <c r="AX6">
-        <f t="shared" si="12"/>
-        <v>37675.23903665915</v>
-      </c>
-      <c r="AY6">
-        <f t="shared" si="13"/>
-        <v>195778.87100487424</v>
+        <f t="shared" ref="AU6:AU18" si="17">AU5+AT6</f>
+        <v>3.5680085207934531</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12.176646483900001</v>
       </c>
@@ -1634,36 +1556,36 @@
         <v>0.19999993483033052</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1986945199194547</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.99869458508912423</v>
       </c>
-      <c r="AE7">
-        <f t="shared" si="7"/>
-        <v>4.9384663104565565</v>
+      <c r="AE7" s="3">
+        <f t="shared" si="8"/>
+        <v>3.4929563013064548</v>
       </c>
       <c r="AF7">
         <f t="shared" si="1"/>
         <v>-2.3025665428696693</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.28265679162930413</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="8"/>
-        <v>1.0495836797723777</v>
+        <f t="shared" si="9"/>
+        <v>1.080624480567558</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="14"/>
-        <v>0.26930372211065978</v>
-      </c>
-      <c r="AJ7">
-        <f t="shared" si="15"/>
-        <v>7.6461633555965847</v>
+        <f t="shared" si="11"/>
+        <v>0.26156800693692328</v>
+      </c>
+      <c r="AJ7" s="2">
+        <f t="shared" si="10"/>
+        <v>0.33487633629698077</v>
       </c>
       <c r="AK7">
         <f t="shared" si="2"/>
@@ -1673,59 +1595,43 @@
         <f t="shared" si="3"/>
         <v>269986.16568114999</v>
       </c>
-      <c r="AM7">
+      <c r="AM7" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.68847699687883801</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="5"/>
+        <v>-0.25464876034754208</v>
+      </c>
+      <c r="AO7" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="12"/>
+        <v>1.5583485062903495</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="13"/>
+        <v>4.2428402698361198</v>
+      </c>
+      <c r="AR7" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.3755968117088691</v>
+      </c>
+      <c r="AS7">
+        <f t="shared" si="15"/>
+        <v>-1.1272969128264572</v>
+      </c>
+      <c r="AT7" s="1">
         <f t="shared" si="16"/>
-        <v>-0.64793134865889312</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="9"/>
-        <v>-0.26443070366573806</v>
-      </c>
-      <c r="AO7" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP7">
+        <v>1.1215985454874777</v>
+      </c>
+      <c r="AU7">
         <f t="shared" si="17"/>
-        <v>1.5583485062903495</v>
-      </c>
-      <c r="AQ7">
-        <f t="shared" si="18"/>
-        <v>4.2428402698361198</v>
-      </c>
-      <c r="AR7">
-        <f t="shared" si="19"/>
-        <v>-0.2479121797403801</v>
-      </c>
-      <c r="AS7">
-        <f t="shared" si="20"/>
-        <v>-0.85188824711902078</v>
-      </c>
-      <c r="AT7">
-        <f t="shared" si="21"/>
-        <v>0.92056722349537501</v>
-      </c>
-      <c r="AU7">
-        <f t="shared" si="22"/>
-        <v>3.858842531712467</v>
-      </c>
-      <c r="AV7">
-        <f t="shared" si="10"/>
-        <v>-127.06275255251531</v>
-      </c>
-      <c r="AW7">
-        <f t="shared" si="11"/>
-        <v>-539.10696332603413</v>
-      </c>
-      <c r="AX7">
-        <f t="shared" si="12"/>
-        <v>58772.927097917222</v>
-      </c>
-      <c r="AY7">
-        <f t="shared" si="13"/>
-        <v>288987.81887893449</v>
+        <v>4.6896070662809306</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15.449823501799999</v>
       </c>
@@ -1812,36 +1718,36 @@
         <v>-0.10677972586135009</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3124094508466104</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.4191891767079605</v>
       </c>
-      <c r="AE8">
-        <f t="shared" si="7"/>
-        <v>6.0396844916037837</v>
+      <c r="AE8" s="3">
+        <f t="shared" si="8"/>
+        <v>4.6186665639133393</v>
       </c>
       <c r="AF8">
         <f t="shared" si="1"/>
         <v>-3.1088253506863501</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.42049459161883629</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="8"/>
-        <v>1.1012181811472272</v>
+        <f t="shared" si="9"/>
+        <v>1.1257102626068844</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="14"/>
-        <v>0.38184494119119372</v>
-      </c>
-      <c r="AJ8">
-        <f t="shared" si="15"/>
-        <v>7.1409729446232255</v>
+        <f t="shared" si="11"/>
+        <v>0.37353713969442559</v>
+      </c>
+      <c r="AJ8" s="2">
+        <f t="shared" si="10"/>
+        <v>0.36322412530515052</v>
       </c>
       <c r="AK8">
         <f t="shared" si="2"/>
@@ -1851,59 +1757,43 @@
         <f t="shared" si="3"/>
         <v>343143.63679850003</v>
       </c>
-      <c r="AM8">
+      <c r="AM8" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.70662969241584817</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="5"/>
+        <v>-0.2616440755961088</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="12"/>
+        <v>1.5290331594502045</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" si="13"/>
+        <v>4.1184248019051992</v>
+      </c>
+      <c r="AR8" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.41718936984660338</v>
+      </c>
+      <c r="AS8">
+        <f t="shared" si="15"/>
+        <v>-1.5444862826730605</v>
+      </c>
+      <c r="AT8" s="1">
         <f t="shared" si="16"/>
-        <v>-0.71876756682523801</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="9"/>
-        <v>-0.25880158644196866</v>
-      </c>
-      <c r="AO8" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP8">
+        <v>1.1485728529075971</v>
+      </c>
+      <c r="AU8">
         <f t="shared" si="17"/>
-        <v>1.5290331594502045</v>
-      </c>
-      <c r="AQ8">
-        <f t="shared" si="18"/>
-        <v>4.1184248019051992</v>
-      </c>
-      <c r="AR8">
-        <f t="shared" si="19"/>
-        <v>-0.36079025530608666</v>
-      </c>
-      <c r="AS8">
-        <f t="shared" si="20"/>
-        <v>-1.2126785024251074</v>
-      </c>
-      <c r="AT8">
-        <f t="shared" si="21"/>
-        <v>0.94486063945373899</v>
-      </c>
-      <c r="AU8">
-        <f t="shared" si="22"/>
-        <v>4.8037031711662062</v>
-      </c>
-      <c r="AV8">
-        <f t="shared" si="10"/>
-        <v>-138.77494418789016</v>
-      </c>
-      <c r="AW8">
-        <f t="shared" si="11"/>
-        <v>-571.53417202641685</v>
-      </c>
-      <c r="AX8">
-        <f t="shared" si="12"/>
-        <v>81050.015233725237</v>
-      </c>
-      <c r="AY8">
-        <f t="shared" si="13"/>
-        <v>383523.2112658472</v>
+        <v>5.8381799191885282</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>18.810443319000001</v>
       </c>
@@ -1990,36 +1880,36 @@
         <v>-0.34012835873640235</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.410704919282195</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.7508332780185973</v>
       </c>
-      <c r="AE9">
-        <f t="shared" si="7"/>
-        <v>7.1192576157988006</v>
+      <c r="AE9" s="3">
+        <f t="shared" si="8"/>
+        <v>5.7179507850072619</v>
       </c>
       <c r="AF9">
         <f t="shared" si="1"/>
         <v>-3.8430691068464022</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.33164410131063682</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="8"/>
-        <v>1.0795731241950168</v>
+        <f t="shared" si="9"/>
+        <v>1.0992842210939227</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="14"/>
-        <v>0.30719929375597144</v>
-      </c>
-      <c r="AJ9">
-        <f t="shared" si="15"/>
-        <v>6.7529279408785516</v>
+        <f t="shared" si="11"/>
+        <v>0.30169095029910487</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f t="shared" si="10"/>
+        <v>0.38623271525634967</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
@@ -2029,59 +1919,43 @@
         <f t="shared" si="3"/>
         <v>416368.13751550001</v>
       </c>
-      <c r="AM9">
+      <c r="AM9" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.72165289016590672</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="5"/>
+        <v>-0.2672667846072983</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="12"/>
+        <v>1.5056348650184768</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="13"/>
+        <v>4.0226244505572453</v>
+      </c>
+      <c r="AR9" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.44123485368654386</v>
+      </c>
+      <c r="AS9">
+        <f t="shared" si="15"/>
+        <v>-1.9857211363596043</v>
+      </c>
+      <c r="AT9" s="1">
         <f t="shared" si="16"/>
-        <v>-0.67112255636500051</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="9"/>
-        <v>-0.27998144525950386</v>
-      </c>
-      <c r="AO9" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP9">
+        <v>1.1424067311172441</v>
+      </c>
+      <c r="AU9">
         <f t="shared" si="17"/>
-        <v>1.5056348650184768</v>
-      </c>
-      <c r="AQ9">
-        <f t="shared" si="18"/>
-        <v>4.0226244505572453</v>
-      </c>
-      <c r="AR9">
-        <f t="shared" si="19"/>
-        <v>-0.28736237553493099</v>
-      </c>
-      <c r="AS9">
-        <f t="shared" si="20"/>
-        <v>-1.5000408779600385</v>
-      </c>
-      <c r="AT9">
-        <f t="shared" si="21"/>
-        <v>0.93542655004669995</v>
-      </c>
-      <c r="AU9">
-        <f t="shared" si="22"/>
-        <v>5.7391297212129064</v>
-      </c>
-      <c r="AV9">
-        <f t="shared" si="10"/>
-        <v>-141.34299245398256</v>
-      </c>
-      <c r="AW9">
-        <f t="shared" si="11"/>
-        <v>-568.56977736031843</v>
-      </c>
-      <c r="AX9">
-        <f t="shared" si="12"/>
-        <v>104861.61675700132</v>
-      </c>
-      <c r="AY9">
-        <f t="shared" si="13"/>
-        <v>481603.04226072901</v>
+        <v>6.9805866503057725</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22.1821845652</v>
       </c>
@@ -2168,36 +2042,36 @@
         <v>-0.69687079219256098</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4964599833587491</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.1933307755513098</v>
       </c>
-      <c r="AE10">
-        <f t="shared" si="7"/>
-        <v>8.2334755863341869</v>
+      <c r="AE10" s="3">
+        <f t="shared" si="8"/>
+        <v>6.8483812175265442</v>
       </c>
       <c r="AF10">
         <f t="shared" si="1"/>
         <v>-4.6974634533275612</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.4424974975327125</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="8"/>
-        <v>1.1142179705353863</v>
+        <f t="shared" si="9"/>
+        <v>1.1304304325192822</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="14"/>
-        <v>0.39713728303995188</v>
-      </c>
-      <c r="AJ10">
-        <f t="shared" si="15"/>
-        <v>6.445796850129458</v>
+        <f t="shared" si="11"/>
+        <v>0.39144160029959618</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f t="shared" si="10"/>
+        <v>0.40523305542392607</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
@@ -2207,59 +2081,43 @@
         <f t="shared" si="3"/>
         <v>488807.77019649994</v>
       </c>
-      <c r="AM10">
+      <c r="AM10" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.73425979909544348</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="5"/>
+        <v>-0.27186852623002888</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" si="12"/>
+        <v>1.4865801781327825</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" si="13"/>
+        <v>3.946796698417784</v>
+      </c>
+      <c r="AR10" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.45358375397901685</v>
+      </c>
+      <c r="AS10">
+        <f t="shared" si="15"/>
+        <v>-2.4393048903386214</v>
+      </c>
+      <c r="AT10" s="1">
         <f t="shared" si="16"/>
-        <v>-0.72886567189208817</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="9"/>
-        <v>-0.27318529731363339</v>
-      </c>
-      <c r="AO10" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP10">
+        <v>1.1193157811484797</v>
+      </c>
+      <c r="AU10">
         <f t="shared" si="17"/>
-        <v>1.4865801781327825</v>
-      </c>
-      <c r="AQ10">
-        <f t="shared" si="18"/>
-        <v>3.946796698417784</v>
-      </c>
-      <c r="AR10">
-        <f t="shared" si="19"/>
-        <v>-0.36511377899795716</v>
-      </c>
-      <c r="AS10">
-        <f t="shared" si="20"/>
-        <v>-1.8651546569579955</v>
-      </c>
-      <c r="AT10">
-        <f t="shared" si="21"/>
-        <v>0.91936414582668879</v>
-      </c>
-      <c r="AU10">
-        <f t="shared" si="22"/>
-        <v>6.6584938670395957</v>
-      </c>
-      <c r="AV10">
-        <f t="shared" si="10"/>
-        <v>-149.42152276187466</v>
-      </c>
-      <c r="AW10">
-        <f t="shared" si="11"/>
-        <v>-589.73637270912468</v>
-      </c>
-      <c r="AX10">
-        <f t="shared" si="12"/>
-        <v>129347.66184672937</v>
-      </c>
-      <c r="AY10">
-        <f t="shared" si="13"/>
-        <v>580112.53623430838</v>
+        <v>8.099902431454252</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25.4604440606</v>
       </c>
@@ -2346,36 +2204,36 @@
         <v>-1.0567213372539408</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5694932356234361</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.6262145728773767</v>
       </c>
-      <c r="AE11">
-        <f t="shared" si="7"/>
-        <v>9.3529214808213137</v>
+      <c r="AE11" s="3">
+        <f t="shared" si="8"/>
+        <v>7.9809777303481413</v>
       </c>
       <c r="AF11">
         <f t="shared" si="1"/>
         <v>-5.557061854788941</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.43288379732606685</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="8"/>
-        <v>1.1194458944871268</v>
+        <f t="shared" si="9"/>
+        <v>1.1325965128215971</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="14"/>
-        <v>0.38669470267197881</v>
-      </c>
-      <c r="AJ11">
-        <f t="shared" si="15"/>
-        <v>6.2044656179427848</v>
+        <f t="shared" si="11"/>
+        <v>0.38220477674581477</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.42095593773000084</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
@@ -2385,59 +2243,43 @@
         <f t="shared" si="3"/>
         <v>555202.86013150006</v>
       </c>
-      <c r="AM11">
+      <c r="AM11" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.74483253924682147</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="5"/>
+        <v>-0.27564569709270981</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="12"/>
+        <v>1.470995298159429</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="13"/>
+        <v>3.8861820301573067</v>
+      </c>
+      <c r="AR11" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.4417966868956909</v>
+      </c>
+      <c r="AS11">
+        <f t="shared" si="15"/>
+        <v>-2.8811015772343125</v>
+      </c>
+      <c r="AT11" s="1">
         <f t="shared" si="16"/>
-        <v>-0.72195724877649503</v>
-      </c>
-      <c r="AN11">
-        <f t="shared" si="9"/>
-        <v>-0.28136948722783045</v>
-      </c>
-      <c r="AO11" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP11">
+        <v>1.0495081487104649</v>
+      </c>
+      <c r="AU11">
         <f t="shared" si="17"/>
-        <v>1.470995298159429</v>
-      </c>
-      <c r="AQ11">
-        <f t="shared" si="18"/>
-        <v>3.8861820301573067</v>
-      </c>
-      <c r="AR11">
-        <f t="shared" si="19"/>
-        <v>-0.33268100544312651</v>
-      </c>
-      <c r="AS11">
-        <f t="shared" si="20"/>
-        <v>-2.1978356624011219</v>
-      </c>
-      <c r="AT11">
-        <f t="shared" si="21"/>
-        <v>0.86031953151768337</v>
-      </c>
-      <c r="AU11">
-        <f t="shared" si="22"/>
-        <v>7.5188133985572794</v>
-      </c>
-      <c r="AV11">
-        <f t="shared" si="10"/>
-        <v>-153.76895230592123</v>
-      </c>
-      <c r="AW11">
-        <f t="shared" si="11"/>
-        <v>-597.57413924738705</v>
-      </c>
-      <c r="AX11">
-        <f t="shared" si="12"/>
-        <v>154001.46825688434</v>
-      </c>
-      <c r="AY11">
-        <f t="shared" si="13"/>
-        <v>677425.41863137204</v>
+        <v>9.1494105801647176</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28.5971191999</v>
       </c>
@@ -2524,36 +2366,36 @@
         <v>-1.3573824484509611</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6299703523638815</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.9873528008148424</v>
       </c>
-      <c r="AE12">
-        <f t="shared" si="7"/>
-        <v>10.457959603650322</v>
+      <c r="AE12" s="3">
+        <f t="shared" si="8"/>
+        <v>9.0964829921638568</v>
       </c>
       <c r="AF12">
         <f t="shared" si="1"/>
         <v>-6.3601318422009614</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.36113822793746575</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="8"/>
-        <v>1.1050381228290078</v>
+        <f t="shared" si="9"/>
+        <v>1.1155052618157155</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="14"/>
-        <v>0.32681065067050885</v>
-      </c>
-      <c r="AJ12">
-        <f t="shared" si="15"/>
-        <v>6.0172755513511387</v>
+        <f t="shared" si="11"/>
+        <v>0.32374408288279932</v>
+      </c>
+      <c r="AJ12" s="2">
+        <f t="shared" si="10"/>
+        <v>0.4337328660539343</v>
       </c>
       <c r="AK12">
         <f t="shared" si="2"/>
@@ -2563,59 +2405,43 @@
         <f t="shared" si="3"/>
         <v>611699.82950849994</v>
       </c>
-      <c r="AM12">
+      <c r="AM12" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75351970980530625</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="5"/>
+        <v>-0.27869324964626974</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="12"/>
+        <v>1.4584525263146098</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="13"/>
+        <v>3.8382892214688829</v>
+      </c>
+      <c r="AR12" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.40762519401662445</v>
+      </c>
+      <c r="AS12">
+        <f t="shared" si="15"/>
+        <v>-3.2887267712509369</v>
+      </c>
+      <c r="AT12" s="1">
         <f t="shared" si="16"/>
-        <v>-0.68338243646254337</v>
-      </c>
-      <c r="AN12">
-        <f t="shared" si="9"/>
-        <v>-0.29715404415682817</v>
-      </c>
-      <c r="AO12" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP12">
+        <v>0.93980702390659199</v>
+      </c>
+      <c r="AU12">
         <f t="shared" si="17"/>
-        <v>1.4584525263146098</v>
-      </c>
-      <c r="AQ12">
-        <f t="shared" si="18"/>
-        <v>3.8382892214688829</v>
-      </c>
-      <c r="AR12">
-        <f t="shared" si="19"/>
-        <v>-0.25059165963659968</v>
-      </c>
-      <c r="AS12">
-        <f t="shared" si="20"/>
-        <v>-2.4484273220377215</v>
-      </c>
-      <c r="AT12">
-        <f t="shared" si="21"/>
-        <v>0.76677935410754638</v>
-      </c>
-      <c r="AU12">
-        <f t="shared" si="22"/>
-        <v>8.2855927526648259</v>
-      </c>
-      <c r="AV12">
-        <f t="shared" si="10"/>
-        <v>-155.2170265322894</v>
-      </c>
-      <c r="AW12">
-        <f t="shared" si="11"/>
-        <v>-595.76783992733613</v>
-      </c>
-      <c r="AX12">
-        <f t="shared" si="12"/>
-        <v>177635.0048945192</v>
-      </c>
-      <c r="AY12">
-        <f t="shared" si="13"/>
-        <v>769277.07780096971</v>
+        <v>10.08921760407131</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>30.854626388900002</v>
       </c>
@@ -2702,36 +2528,36 @@
         <v>-2.0595318912459915</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6559313815255983</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.7154632727715899</v>
       </c>
-      <c r="AE13">
-        <f t="shared" si="7"/>
-        <v>11.68986396061533</v>
+      <c r="AE13" s="3">
+        <f t="shared" si="8"/>
+        <v>10.332769511837222</v>
       </c>
       <c r="AF13">
         <f t="shared" si="1"/>
         <v>-7.5612085563459912</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.7281104719567475</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="8"/>
-        <v>1.2319043569650088</v>
+        <f t="shared" si="9"/>
+        <v>1.2362865196733654</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="14"/>
-        <v>0.59104464388011646</v>
-      </c>
-      <c r="AJ13">
-        <f t="shared" si="15"/>
-        <v>5.9401779513004955</v>
+        <f t="shared" si="11"/>
+        <v>0.58894961675155921</v>
+      </c>
+      <c r="AJ13" s="2">
+        <f t="shared" si="10"/>
+        <v>0.44177279741358977</v>
       </c>
       <c r="AK13">
         <f t="shared" si="2"/>
@@ -2741,59 +2567,43 @@
         <f t="shared" si="3"/>
         <v>626967.5865185</v>
       </c>
-      <c r="AM13">
+      <c r="AM13" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75903062693197265</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="5"/>
+        <v>-0.28060038175465879</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="12"/>
+        <v>1.4506159942722798</v>
+      </c>
+      <c r="AQ13">
+        <f t="shared" si="13"/>
+        <v>3.8087601051314892</v>
+      </c>
+      <c r="AR13" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.1872485184731727</v>
+      </c>
+      <c r="AS13">
+        <f t="shared" si="15"/>
+        <v>-3.4759752897241096</v>
+      </c>
+      <c r="AT13" s="1">
         <f t="shared" si="16"/>
-        <v>-0.86802963723170545</v>
-      </c>
-      <c r="AN13">
-        <f t="shared" si="9"/>
-        <v>-0.25595093859194906</v>
-      </c>
-      <c r="AO13" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP13">
+        <v>0.42385705858178896</v>
+      </c>
+      <c r="AU13">
         <f t="shared" si="17"/>
-        <v>1.4506159942722798</v>
-      </c>
-      <c r="AQ13">
-        <f t="shared" si="18"/>
-        <v>3.8087601051314892</v>
-      </c>
-      <c r="AR13">
-        <f t="shared" si="19"/>
-        <v>-0.2095995379177385</v>
-      </c>
-      <c r="AS13">
-        <f t="shared" si="20"/>
-        <v>-2.6580268599554602</v>
-      </c>
-      <c r="AT13">
-        <f t="shared" si="21"/>
-        <v>0.35462556016369595</v>
-      </c>
-      <c r="AU13">
-        <f t="shared" si="22"/>
-        <v>8.6402183128285213</v>
-      </c>
-      <c r="AV13">
-        <f t="shared" si="10"/>
-        <v>-170.60193042188445</v>
-      </c>
-      <c r="AW13">
-        <f t="shared" si="11"/>
-        <v>-649.78182644929188</v>
-      </c>
-      <c r="AX13">
-        <f t="shared" si="12"/>
-        <v>199160.45354055756</v>
-      </c>
-      <c r="AY13">
-        <f t="shared" si="13"/>
-        <v>851903.01305059181</v>
+        <v>10.513074662653098</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32.080066029599998</v>
       </c>
@@ -2880,36 +2690,36 @@
         <v>-3.1772879905688667</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6592719331412191</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-4.8365599237100856</v>
       </c>
-      <c r="AE14">
-        <f t="shared" si="7"/>
-        <v>13.062964914256289</v>
+      <c r="AE14" s="3">
+        <f t="shared" si="8"/>
+        <v>11.706429645419904</v>
       </c>
       <c r="AF14">
         <f t="shared" si="1"/>
         <v>-9.1792224492688668</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.1210966509384956</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="8"/>
-        <v>1.3731009536409591</v>
+        <f t="shared" si="9"/>
+        <v>1.3736601335826819</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="14"/>
-        <v>0.81647066660740375</v>
-      </c>
-      <c r="AJ14">
-        <f t="shared" si="15"/>
-        <v>5.9303935889761288</v>
+        <f t="shared" si="11"/>
+        <v>0.8161383034495816</v>
+      </c>
+      <c r="AJ14" s="2">
+        <f t="shared" si="10"/>
+        <v>0.44446908167319388</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
@@ -2919,59 +2729,43 @@
         <f t="shared" si="3"/>
         <v>613789.68986549997</v>
       </c>
-      <c r="AM14">
+      <c r="AM14" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.76088654131655131</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="5"/>
+        <v>-0.28123808099769321</v>
+      </c>
+      <c r="AO14" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" si="12"/>
+        <v>1.4479976141598188</v>
+      </c>
+      <c r="AQ14">
+        <f t="shared" si="13"/>
+        <v>3.7989601576081489</v>
+      </c>
+      <c r="AR14" s="1">
+        <f t="shared" si="14"/>
+        <v>-2.4645842079890293E-2</v>
+      </c>
+      <c r="AS14">
+        <f t="shared" si="15"/>
+        <v>-3.5006211318039999</v>
+      </c>
+      <c r="AT14" s="1">
         <f t="shared" si="16"/>
-        <v>-1.0608836946597158</v>
-      </c>
-      <c r="AN14">
-        <f t="shared" si="9"/>
-        <v>-0.22235141563771343</v>
-      </c>
-      <c r="AO14" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP14">
+        <v>5.5450070873572531E-2</v>
+      </c>
+      <c r="AU14">
         <f t="shared" si="17"/>
-        <v>1.4479976141598188</v>
-      </c>
-      <c r="AQ14">
-        <f t="shared" si="18"/>
-        <v>3.7989601576081489</v>
-      </c>
-      <c r="AR14">
-        <f t="shared" si="19"/>
-        <v>-3.9503459656514736E-2</v>
-      </c>
-      <c r="AS14">
-        <f t="shared" si="20"/>
-        <v>-2.6975303196119751</v>
-      </c>
-      <c r="AT14">
-        <f t="shared" si="21"/>
-        <v>4.8383195223239785E-2</v>
-      </c>
-      <c r="AU14">
-        <f t="shared" si="22"/>
-        <v>8.6886015080517609</v>
-      </c>
-      <c r="AV14">
-        <f t="shared" si="10"/>
-        <v>-183.00210737962752</v>
-      </c>
-      <c r="AW14">
-        <f t="shared" si="11"/>
-        <v>-695.21771469353337</v>
-      </c>
-      <c r="AX14">
-        <f t="shared" si="12"/>
-        <v>208970.21281921203</v>
-      </c>
-      <c r="AY14">
-        <f t="shared" si="13"/>
-        <v>889267.82624312339</v>
+        <v>10.568524733526671</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32.297219829100001</v>
       </c>
@@ -3058,36 +2852,36 @@
         <v>-5.3026998397139868</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6291803705873067</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.9318802103012933</v>
       </c>
-      <c r="AE15">
-        <f t="shared" si="7"/>
-        <v>14.772471457237996</v>
+      <c r="AE15" s="3">
+        <f t="shared" si="8"/>
+        <v>13.410860474009127</v>
       </c>
       <c r="AF15">
         <f t="shared" si="1"/>
         <v>-11.805152261713987</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.0953202865912077</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="8"/>
-        <v>1.7095065429817069</v>
+        <f t="shared" si="9"/>
+        <v>1.7044308285892225</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="14"/>
-        <v>1.225687199147286</v>
-      </c>
-      <c r="AJ15">
-        <f t="shared" si="15"/>
-        <v>6.0196514173841384</v>
+        <f t="shared" si="11"/>
+        <v>1.2293372376545952</v>
+      </c>
+      <c r="AJ15" s="2">
+        <f t="shared" si="10"/>
+        <v>0.44201257516055953</v>
       </c>
       <c r="AK15">
         <f t="shared" si="2"/>
@@ -3097,59 +2891,43 @@
         <f t="shared" si="3"/>
         <v>557979.83421200002</v>
       </c>
-      <c r="AM15">
+      <c r="AM15" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75919551296561028</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="5"/>
+        <v>-0.28065713032120482</v>
+      </c>
+      <c r="AO15" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="12"/>
+        <v>1.4503829472856433</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="13"/>
+        <v>3.807886525406599</v>
+      </c>
+      <c r="AR15" s="1">
+        <f t="shared" si="14"/>
+        <v>0.21747446747966642</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="15"/>
+        <v>-3.2831466643243337</v>
+      </c>
+      <c r="AT15" s="1">
         <f t="shared" si="16"/>
-        <v>-1.536193166073847</v>
-      </c>
-      <c r="AN15">
-        <f t="shared" si="9"/>
-        <v>-0.16641795850376784</v>
-      </c>
-      <c r="AO15" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP15">
+        <v>-0.4920096841151399</v>
+      </c>
+      <c r="AU15">
         <f t="shared" si="17"/>
-        <v>1.4503829472856433</v>
-      </c>
-      <c r="AQ15">
-        <f t="shared" si="18"/>
-        <v>3.807886525406599</v>
-      </c>
-      <c r="AR15">
-        <f t="shared" si="19"/>
-        <v>0.59551018146471824</v>
-      </c>
-      <c r="AS15">
-        <f t="shared" si="20"/>
-        <v>-2.1020201381472567</v>
-      </c>
-      <c r="AT15">
-        <f t="shared" si="21"/>
-        <v>-0.48585820418049264</v>
-      </c>
-      <c r="AU15">
-        <f t="shared" si="22"/>
-        <v>8.2027433038712676</v>
-      </c>
-      <c r="AV15">
-        <f t="shared" si="10"/>
-        <v>-200.64756343702322</v>
-      </c>
-      <c r="AW15">
-        <f t="shared" si="11"/>
-        <v>-764.04315316750672</v>
-      </c>
-      <c r="AX15">
-        <f t="shared" si="12"/>
-        <v>210242.23607456798</v>
-      </c>
-      <c r="AY15">
-        <f t="shared" si="13"/>
-        <v>894098.40085582249</v>
+        <v>10.076515049411531</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31.505757123799999</v>
       </c>
@@ -3236,36 +3014,36 @@
         <v>-6.403433079926435</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5792516072617018</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-7.9826846871881365</v>
       </c>
-      <c r="AE16">
-        <f t="shared" si="7"/>
-        <v>16.13500808720881</v>
+      <c r="AE16" s="3">
+        <f t="shared" si="8"/>
+        <v>14.764778428725549</v>
       </c>
       <c r="AF16">
         <f t="shared" si="1"/>
         <v>-13.403698276876435</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-1.0508044768868432</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="8"/>
-        <v>1.3625366299708137</v>
+        <f t="shared" si="9"/>
+        <v>1.3539179547164224</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="14"/>
-        <v>0.77121191003088996</v>
-      </c>
-      <c r="AJ16">
-        <f t="shared" si="15"/>
-        <v>6.1735165051136001</v>
+        <f t="shared" si="11"/>
+        <v>0.77612123631740582</v>
+      </c>
+      <c r="AJ16" s="2">
+        <f t="shared" si="10"/>
+        <v>0.43456075696068175</v>
       </c>
       <c r="AK16">
         <f t="shared" si="2"/>
@@ -3275,59 +3053,43 @@
         <f t="shared" si="3"/>
         <v>481797.63894000003</v>
       </c>
-      <c r="AM16">
+      <c r="AM16" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75408558678972093</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="5"/>
+        <v>-0.27889001452943801</v>
+      </c>
+      <c r="AO16" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="12"/>
+        <v>1.4576435805439203</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" si="13"/>
+        <v>3.8352271151267998</v>
+      </c>
+      <c r="AR16" s="1">
+        <f t="shared" si="14"/>
+        <v>0.33890711980735105</v>
+      </c>
+      <c r="AS16">
+        <f t="shared" si="15"/>
+        <v>-2.9442395445169827</v>
+      </c>
+      <c r="AT16" s="1">
         <f t="shared" si="16"/>
-        <v>-1.0190344789855583</v>
-      </c>
-      <c r="AN16">
-        <f t="shared" si="9"/>
-        <v>-0.22589090104026496</v>
-      </c>
-      <c r="AO16" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP16">
+        <v>-0.7798843185419404</v>
+      </c>
+      <c r="AU16">
         <f t="shared" si="17"/>
-        <v>1.4576435805439203</v>
-      </c>
-      <c r="AQ16">
-        <f t="shared" si="18"/>
-        <v>3.8352271151267998</v>
-      </c>
-      <c r="AR16">
-        <f t="shared" si="19"/>
-        <v>0.51981264022386986</v>
-      </c>
-      <c r="AS16">
-        <f t="shared" si="20"/>
-        <v>-1.5822074979233869</v>
-      </c>
-      <c r="AT16">
-        <f t="shared" si="21"/>
-        <v>-0.67402050391448121</v>
-      </c>
-      <c r="AU16">
-        <f t="shared" si="22"/>
-        <v>7.5287227999567863</v>
-      </c>
-      <c r="AV16">
-        <f t="shared" si="10"/>
-        <v>-180.88039570788899</v>
-      </c>
-      <c r="AW16">
-        <f t="shared" si="11"/>
-        <v>-693.71739821376127</v>
-      </c>
-      <c r="AX16">
-        <f t="shared" si="12"/>
-        <v>198856.80970911897</v>
-      </c>
-      <c r="AY16">
-        <f t="shared" si="13"/>
-        <v>850739.04383613251</v>
+        <v>9.296630730869591</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32.253108226000002</v>
       </c>
@@ -3414,36 +3176,36 @@
         <v>-6.8663253380735645</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5888945238585055</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-8.4552198619320702</v>
       </c>
-      <c r="AE17">
-        <f t="shared" si="7"/>
-        <v>17.289686448891189</v>
+      <c r="AE17" s="3">
+        <f t="shared" si="8"/>
+        <v>15.921140958958379</v>
       </c>
       <c r="AF17">
         <f t="shared" si="1"/>
         <v>-14.366781006173564</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.47253517474393369</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="8"/>
-        <v>1.1546783616823788</v>
+        <f t="shared" si="9"/>
+        <v>1.1563625302328298</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="14"/>
-        <v>0.40923532511291272</v>
-      </c>
-      <c r="AJ17">
-        <f t="shared" si="15"/>
-        <v>6.1432205940986835</v>
+        <f t="shared" si="11"/>
+        <v>0.40863929986454189</v>
+      </c>
+      <c r="AJ17" s="2">
+        <f t="shared" si="10"/>
+        <v>0.43070722447720716</v>
       </c>
       <c r="AK17">
         <f t="shared" si="2"/>
@@ -3453,59 +3215,43 @@
         <f t="shared" si="3"/>
         <v>488492.35904600006</v>
       </c>
-      <c r="AM17">
+      <c r="AM17" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.75145473605449731</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="5"/>
+        <v>-0.27797340777508867</v>
+      </c>
+      <c r="AO17" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="12"/>
+        <v>1.461412835230103</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="13"/>
+        <v>3.8495223449663918</v>
+      </c>
+      <c r="AR17" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.3372117316071758E-2</v>
+      </c>
+      <c r="AS17">
+        <f t="shared" si="15"/>
+        <v>-3.0076116618330544</v>
+      </c>
+      <c r="AT17" s="1">
         <f t="shared" si="16"/>
-        <v>-0.73693892140015482</v>
-      </c>
-      <c r="AN17">
-        <f t="shared" si="9"/>
-        <v>-0.28159749888832464</v>
-      </c>
-      <c r="AO17" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP17">
+        <v>0.1471350228522238</v>
+      </c>
+      <c r="AU17">
         <f t="shared" si="17"/>
-        <v>1.461412835230103</v>
-      </c>
-      <c r="AQ17">
-        <f t="shared" si="18"/>
-        <v>3.8495223449663918</v>
-      </c>
-      <c r="AR17">
-        <f t="shared" si="19"/>
-        <v>-4.9397454599781412E-2</v>
-      </c>
-      <c r="AS17">
-        <f t="shared" si="20"/>
-        <v>-1.6316049525231684</v>
-      </c>
-      <c r="AT17">
-        <f t="shared" si="21"/>
-        <v>0.12070672194818977</v>
-      </c>
-      <c r="AU17">
-        <f t="shared" si="22"/>
-        <v>7.6494295219049757</v>
-      </c>
-      <c r="AV17">
-        <f t="shared" si="10"/>
-        <v>-160.63352874455379</v>
-      </c>
-      <c r="AW17">
-        <f t="shared" si="11"/>
-        <v>-618.36235825296103</v>
-      </c>
-      <c r="AX17">
-        <f t="shared" si="12"/>
-        <v>180981.45028094825</v>
-      </c>
-      <c r="AY17">
-        <f t="shared" si="13"/>
-        <v>782180.68437136151</v>
+        <v>9.4437657537218147</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31.807406181800001</v>
       </c>
@@ -3592,36 +3338,36 @@
         <v>-7.8129003470491121</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5562103213068299</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-9.3691106683559422</v>
       </c>
-      <c r="AE18">
-        <f t="shared" si="7"/>
-        <v>18.607424828283037</v>
+      <c r="AE18" s="3">
+        <f t="shared" si="8"/>
+        <v>17.233131929956755</v>
       </c>
       <c r="AF18">
         <f t="shared" si="1"/>
         <v>-15.814462703349111</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.91389080642387199</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="8"/>
-        <v>1.317738379391848</v>
+        <f t="shared" si="9"/>
+        <v>1.3119909709983766</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="14"/>
-        <v>0.69352977853285525</v>
-      </c>
-      <c r="AJ18">
-        <f t="shared" si="15"/>
-        <v>6.2470699448972535</v>
+        <f t="shared" si="11"/>
+        <v>0.69656790833585913</v>
+      </c>
+      <c r="AJ18" s="2">
+        <f t="shared" si="10"/>
+        <v>0.42852479015426859</v>
       </c>
       <c r="AK18">
         <f t="shared" si="2"/>
@@ -3631,59 +3377,43 @@
         <f t="shared" si="3"/>
         <v>442908.0974035</v>
       </c>
-      <c r="AM18">
+      <c r="AM18" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.74996826054176313</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="5"/>
+        <v>-0.27745346311550806</v>
+      </c>
+      <c r="AO18" s="3">
+        <v>42530.539337002985</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="12"/>
+        <v>1.4635519513705091</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="13"/>
+        <v>3.8576663285348212</v>
+      </c>
+      <c r="AR18" s="1">
+        <f t="shared" si="14"/>
+        <v>0.21086175420273567</v>
+      </c>
+      <c r="AS18">
+        <f t="shared" si="15"/>
+        <v>-2.7967499076303186</v>
+      </c>
+      <c r="AT18" s="1">
         <f t="shared" si="16"/>
-        <v>-0.95103321001801278</v>
-      </c>
-      <c r="AN18">
-        <f t="shared" si="9"/>
-        <v>-0.23545219472018389</v>
-      </c>
-      <c r="AO18" s="1">
-        <v>77626.17248935283</v>
-      </c>
-      <c r="AP18">
+        <v>-0.49206430770743886</v>
+      </c>
+      <c r="AU18">
         <f t="shared" si="17"/>
-        <v>1.4635519513705091</v>
-      </c>
-      <c r="AQ18">
-        <f t="shared" si="18"/>
-        <v>3.8576663285348212</v>
-      </c>
-      <c r="AR18">
-        <f t="shared" si="19"/>
-        <v>0.29056282688067597</v>
-      </c>
-      <c r="AS18">
-        <f t="shared" si="20"/>
-        <v>-1.3410421256424925</v>
-      </c>
-      <c r="AT18">
-        <f t="shared" si="21"/>
-        <v>-0.41896229386913175</v>
-      </c>
-      <c r="AU18">
-        <f t="shared" si="22"/>
-        <v>7.2304672280358435</v>
-      </c>
-      <c r="AV18">
-        <f t="shared" si="10"/>
-        <v>-176.10123060451687</v>
-      </c>
-      <c r="AW18">
-        <f t="shared" si="11"/>
-        <v>-679.33978771659054</v>
-      </c>
-      <c r="AX18">
-        <f t="shared" si="12"/>
-        <v>184324.4150799753</v>
-      </c>
-      <c r="AY18">
-        <f t="shared" si="13"/>
-        <v>795048.06789812376</v>
+        <v>8.9517014460143756</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31.567336453999999</v>
       </c>
@@ -3770,7 +3500,7 @@
         <v>-8.4108845215175485</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31.4068883148</v>
       </c>
@@ -3857,7 +3587,7 @@
         <v>-8.9525746769235415</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31.270712094699999</v>
       </c>
@@ -3944,7 +3674,7 @@
         <v>-9.3346573756835518</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>31.137649633700001</v>
       </c>

</xml_diff>

<commit_message>
equlibrium condition cannot be satisfied, which direction is positive?
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t># avgT</t>
   </si>
@@ -178,6 +178,10 @@
   </si>
   <si>
     <t>eq_pla</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_n_real_pred</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -510,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU22"/>
+  <dimension ref="A1:AV22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3:AO18"/>
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -542,10 +546,11 @@
     <col min="42" max="42" width="12.77734375" customWidth="1"/>
     <col min="44" max="44" width="12.44140625" customWidth="1"/>
     <col min="45" max="45" width="11.21875" customWidth="1"/>
-    <col min="48" max="1027" width="11.5546875"/>
+    <col min="48" max="48" width="13.33203125" style="2" customWidth="1"/>
+    <col min="49" max="1027" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,8 +692,11 @@
       <c r="AU1" t="s">
         <v>44</v>
       </c>
+      <c r="AV1" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.17366852143</v>
       </c>
@@ -820,8 +828,12 @@
       <c r="AU2">
         <v>0</v>
       </c>
+      <c r="AV2" s="2">
+        <f>(AQ2*X2-2*X2*(1-0.01*P2-2*0.01*AF2)/(-0.08/0.4*0.01*P2-(2*0.08/0.4+3)*0.01*AF2+1+0.08/0.4)+4*0.5*232000*(-0.4*0.01*AF2-0.08*0.01*P2)/((1-2*0.01*AF2)*0.4*0.08))/1000</f>
+        <v>-2.389488768044183</v>
+      </c>
     </row>
-    <row r="3" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.3863060409200001</v>
       </c>
@@ -982,8 +994,12 @@
         <f>AU2+AT3</f>
         <v>0.57237542883510506</v>
       </c>
+      <c r="AV3" s="2">
+        <f t="shared" ref="AV3:AV18" si="11">(AQ3*X3-2*X3*(1-0.01*P3-2*0.01*AF3)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+1+0.08/0.4)+4*0.5*232000*(-0.4*0.01*AF3-0.08*0.01*P3)/((1-2*0.01*AF3)*0.4*0.08))/1000</f>
+        <v>43.490396860164267</v>
+      </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.4615371024499999</v>
       </c>
@@ -1094,7 +1110,7 @@
         <v>1.0747104268205803</v>
       </c>
       <c r="AI4">
-        <f t="shared" ref="AI4:AI18" si="11">-AG4/AH4</f>
+        <f t="shared" ref="AI4:AI18" si="12">-AG4/AH4</f>
         <v>0.15649101116211753</v>
       </c>
       <c r="AJ4" s="2">
@@ -1121,31 +1137,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP4">
-        <f t="shared" ref="AP4:AP18" si="12">(AK4*1.35*(AK4/3255000)^-0.0723-AK3*1.35*(AK3/3255000)^-0.0723)/(AK4-AK3)</f>
+        <f t="shared" ref="AP4:AP18" si="13">(AK4*1.35*(AK4/3255000)^-0.0723-AK3*1.35*(AK3/3255000)^-0.0723)/(AK4-AK3)</f>
         <v>1.7404396115775711</v>
       </c>
       <c r="AQ4">
-        <f t="shared" ref="AQ4:AQ18" si="13">(2*AP4+3)/(3-AP4)</f>
+        <f t="shared" ref="AQ4:AQ18" si="14">(2*AP4+3)/(3-AP4)</f>
         <v>5.1453501417842284</v>
       </c>
       <c r="AR4" s="1">
-        <f t="shared" ref="AR4:AR18" si="14">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
+        <f t="shared" ref="AR4:AR18" si="15">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
         <v>-0.1537741601894102</v>
       </c>
       <c r="AS4">
-        <f t="shared" ref="AS4:AS18" si="15">AS3+AR4</f>
+        <f t="shared" ref="AS4:AS18" si="16">AS3+AR4</f>
         <v>-0.17172868090907556</v>
       </c>
       <c r="AT4" s="1">
-        <f t="shared" ref="AT4:AT18" si="16">2*(1-AM4)*(AK4-AK3)*(1-AP4/3)/(9*AN4*AO4*AM4)</f>
+        <f t="shared" ref="AT4:AT18" si="17">2*(1-AM4)*(AK4-AK3)*(1-AP4/3)/(9*AN4*AO4*AM4)</f>
         <v>0.90923795167839838</v>
       </c>
       <c r="AU4">
         <f>AU3+AT4</f>
         <v>1.4816133805135034</v>
       </c>
+      <c r="AV4" s="2">
+        <f t="shared" si="11"/>
+        <v>100.38870592819272</v>
+      </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.0730406484000001</v>
       </c>
@@ -1256,7 +1276,7 @@
         <v>1.0499189116276664</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.15661454046042708</v>
       </c>
       <c r="AJ5" s="2">
@@ -1283,31 +1303,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.6531141584289157</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.6820807838486802</v>
       </c>
       <c r="AR5" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.26272807087725686</v>
       </c>
       <c r="AS5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.43445675178633242</v>
       </c>
       <c r="AT5" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.065573817222305</v>
       </c>
       <c r="AU5">
         <f>AU4+AT5</f>
         <v>2.5471871977358083</v>
       </c>
+      <c r="AV5" s="2">
+        <f t="shared" si="11"/>
+        <v>165.61159218104311</v>
+      </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.0101377271699992</v>
       </c>
@@ -1418,7 +1442,7 @@
         <v>1.1194774874981679</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.35140776789751105</v>
       </c>
       <c r="AJ6" s="2">
@@ -1445,31 +1469,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5974582636996595</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.4169213414927846</v>
       </c>
       <c r="AR6" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.34915420953330917</v>
       </c>
       <c r="AS6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.78361096131964159</v>
       </c>
       <c r="AT6" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1722889375191792</v>
       </c>
       <c r="AU6">
-        <f t="shared" ref="AU6:AU18" si="17">AU5+AT6</f>
+        <f t="shared" ref="AU6:AU18" si="18">AU5+AT6</f>
         <v>3.7194761352549874</v>
       </c>
+      <c r="AV6" s="2">
+        <f t="shared" si="11"/>
+        <v>248.65181696704354</v>
+      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12.176646483900001</v>
       </c>
@@ -1580,7 +1608,7 @@
         <v>1.080624480567558</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.26156800693692328</v>
       </c>
       <c r="AJ7" s="2">
@@ -1607,31 +1635,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5583485062903495</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.2428402698361198</v>
       </c>
       <c r="AR7" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.39154149141951317</v>
       </c>
       <c r="AS7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.1751524527391548</v>
       </c>
       <c r="AT7" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1692121806787794</v>
       </c>
       <c r="AU7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>4.8886883159337664</v>
       </c>
+      <c r="AV7" s="2">
+        <f t="shared" si="11"/>
+        <v>324.76867781279105</v>
+      </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15.449823501799999</v>
       </c>
@@ -1742,7 +1774,7 @@
         <v>1.1257102626068844</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.37353713969442559</v>
       </c>
       <c r="AJ8" s="2">
@@ -1769,31 +1801,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5290331594502045</v>
       </c>
       <c r="AQ8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.1184248019051992</v>
       </c>
       <c r="AR8" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.43489971954479406</v>
       </c>
       <c r="AS8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.6100521722839489</v>
       </c>
       <c r="AT8" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1973315901839605</v>
       </c>
       <c r="AU8">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>6.0860199061177269</v>
       </c>
+      <c r="AV8" s="2">
+        <f t="shared" si="11"/>
+        <v>409.9766882292443</v>
+      </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>18.810443319000001</v>
       </c>
@@ -1904,7 +1940,7 @@
         <v>1.0992842210939227</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.30169095029910487</v>
       </c>
       <c r="AJ9" s="2">
@@ -1931,31 +1967,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5056348650184768</v>
       </c>
       <c r="AQ9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.0226244505572453</v>
       </c>
       <c r="AR9" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.45996597226871672</v>
       </c>
       <c r="AS9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.0700181445526655</v>
       </c>
       <c r="AT9" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1909037067546928</v>
       </c>
       <c r="AU9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.2769236128724195</v>
       </c>
+      <c r="AV9" s="2">
+        <f t="shared" si="11"/>
+        <v>490.2560135850552</v>
+      </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22.1821845652</v>
       </c>
@@ -2066,7 +2106,7 @@
         <v>1.1304304325192822</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.39144160029959618</v>
       </c>
       <c r="AJ10" s="2">
@@ -2093,31 +2133,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4865801781327825</v>
       </c>
       <c r="AQ10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.946796698417784</v>
       </c>
       <c r="AR10" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.47283910294282233</v>
       </c>
       <c r="AS10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.5428572474954878</v>
       </c>
       <c r="AT10" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.1668325093770344</v>
       </c>
       <c r="AU10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.4437561222494537</v>
       </c>
+      <c r="AV10" s="2">
+        <f t="shared" si="11"/>
+        <v>575.61410862042919</v>
+      </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25.4604440606</v>
       </c>
@@ -2228,7 +2272,7 @@
         <v>1.1325965128215971</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.38220477674581477</v>
       </c>
       <c r="AJ11" s="2">
@@ -2255,31 +2299,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.470995298159429</v>
       </c>
       <c r="AQ11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8861820301573067</v>
       </c>
       <c r="AR11" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.46055165618769789</v>
       </c>
       <c r="AS11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.0034089036831855</v>
       </c>
       <c r="AT11" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.0940614323466165</v>
       </c>
       <c r="AU11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.5378175545960708</v>
       </c>
+      <c r="AV11" s="2">
+        <f t="shared" si="11"/>
+        <v>658.73873112344756</v>
+      </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28.5971191999</v>
       </c>
@@ -2390,7 +2438,7 @@
         <v>1.1155052618157155</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.32374408288279932</v>
       </c>
       <c r="AJ12" s="2">
@@ -2417,31 +2465,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4584525263146098</v>
       </c>
       <c r="AQ12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8382892214688829</v>
       </c>
       <c r="AR12" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.42492952929842154</v>
       </c>
       <c r="AS12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.4283384329816071</v>
       </c>
       <c r="AT12" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.97970332099661983</v>
       </c>
       <c r="AU12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.517520875592691</v>
       </c>
+      <c r="AV12" s="2">
+        <f t="shared" si="11"/>
+        <v>735.49600308601498</v>
+      </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>30.854626388900002</v>
       </c>
@@ -2552,7 +2604,7 @@
         <v>1.2362865196733654</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.58894961675155921</v>
       </c>
       <c r="AJ13" s="2">
@@ -2579,31 +2631,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4506159942722798</v>
       </c>
       <c r="AQ13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8087601051314892</v>
       </c>
       <c r="AR13" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.19519751473798011</v>
       </c>
       <c r="AS13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6235359477195872</v>
       </c>
       <c r="AT13" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.44185046223032903</v>
       </c>
       <c r="AU13">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.95937133782302</v>
       </c>
+      <c r="AV13" s="2">
+        <f t="shared" si="11"/>
+        <v>808.35797727790668</v>
+      </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32.080066029599998</v>
       </c>
@@ -2714,7 +2770,7 @@
         <v>1.3736601335826819</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.8161383034495816</v>
       </c>
       <c r="AJ14" s="2">
@@ -2741,31 +2797,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4479976141598188</v>
       </c>
       <c r="AQ14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.7989601576081489</v>
       </c>
       <c r="AR14" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-2.5692097122298814E-2</v>
       </c>
       <c r="AS14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.6492280448418861</v>
       </c>
       <c r="AT14" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.7804014231049541E-2</v>
       </c>
       <c r="AU14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>11.017175352054069</v>
       </c>
+      <c r="AV14" s="2">
+        <f t="shared" si="11"/>
+        <v>885.76059384810037</v>
+      </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32.297219829100001</v>
       </c>
@@ -2876,7 +2936,7 @@
         <v>1.7044308285892225</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.2293372376545952</v>
       </c>
       <c r="AJ15" s="2">
@@ -2903,31 +2963,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4503829472856433</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.807886525406599</v>
       </c>
       <c r="AR15" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.22670660316641431</v>
       </c>
       <c r="AS15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.4225214416754719</v>
       </c>
       <c r="AT15" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.51289627469097221</v>
       </c>
       <c r="AU15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10.504279077363098</v>
       </c>
+      <c r="AV15" s="2">
+        <f t="shared" si="11"/>
+        <v>976.41224289031788</v>
+      </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31.505757123799999</v>
       </c>
@@ -3038,7 +3102,7 @@
         <v>1.3539179547164224</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.77612123631740582</v>
       </c>
       <c r="AJ16" s="2">
@@ -3065,31 +3129,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4576435805439203</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8352271151267998</v>
       </c>
       <c r="AR16" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.35329426396972924</v>
       </c>
       <c r="AS16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.0692271777057427</v>
       </c>
       <c r="AT16" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.81299164342558139</v>
       </c>
       <c r="AU16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.6912874339375161</v>
       </c>
+      <c r="AV16" s="2">
+        <f t="shared" si="11"/>
+        <v>1013.9586074513988</v>
+      </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32.253108226000002</v>
       </c>
@@ -3200,7 +3268,7 @@
         <v>1.1563625302328298</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.40863929986454189</v>
       </c>
       <c r="AJ17" s="2">
@@ -3227,31 +3295,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.461412835230103</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8495223449663918</v>
       </c>
       <c r="AR17" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-6.606236409583767E-2</v>
       </c>
       <c r="AS17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.1352895418015803</v>
       </c>
       <c r="AT17" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.15338113767658354</v>
       </c>
       <c r="AU17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.8446685716141005</v>
       </c>
+      <c r="AV17" s="2">
+        <f t="shared" si="11"/>
+        <v>1059.6112910714935</v>
+      </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31.807406181800001</v>
       </c>
@@ -3362,7 +3434,7 @@
         <v>1.3119909709983766</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.69656790833585913</v>
       </c>
       <c r="AJ18" s="2">
@@ -3389,31 +3461,35 @@
         <v>40798.57518375088</v>
       </c>
       <c r="AP18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.4635519513705091</v>
       </c>
       <c r="AQ18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.8576663285348212</v>
       </c>
       <c r="AR18" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21981316973443407</v>
       </c>
       <c r="AS18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.9154763720671464</v>
       </c>
       <c r="AT18" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-0.51295321714130371</v>
       </c>
       <c r="AU18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.3317153544727969</v>
       </c>
+      <c r="AV18" s="2">
+        <f t="shared" si="11"/>
+        <v>1090.6217468023619</v>
+      </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31.567336453999999</v>
       </c>
@@ -3500,7 +3576,7 @@
         <v>-8.4108845215175485</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31.4068883148</v>
       </c>
@@ -3587,7 +3663,7 @@
         <v>-8.9525746769235415</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31.270712094699999</v>
       </c>
@@ -3674,7 +3750,7 @@
         <v>-9.3346573756835518</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>31.137649633700001</v>
       </c>

</xml_diff>

<commit_message>
Validate analytical solution with simulation data in the PE geosynthetic container case
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:AV22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
+      <selection activeCell="AV1" sqref="AV1:AV1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -829,8 +829,8 @@
         <v>0</v>
       </c>
       <c r="AV2" s="2">
-        <f>(AQ2*X2-2*X2*(1-0.01*P2-2*0.01*AF2)/(-0.08/0.4*0.01*P2-(2*0.08/0.4+3)*0.01*AF2+1+0.08/0.4)+4*0.5*232000*(-0.4*0.01*AF2-0.08*0.01*P2)/((1-2*0.01*AF2)*0.4*0.08))/1000</f>
-        <v>-2.389488768044183</v>
+        <f>(AQ2*X2-4*X2*(1-0.01*P2-2*0.01*AF2)*(0.08/0.4)/(-0.08/0.4*0.01*P2-(2*0.08/0.4+3)*0.01*AF2+0.08/0.4+1))/1000</f>
+        <v>-0.95579557395708714</v>
       </c>
     </row>
     <row r="3" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -995,8 +995,8 @@
         <v>0.57237542883510506</v>
       </c>
       <c r="AV3" s="2">
-        <f t="shared" ref="AV3:AV18" si="11">(AQ3*X3-2*X3*(1-0.01*P3-2*0.01*AF3)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+1+0.08/0.4)+4*0.5*232000*(-0.4*0.01*AF3-0.08*0.01*P3)/((1-2*0.01*AF3)*0.4*0.08))/1000</f>
-        <v>43.490396860164267</v>
+        <f t="shared" ref="AV3:AV18" si="11">(AQ3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
+        <v>61.573331518164267</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="AV4" s="2">
         <f t="shared" si="11"/>
-        <v>100.38870592819272</v>
+        <v>123.63582364180566</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="AV5" s="2">
         <f t="shared" si="11"/>
-        <v>165.61159218104311</v>
+        <v>193.61859757528433</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
       </c>
       <c r="AV6" s="2">
         <f t="shared" si="11"/>
-        <v>248.65181696704354</v>
+        <v>268.73281207978994</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="AV7" s="2">
         <f t="shared" si="11"/>
-        <v>324.76867781279105</v>
+        <v>341.68565419548128</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="AV8" s="2">
         <f t="shared" si="11"/>
-        <v>409.9766882292443</v>
+        <v>416.42950066425135</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="AV9" s="2">
         <f t="shared" si="11"/>
-        <v>490.2560135850552</v>
+        <v>490.76000851941723</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="AV10" s="2">
         <f t="shared" si="11"/>
-        <v>575.61410862042919</v>
+        <v>564.22397859727892</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="AV11" s="2">
         <f t="shared" si="11"/>
-        <v>658.73873112344756</v>
+        <v>635.17882804811688</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
@@ -2490,7 +2490,7 @@
       </c>
       <c r="AV12" s="2">
         <f t="shared" si="11"/>
-        <v>735.49600308601498</v>
+        <v>701.86092936402974</v>
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="AV13" s="2">
         <f t="shared" si="11"/>
-        <v>808.35797727790668</v>
+        <v>737.06366727525415</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="AV14" s="2">
         <f t="shared" si="11"/>
-        <v>885.76059384810037</v>
+        <v>753.96217613891213</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="AV15" s="2">
         <f t="shared" si="11"/>
-        <v>976.41224289031788</v>
+        <v>735.40119360157871</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
       </c>
       <c r="AV16" s="2">
         <f t="shared" si="11"/>
-        <v>1013.9586074513988</v>
+        <v>708.58070636773732</v>
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="AV17" s="2">
         <f t="shared" si="11"/>
-        <v>1059.6112910714935</v>
+        <v>729.31752827366404</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
       </c>
       <c r="AV18" s="2">
         <f t="shared" si="11"/>
-        <v>1090.6217468023619</v>
+        <v>708.70349050179982</v>
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Use tartget fuction f(x,y) =c/y+(M^2-x^2)/(2*x)
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -109,6 +109,54 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>q</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D/E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dratio</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>K_p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev_pla_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev_pla_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_n_real_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>ev_ela</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -117,6 +165,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>eq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>er_from_ev</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -130,58 +182,6 @@
   </si>
   <si>
     <t>dev/deq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>p</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>q</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D/E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dratio</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>K_p</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev_pla_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_pla_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev/deq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eq_pla</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>s_n_real_pred</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AV22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AV1" sqref="AV1:AV1048576"/>
+      <selection activeCell="AH3" sqref="AH3:AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -538,8 +538,10 @@
     <col min="19" max="26" width="13.77734375"/>
     <col min="27" max="27" width="12.77734375"/>
     <col min="28" max="28" width="11.5546875"/>
+    <col min="29" max="30" width="8.88671875" style="2"/>
     <col min="31" max="31" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.109375" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" style="2" customWidth="1"/>
+    <col min="33" max="35" width="8.88671875" style="2"/>
     <col min="36" max="36" width="12.88671875" customWidth="1"/>
     <col min="39" max="39" width="8.88671875" style="2"/>
     <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -635,65 +637,65 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>30</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
       </c>
       <c r="AM1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AN1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AU1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
@@ -782,19 +784,19 @@
         <f t="shared" ref="AB2:AB22" si="0">-100*((H2+1)/(0.6685676252+1)-1)</f>
         <v>-2.8766988791062431E-9</v>
       </c>
-      <c r="AC2">
-        <f>0.0762*AK2^0.2606-0.5912</f>
-        <v>-2.4003601210058623E-3</v>
-      </c>
-      <c r="AD2">
+      <c r="AC2" s="2">
+        <f>1.34 *((AK2/100000)^0.3-(2594/100000)^0.3)</f>
+        <v>-1.9765021816098051E-3</v>
+      </c>
+      <c r="AD2" s="2">
         <f>AB2-AC2</f>
-        <v>2.4003572443069832E-3</v>
-      </c>
-      <c r="AE2" s="3">
-        <f>P2-AB2/3-2*(1.35*(AK2/3255000)^-0.0723)*(1+0.33)/(9*(1-2*0.33))</f>
-        <v>-1.9678144869574707</v>
-      </c>
-      <c r="AF2">
+        <v>1.976499304910926E-3</v>
+      </c>
+      <c r="AE2" s="4">
+        <f>P2-AB2/3</f>
+        <v>9.588996263687477E-10</v>
+      </c>
+      <c r="AF2" s="2">
         <f t="shared" ref="AF2:AF18" si="1">AB2-P2/2</f>
         <v>-2.8766988791062431E-9</v>
       </c>
@@ -919,36 +921,36 @@
         <f t="shared" si="0"/>
         <v>0.42455699990888718</v>
       </c>
-      <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC18" si="6">0.0762*AK3^0.2606-0.5912</f>
-        <v>0.41458661901056004</v>
-      </c>
-      <c r="AD3" s="1">
+      <c r="AC3" s="2">
+        <f t="shared" ref="AC3:AC18" si="6">1.34 *((AK3/100000)^0.3-(2594/100000)^0.3)</f>
+        <v>0.37815519616697812</v>
+      </c>
+      <c r="AD3" s="2">
         <f t="shared" ref="AD3:AD18" si="7">AB3-AC3</f>
-        <v>9.9703808983271358E-3</v>
-      </c>
-      <c r="AE3" s="3">
-        <f t="shared" ref="AE3:AE18" si="8">P3-AB3/3-2*(1.35*(AK3/3255000)^-0.0723)*(1+0.33)/(9*(1-2*0.33))</f>
-        <v>-0.83177500520751779</v>
-      </c>
-      <c r="AF3" s="1">
+        <v>4.6401803741909053E-2</v>
+      </c>
+      <c r="AE3" s="4">
+        <f t="shared" ref="AE3:AE18" si="8">P3-AB3/3</f>
+        <v>0.86439544855037098</v>
+      </c>
+      <c r="AF3" s="2">
         <f t="shared" si="1"/>
         <v>-7.8400224351112824E-2</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="3">
         <f t="shared" ref="AG3:AH18" si="9">AD3-AD2</f>
-        <v>7.5700236540201526E-3</v>
-      </c>
-      <c r="AH3" s="1">
+        <v>4.4425304436998131E-2</v>
+      </c>
+      <c r="AH3" s="3">
         <f t="shared" si="9"/>
-        <v>1.1360394817499531</v>
-      </c>
-      <c r="AI3" s="1">
-        <f>-AG3/AH3</f>
-        <v>-6.6635216254626135E-3</v>
+        <v>0.86439544759147136</v>
+      </c>
+      <c r="AI3" s="2">
+        <f t="shared" ref="AI3:AI18" si="10">-AG3/AH3</f>
+        <v>-5.1394653408672643E-2</v>
       </c>
       <c r="AJ3" s="2">
-        <f t="shared" ref="AJ3:AJ18" si="10">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
+        <f t="shared" ref="AJ3:AJ18" si="11">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
         <v>3.1368433750215918E-2</v>
       </c>
       <c r="AK3" s="1">
@@ -995,7 +997,7 @@
         <v>0.57237542883510506</v>
       </c>
       <c r="AV3" s="2">
-        <f t="shared" ref="AV3:AV18" si="11">(AQ3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
+        <f t="shared" ref="AV3:AV18" si="12">(AQ3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
         <v>61.573331518164267</v>
       </c>
     </row>
@@ -1085,36 +1087,36 @@
         <f t="shared" si="0"/>
         <v>0.53723081921390747</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="2">
         <f t="shared" si="6"/>
-        <v>0.69544295971520387</v>
-      </c>
-      <c r="AD4">
+        <v>0.64894857499996228</v>
+      </c>
+      <c r="AD4" s="2">
         <f t="shared" si="7"/>
-        <v>-0.15821214050129639</v>
-      </c>
-      <c r="AE4" s="3">
+        <v>-0.11171775578605481</v>
+      </c>
+      <c r="AE4" s="4">
         <f t="shared" si="8"/>
-        <v>0.24293542161306259</v>
-      </c>
-      <c r="AF4">
+        <v>1.8270880839220307</v>
+      </c>
+      <c r="AF4" s="2">
         <f t="shared" si="1"/>
         <v>-0.46585169261609249</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="3">
         <f t="shared" si="9"/>
-        <v>-0.16818252139962353</v>
-      </c>
-      <c r="AH4">
+        <v>-0.15811955952796386</v>
+      </c>
+      <c r="AH4" s="3">
         <f t="shared" si="9"/>
-        <v>1.0747104268205803</v>
-      </c>
-      <c r="AI4">
-        <f t="shared" ref="AI4:AI18" si="12">-AG4/AH4</f>
-        <v>0.15649101116211753</v>
+        <v>0.96269263537165972</v>
+      </c>
+      <c r="AI4" s="2">
+        <f t="shared" si="10"/>
+        <v>0.16424718930868293</v>
       </c>
       <c r="AJ4" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16912422089899823</v>
       </c>
       <c r="AK4">
@@ -1161,7 +1163,7 @@
         <v>1.4816133805135034</v>
       </c>
       <c r="AV4" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>123.63582364180566</v>
       </c>
     </row>
@@ -1251,36 +1253,36 @@
         <f t="shared" si="0"/>
         <v>0.57836850681094454</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="2">
         <f t="shared" si="6"/>
-        <v>0.90101321517751964</v>
-      </c>
-      <c r="AD5">
+        <v>0.85304626901129565</v>
+      </c>
+      <c r="AD5" s="2">
         <f t="shared" si="7"/>
-        <v>-0.32264470836657511</v>
-      </c>
-      <c r="AE5" s="3">
+        <v>-0.27467776220035112</v>
+      </c>
+      <c r="AE5" s="4">
         <f t="shared" si="8"/>
-        <v>1.292854333240729</v>
-      </c>
-      <c r="AF5">
+        <v>2.8131835652496848</v>
+      </c>
+      <c r="AF5" s="2">
         <f t="shared" si="1"/>
         <v>-0.92461802694905537</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="3">
         <f t="shared" si="9"/>
-        <v>-0.16443256786527871</v>
-      </c>
-      <c r="AH5">
+        <v>-0.16296000641429631</v>
+      </c>
+      <c r="AH5" s="3">
         <f t="shared" si="9"/>
-        <v>1.0499189116276664</v>
-      </c>
-      <c r="AI5">
-        <f t="shared" si="12"/>
-        <v>0.15661454046042708</v>
+        <v>0.98609548132765412</v>
+      </c>
+      <c r="AI5" s="2">
+        <f t="shared" si="10"/>
+        <v>0.16525783709594841</v>
       </c>
       <c r="AJ5" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.2465601787796606</v>
       </c>
       <c r="AK5">
@@ -1327,7 +1329,7 @@
         <v>2.5471871977358083</v>
       </c>
       <c r="AV5" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>193.61859757528433</v>
       </c>
     </row>
@@ -1417,36 +1419,36 @@
         <f t="shared" si="0"/>
         <v>0.35070042781746302</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="2">
         <f t="shared" si="6"/>
-        <v>1.0667382212772831</v>
-      </c>
-      <c r="AD6">
+        <v>1.0207434038263898</v>
+      </c>
+      <c r="AD6" s="2">
         <f t="shared" si="7"/>
-        <v>-0.7160377934598201</v>
-      </c>
-      <c r="AE6" s="3">
+        <v>-0.67004297600892682</v>
+      </c>
+      <c r="AE6" s="4">
         <f t="shared" si="8"/>
-        <v>2.4123318207388968</v>
-      </c>
-      <c r="AF6">
+        <v>3.8888826306841788</v>
+      </c>
+      <c r="AF6" s="2">
         <f t="shared" si="1"/>
         <v>-1.652190958827537</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="3">
         <f t="shared" si="9"/>
-        <v>-0.393393085093245</v>
-      </c>
-      <c r="AH6">
+        <v>-0.3953652138085757</v>
+      </c>
+      <c r="AH6" s="3">
         <f t="shared" si="9"/>
-        <v>1.1194774874981679</v>
-      </c>
-      <c r="AI6">
-        <f t="shared" si="12"/>
-        <v>0.35140776789751105</v>
+        <v>1.075699065434494</v>
+      </c>
+      <c r="AI6" s="2">
+        <f t="shared" si="10"/>
+        <v>0.36754258371404336</v>
       </c>
       <c r="AJ6" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.29783972053186508</v>
       </c>
       <c r="AK6">
@@ -1493,7 +1495,7 @@
         <v>3.7194761352549874</v>
       </c>
       <c r="AV6" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>268.73281207978994</v>
       </c>
     </row>
@@ -1583,36 +1585,36 @@
         <f t="shared" si="0"/>
         <v>0.19999993483033052</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="2">
         <f t="shared" si="6"/>
-        <v>1.1986945199194547</v>
-      </c>
-      <c r="AD7">
+        <v>1.1561091253948397</v>
+      </c>
+      <c r="AD7" s="2">
         <f t="shared" si="7"/>
-        <v>-0.99869458508912423</v>
-      </c>
-      <c r="AE7" s="3">
+        <v>-0.95610919056450916</v>
+      </c>
+      <c r="AE7" s="4">
         <f t="shared" si="8"/>
-        <v>3.4929563013064548</v>
-      </c>
-      <c r="AF7">
+        <v>4.9384663104565565</v>
+      </c>
+      <c r="AF7" s="2">
         <f t="shared" si="1"/>
         <v>-2.3025665428696693</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="3">
         <f t="shared" si="9"/>
-        <v>-0.28265679162930413</v>
-      </c>
-      <c r="AH7">
+        <v>-0.28606621455558234</v>
+      </c>
+      <c r="AH7" s="3">
         <f t="shared" si="9"/>
-        <v>1.080624480567558</v>
-      </c>
-      <c r="AI7">
-        <f t="shared" si="12"/>
-        <v>0.26156800693692328</v>
+        <v>1.0495836797723777</v>
+      </c>
+      <c r="AI7" s="2">
+        <f t="shared" si="10"/>
+        <v>0.27255207952320798</v>
       </c>
       <c r="AJ7" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.33487633629698077</v>
       </c>
       <c r="AK7">
@@ -1659,7 +1661,7 @@
         <v>4.8886883159337664</v>
       </c>
       <c r="AV7" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>341.68565419548128</v>
       </c>
     </row>
@@ -1749,36 +1751,36 @@
         <f t="shared" si="0"/>
         <v>-0.10677972586135009</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="2">
         <f t="shared" si="6"/>
-        <v>1.3124094508466104</v>
-      </c>
-      <c r="AD8">
+        <v>1.2739837410670807</v>
+      </c>
+      <c r="AD8" s="2">
         <f t="shared" si="7"/>
-        <v>-1.4191891767079605</v>
-      </c>
-      <c r="AE8" s="3">
+        <v>-1.3807634669284308</v>
+      </c>
+      <c r="AE8" s="4">
         <f t="shared" si="8"/>
-        <v>4.6186665639133393</v>
-      </c>
-      <c r="AF8">
+        <v>6.0396844916037837</v>
+      </c>
+      <c r="AF8" s="2">
         <f t="shared" si="1"/>
         <v>-3.1088253506863501</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="3">
         <f t="shared" si="9"/>
-        <v>-0.42049459161883629</v>
-      </c>
-      <c r="AH8">
+        <v>-0.42465427636392161</v>
+      </c>
+      <c r="AH8" s="3">
         <f t="shared" si="9"/>
-        <v>1.1257102626068844</v>
-      </c>
-      <c r="AI8">
-        <f t="shared" si="12"/>
-        <v>0.37353713969442559</v>
+        <v>1.1012181811472272</v>
+      </c>
+      <c r="AI8" s="2">
+        <f t="shared" si="10"/>
+        <v>0.38562228960070855</v>
       </c>
       <c r="AJ8" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.36322412530515052</v>
       </c>
       <c r="AK8">
@@ -1825,7 +1827,7 @@
         <v>6.0860199061177269</v>
       </c>
       <c r="AV8" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>416.42950066425135</v>
       </c>
     </row>
@@ -1915,36 +1917,36 @@
         <f t="shared" si="0"/>
         <v>-0.34012835873640235</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="2">
         <f t="shared" si="6"/>
-        <v>1.410704919282195</v>
-      </c>
-      <c r="AD9">
+        <v>1.3767389866898236</v>
+      </c>
+      <c r="AD9" s="2">
         <f t="shared" si="7"/>
-        <v>-1.7508332780185973</v>
-      </c>
-      <c r="AE9" s="3">
+        <v>-1.716867345426226</v>
+      </c>
+      <c r="AE9" s="4">
         <f t="shared" si="8"/>
-        <v>5.7179507850072619</v>
-      </c>
-      <c r="AF9">
+        <v>7.1192576157988006</v>
+      </c>
+      <c r="AF9" s="2">
         <f t="shared" si="1"/>
         <v>-3.8430691068464022</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="3">
         <f t="shared" si="9"/>
-        <v>-0.33164410131063682</v>
-      </c>
-      <c r="AH9">
+        <v>-0.33610387849779522</v>
+      </c>
+      <c r="AH9" s="3">
         <f t="shared" si="9"/>
-        <v>1.0992842210939227</v>
-      </c>
-      <c r="AI9">
-        <f t="shared" si="12"/>
-        <v>0.30169095029910487</v>
+        <v>1.0795731241950168</v>
+      </c>
+      <c r="AI9" s="2">
+        <f t="shared" si="10"/>
+        <v>0.31133034989955954</v>
       </c>
       <c r="AJ9" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.38623271525634967</v>
       </c>
       <c r="AK9">
@@ -1991,7 +1993,7 @@
         <v>7.2769236128724195</v>
       </c>
       <c r="AV9" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>490.76000851941723</v>
       </c>
     </row>
@@ -2081,36 +2083,36 @@
         <f t="shared" si="0"/>
         <v>-0.69687079219256098</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" s="2">
         <f t="shared" si="6"/>
-        <v>1.4964599833587491</v>
-      </c>
-      <c r="AD10">
+        <v>1.467011534629955</v>
+      </c>
+      <c r="AD10" s="2">
         <f t="shared" si="7"/>
-        <v>-2.1933307755513098</v>
-      </c>
-      <c r="AE10" s="3">
+        <v>-2.1638823268225158</v>
+      </c>
+      <c r="AE10" s="4">
         <f t="shared" si="8"/>
-        <v>6.8483812175265442</v>
-      </c>
-      <c r="AF10">
+        <v>8.2334755863341869</v>
+      </c>
+      <c r="AF10" s="2">
         <f t="shared" si="1"/>
         <v>-4.6974634533275612</v>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="3">
         <f t="shared" si="9"/>
-        <v>-0.4424974975327125</v>
-      </c>
-      <c r="AH10">
+        <v>-0.44701498139628981</v>
+      </c>
+      <c r="AH10" s="3">
         <f t="shared" si="9"/>
-        <v>1.1304304325192822</v>
-      </c>
-      <c r="AI10">
-        <f t="shared" si="12"/>
-        <v>0.39144160029959618</v>
+        <v>1.1142179705353863</v>
+      </c>
+      <c r="AI10" s="2">
+        <f t="shared" si="10"/>
+        <v>0.40119168171511116</v>
       </c>
       <c r="AJ10" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.40523305542392607</v>
       </c>
       <c r="AK10">
@@ -2157,7 +2159,7 @@
         <v>8.4437561222494537</v>
       </c>
       <c r="AV10" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>564.22397859727892</v>
       </c>
     </row>
@@ -2247,36 +2249,36 @@
         <f t="shared" si="0"/>
         <v>-1.0567213372539408</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="2">
         <f t="shared" si="6"/>
-        <v>1.5694932356234361</v>
-      </c>
-      <c r="AD11">
+        <v>1.5443363891529516</v>
+      </c>
+      <c r="AD11" s="2">
         <f t="shared" si="7"/>
-        <v>-2.6262145728773767</v>
-      </c>
-      <c r="AE11" s="3">
+        <v>-2.6010577264068924</v>
+      </c>
+      <c r="AE11" s="4">
         <f t="shared" si="8"/>
-        <v>7.9809777303481413</v>
-      </c>
-      <c r="AF11">
+        <v>9.3529214808213137</v>
+      </c>
+      <c r="AF11" s="2">
         <f t="shared" si="1"/>
         <v>-5.557061854788941</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="3">
         <f t="shared" si="9"/>
-        <v>-0.43288379732606685</v>
-      </c>
-      <c r="AH11">
+        <v>-0.43717539958437657</v>
+      </c>
+      <c r="AH11" s="3">
         <f t="shared" si="9"/>
-        <v>1.1325965128215971</v>
-      </c>
-      <c r="AI11">
-        <f t="shared" si="12"/>
-        <v>0.38220477674581477</v>
+        <v>1.1194458944871268</v>
+      </c>
+      <c r="AI11" s="2">
+        <f t="shared" si="10"/>
+        <v>0.39052838706837911</v>
       </c>
       <c r="AJ11" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.42095593773000084</v>
       </c>
       <c r="AK11">
@@ -2323,7 +2325,7 @@
         <v>9.5378175545960708</v>
       </c>
       <c r="AV11" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>635.17882804811688</v>
       </c>
     </row>
@@ -2413,36 +2415,36 @@
         <f t="shared" si="0"/>
         <v>-1.3573824484509611</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" s="2">
         <f t="shared" si="6"/>
-        <v>1.6299703523638815</v>
-      </c>
-      <c r="AD12">
+        <v>1.6086676769888566</v>
+      </c>
+      <c r="AD12" s="2">
         <f t="shared" si="7"/>
-        <v>-2.9873528008148424</v>
-      </c>
-      <c r="AE12" s="3">
+        <v>-2.9660501254398177</v>
+      </c>
+      <c r="AE12" s="4">
         <f t="shared" si="8"/>
-        <v>9.0964829921638568</v>
-      </c>
-      <c r="AF12">
+        <v>10.457959603650322</v>
+      </c>
+      <c r="AF12" s="2">
         <f t="shared" si="1"/>
         <v>-6.3601318422009614</v>
       </c>
-      <c r="AG12">
+      <c r="AG12" s="3">
         <f t="shared" si="9"/>
-        <v>-0.36113822793746575</v>
-      </c>
-      <c r="AH12">
+        <v>-0.36499239903292535</v>
+      </c>
+      <c r="AH12" s="3">
         <f t="shared" si="9"/>
-        <v>1.1155052618157155</v>
-      </c>
-      <c r="AI12">
-        <f t="shared" si="12"/>
-        <v>0.32374408288279932</v>
+        <v>1.1050381228290078</v>
+      </c>
+      <c r="AI12" s="2">
+        <f t="shared" si="10"/>
+        <v>0.330298467982723</v>
       </c>
       <c r="AJ12" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.4337328660539343</v>
       </c>
       <c r="AK12">
@@ -2489,7 +2491,7 @@
         <v>10.517520875592691</v>
       </c>
       <c r="AV12" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>701.86092936402974</v>
       </c>
     </row>
@@ -2579,36 +2581,36 @@
         <f t="shared" si="0"/>
         <v>-2.0595318912459915</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="2">
         <f t="shared" si="6"/>
-        <v>1.6559313815255983</v>
-      </c>
-      <c r="AD13">
+        <v>1.6363649598467622</v>
+      </c>
+      <c r="AD13" s="2">
         <f t="shared" si="7"/>
-        <v>-3.7154632727715899</v>
-      </c>
-      <c r="AE13" s="3">
+        <v>-3.6958968510927539</v>
+      </c>
+      <c r="AE13" s="4">
         <f t="shared" si="8"/>
-        <v>10.332769511837222</v>
-      </c>
-      <c r="AF13">
+        <v>11.68986396061533</v>
+      </c>
+      <c r="AF13" s="2">
         <f t="shared" si="1"/>
         <v>-7.5612085563459912</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="3">
         <f t="shared" si="9"/>
-        <v>-0.7281104719567475</v>
-      </c>
-      <c r="AH13">
+        <v>-0.72984672565293618</v>
+      </c>
+      <c r="AH13" s="3">
         <f t="shared" si="9"/>
-        <v>1.2362865196733654</v>
-      </c>
-      <c r="AI13">
-        <f t="shared" si="12"/>
-        <v>0.58894961675155921</v>
+        <v>1.2319043569650088</v>
+      </c>
+      <c r="AI13" s="2">
+        <f t="shared" si="10"/>
+        <v>0.59245405012693442</v>
       </c>
       <c r="AJ13" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.44177279741358977</v>
       </c>
       <c r="AK13">
@@ -2655,7 +2657,7 @@
         <v>10.95937133782302</v>
       </c>
       <c r="AV13" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>737.06366727525415</v>
       </c>
     </row>
@@ -2745,36 +2747,36 @@
         <f t="shared" si="0"/>
         <v>-3.1772879905688667</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="2">
         <f t="shared" si="6"/>
-        <v>1.6592719331412191</v>
-      </c>
-      <c r="AD14">
+        <v>1.6399324512181561</v>
+      </c>
+      <c r="AD14" s="2">
         <f t="shared" si="7"/>
-        <v>-4.8365599237100856</v>
-      </c>
-      <c r="AE14" s="3">
+        <v>-4.8172204417870228</v>
+      </c>
+      <c r="AE14" s="4">
         <f t="shared" si="8"/>
-        <v>11.706429645419904</v>
-      </c>
-      <c r="AF14">
+        <v>13.062964914256289</v>
+      </c>
+      <c r="AF14" s="2">
         <f t="shared" si="1"/>
         <v>-9.1792224492688668</v>
       </c>
-      <c r="AG14">
+      <c r="AG14" s="3">
         <f t="shared" si="9"/>
-        <v>-1.1210966509384956</v>
-      </c>
-      <c r="AH14">
+        <v>-1.1213235906942689</v>
+      </c>
+      <c r="AH14" s="3">
         <f t="shared" si="9"/>
-        <v>1.3736601335826819</v>
-      </c>
-      <c r="AI14">
-        <f t="shared" si="12"/>
-        <v>0.8161383034495816</v>
+        <v>1.3731009536409591</v>
+      </c>
+      <c r="AI14" s="2">
+        <f t="shared" si="10"/>
+        <v>0.81663594196838252</v>
       </c>
       <c r="AJ14" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.44446908167319388</v>
       </c>
       <c r="AK14">
@@ -2821,7 +2823,7 @@
         <v>11.017175352054069</v>
       </c>
       <c r="AV14" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>753.96217613891213</v>
       </c>
     </row>
@@ -2911,36 +2913,36 @@
         <f t="shared" si="0"/>
         <v>-5.3026998397139868</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" s="2">
         <f t="shared" si="6"/>
-        <v>1.6291803705873067</v>
-      </c>
-      <c r="AD15">
+        <v>1.6078256260480841</v>
+      </c>
+      <c r="AD15" s="2">
         <f t="shared" si="7"/>
-        <v>-6.9318802103012933</v>
-      </c>
-      <c r="AE15" s="3">
+        <v>-6.9105254657620705</v>
+      </c>
+      <c r="AE15" s="4">
         <f t="shared" si="8"/>
-        <v>13.410860474009127</v>
-      </c>
-      <c r="AF15">
+        <v>14.772471457237996</v>
+      </c>
+      <c r="AF15" s="2">
         <f t="shared" si="1"/>
         <v>-11.805152261713987</v>
       </c>
-      <c r="AG15">
+      <c r="AG15" s="3">
         <f t="shared" si="9"/>
-        <v>-2.0953202865912077</v>
-      </c>
-      <c r="AH15">
+        <v>-2.0933050239750477</v>
+      </c>
+      <c r="AH15" s="3">
         <f t="shared" si="9"/>
-        <v>1.7044308285892225</v>
-      </c>
-      <c r="AI15">
-        <f t="shared" si="12"/>
-        <v>1.2293372376545952</v>
+        <v>1.7095065429817069</v>
+      </c>
+      <c r="AI15" s="2">
+        <f t="shared" si="10"/>
+        <v>1.2245083428133143</v>
       </c>
       <c r="AJ15" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.44201257516055953</v>
       </c>
       <c r="AK15">
@@ -2987,7 +2989,7 @@
         <v>10.504279077363098</v>
       </c>
       <c r="AV15" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>735.40119360157871</v>
       </c>
     </row>
@@ -3077,36 +3079,36 @@
         <f t="shared" si="0"/>
         <v>-6.403433079926435</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" s="2">
         <f t="shared" si="6"/>
-        <v>1.5792516072617018</v>
-      </c>
-      <c r="AD16">
+        <v>1.5546984421060532</v>
+      </c>
+      <c r="AD16" s="2">
         <f t="shared" si="7"/>
-        <v>-7.9826846871881365</v>
-      </c>
-      <c r="AE16" s="3">
+        <v>-7.9581315220324882</v>
+      </c>
+      <c r="AE16" s="4">
         <f t="shared" si="8"/>
-        <v>14.764778428725549</v>
-      </c>
-      <c r="AF16">
+        <v>16.13500808720881</v>
+      </c>
+      <c r="AF16" s="2">
         <f t="shared" si="1"/>
         <v>-13.403698276876435</v>
       </c>
-      <c r="AG16">
+      <c r="AG16" s="3">
         <f t="shared" si="9"/>
-        <v>-1.0508044768868432</v>
-      </c>
-      <c r="AH16">
+        <v>-1.0476060562704177</v>
+      </c>
+      <c r="AH16" s="3">
         <f t="shared" si="9"/>
-        <v>1.3539179547164224</v>
-      </c>
-      <c r="AI16">
-        <f t="shared" si="12"/>
-        <v>0.77612123631740582</v>
+        <v>1.3625366299708137</v>
+      </c>
+      <c r="AI16" s="2">
+        <f t="shared" si="10"/>
+        <v>0.76886450846672505</v>
       </c>
       <c r="AJ16" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.43456075696068175</v>
       </c>
       <c r="AK16">
@@ -3153,7 +3155,7 @@
         <v>9.6912874339375161</v>
       </c>
       <c r="AV16" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>708.58070636773732</v>
       </c>
     </row>
@@ -3243,36 +3245,36 @@
         <f t="shared" si="0"/>
         <v>-6.8663253380735645</v>
       </c>
-      <c r="AC17">
+      <c r="AC17" s="2">
         <f t="shared" si="6"/>
-        <v>1.5888945238585055</v>
-      </c>
-      <c r="AD17">
+        <v>1.5649448192025073</v>
+      </c>
+      <c r="AD17" s="2">
         <f t="shared" si="7"/>
-        <v>-8.4552198619320702</v>
-      </c>
-      <c r="AE17" s="3">
+        <v>-8.4312701572760709</v>
+      </c>
+      <c r="AE17" s="4">
         <f t="shared" si="8"/>
-        <v>15.921140958958379</v>
-      </c>
-      <c r="AF17">
+        <v>17.289686448891189</v>
+      </c>
+      <c r="AF17" s="2">
         <f t="shared" si="1"/>
         <v>-14.366781006173564</v>
       </c>
-      <c r="AG17">
+      <c r="AG17" s="3">
         <f t="shared" si="9"/>
-        <v>-0.47253517474393369</v>
-      </c>
-      <c r="AH17">
+        <v>-0.47313863524358268</v>
+      </c>
+      <c r="AH17" s="3">
         <f t="shared" si="9"/>
-        <v>1.1563625302328298</v>
-      </c>
-      <c r="AI17">
-        <f t="shared" si="12"/>
-        <v>0.40863929986454189</v>
+        <v>1.1546783616823788</v>
+      </c>
+      <c r="AI17" s="2">
+        <f t="shared" si="10"/>
+        <v>0.40975794727305237</v>
       </c>
       <c r="AJ17" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.43070722447720716</v>
       </c>
       <c r="AK17">
@@ -3319,7 +3321,7 @@
         <v>9.8446685716141005</v>
       </c>
       <c r="AV17" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>729.31752827366404</v>
       </c>
     </row>
@@ -3409,36 +3411,36 @@
         <f t="shared" si="0"/>
         <v>-7.8129003470491121</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" s="2">
         <f t="shared" si="6"/>
-        <v>1.5562103213068299</v>
-      </c>
-      <c r="AD18">
+        <v>1.530243126630487</v>
+      </c>
+      <c r="AD18" s="2">
         <f t="shared" si="7"/>
-        <v>-9.3691106683559422</v>
-      </c>
-      <c r="AE18" s="3">
+        <v>-9.3431434736796</v>
+      </c>
+      <c r="AE18" s="4">
         <f t="shared" si="8"/>
-        <v>17.233131929956755</v>
-      </c>
-      <c r="AF18">
+        <v>18.607424828283037</v>
+      </c>
+      <c r="AF18" s="2">
         <f t="shared" si="1"/>
         <v>-15.814462703349111</v>
       </c>
-      <c r="AG18">
+      <c r="AG18" s="3">
         <f t="shared" si="9"/>
-        <v>-0.91389080642387199</v>
-      </c>
-      <c r="AH18">
+        <v>-0.91187331640352909</v>
+      </c>
+      <c r="AH18" s="3">
         <f t="shared" si="9"/>
-        <v>1.3119909709983766</v>
-      </c>
-      <c r="AI18">
-        <f t="shared" si="12"/>
-        <v>0.69656790833585913</v>
+        <v>1.317738379391848</v>
+      </c>
+      <c r="AI18" s="2">
+        <f t="shared" si="10"/>
+        <v>0.69199875382271969</v>
       </c>
       <c r="AJ18" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.42852479015426859</v>
       </c>
       <c r="AK18">
@@ -3485,7 +3487,7 @@
         <v>9.3317153544727969</v>
       </c>
       <c r="AV18" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>708.70349050179982</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Consider characteristic state line + failure state line for stress state
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -105,10 +105,6 @@
     <t>ev</t>
   </si>
   <si>
-    <t>K_phi</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>p</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -125,63 +121,67 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>K_p</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev_pla_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev_pla_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_n_real_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev_ela</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ev_pla</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>er_from_ev</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev_pla</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>dratio</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>K_p</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev_pla_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_pla_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev/deq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>s_n_real_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_ela</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ev_pla</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>er_from_ev</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev_pla</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dev/deq</t>
+    <t>K_phi</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AV22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH12"/>
+      <selection activeCell="AM1" sqref="AM1:AM1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -545,7 +545,7 @@
     <col min="36" max="36" width="12.88671875" customWidth="1"/>
     <col min="39" max="39" width="8.88671875" style="2"/>
     <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.77734375" customWidth="1"/>
+    <col min="42" max="42" width="12.77734375" style="2" customWidth="1"/>
     <col min="44" max="44" width="12.44140625" customWidth="1"/>
     <col min="45" max="45" width="11.21875" customWidth="1"/>
     <col min="48" max="48" width="13.33203125" style="2" customWidth="1"/>
@@ -638,64 +638,64 @@
         <v>27</v>
       </c>
       <c r="AC1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>35</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>36</v>
       </c>
-      <c r="AT1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
@@ -800,9 +800,9 @@
         <f t="shared" ref="AF2:AF18" si="1">AB2-P2/2</f>
         <v>-2.8766988791062431E-9</v>
       </c>
-      <c r="AJ2" s="2" t="e">
+      <c r="AJ2" s="2">
         <f>(( 1.588*EXP(-0.0005387*0.5*232))^2-AP2^2)/(2*AP2)+0.4</f>
-        <v>#DIV/0!</v>
+        <v>0.56109386188935539</v>
       </c>
       <c r="AK2">
         <f t="shared" ref="AK2:AK18" si="2">(X2+Y2+Z2)/3</f>
@@ -812,17 +812,21 @@
         <f t="shared" ref="AL2:AL18" si="3">Z2-(Y2+X2)/2</f>
         <v>3423.5295013549999</v>
       </c>
-      <c r="AM2" s="3" t="e">
-        <f t="shared" ref="AM2:AM18" si="4">(-2*AJ2-3)/(-2*AJ2+6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AN2" t="e">
-        <f t="shared" ref="AN2:AN18" si="5">1/(2+AM2*AQ2-2*0.33*(1+AM2+AQ2))</f>
-        <v>#DIV/0!</v>
+      <c r="AM2" s="3">
+        <f>(-2*AI2-3)/(-2*AI2+6)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" ref="AN2:AN18" si="4">1/(2+AM2*AQ2-2*0.33*(1+AM2+AQ2))</f>
+        <v>0.5988023952095809</v>
       </c>
       <c r="AO2" s="1" t="e">
         <f>3*(1-2*0.33)*(AK2-AK1)/(AC2-AC1)</f>
         <v>#VALUE!</v>
+      </c>
+      <c r="AP2" s="2">
+        <f>AL2/AK2</f>
+        <v>1.3393829194319284</v>
       </c>
       <c r="AS2">
         <v>0</v>
@@ -922,15 +926,15 @@
         <v>0.42455699990888718</v>
       </c>
       <c r="AC3" s="2">
-        <f t="shared" ref="AC3:AC18" si="6">1.34 *((AK3/100000)^0.3-(2594/100000)^0.3)</f>
+        <f t="shared" ref="AC3:AC18" si="5">1.34 *((AK3/100000)^0.3-(2594/100000)^0.3)</f>
         <v>0.37815519616697812</v>
       </c>
       <c r="AD3" s="2">
-        <f t="shared" ref="AD3:AD18" si="7">AB3-AC3</f>
+        <f t="shared" ref="AD3:AD18" si="6">AB3-AC3</f>
         <v>4.6401803741909053E-2</v>
       </c>
       <c r="AE3" s="4">
-        <f t="shared" ref="AE3:AE18" si="8">P3-AB3/3</f>
+        <f t="shared" ref="AE3:AE18" si="7">P3-AB3/3</f>
         <v>0.86439544855037098</v>
       </c>
       <c r="AF3" s="2">
@@ -938,20 +942,20 @@
         <v>-7.8400224351112824E-2</v>
       </c>
       <c r="AG3" s="3">
-        <f t="shared" ref="AG3:AH18" si="9">AD3-AD2</f>
+        <f t="shared" ref="AG3:AH18" si="8">AD3-AD2</f>
         <v>4.4425304436998131E-2</v>
       </c>
       <c r="AH3" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.86439544759147136</v>
       </c>
       <c r="AI3" s="2">
-        <f t="shared" ref="AI3:AI18" si="10">-AG3/AH3</f>
+        <f t="shared" ref="AI3:AI18" si="9">-AG3/AH3</f>
         <v>-5.1394653408672643E-2</v>
       </c>
       <c r="AJ3" s="2">
-        <f t="shared" ref="AJ3:AJ18" si="11">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
-        <v>3.1368433750215918E-2</v>
+        <f t="shared" ref="AJ3:AJ18" si="10">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
+        <v>0.54583656219090648</v>
       </c>
       <c r="AK3" s="1">
         <f t="shared" si="2"/>
@@ -962,43 +966,43 @@
         <v>26990.528974650002</v>
       </c>
       <c r="AM3" s="3">
+        <f>(-2*AI3-3)/(-2*AI3+6)</f>
+        <v>-0.47473549348102495</v>
+      </c>
+      <c r="AN3" s="1">
         <f t="shared" si="4"/>
-        <v>-0.51584994620425884</v>
-      </c>
-      <c r="AN3" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.17746035224544451</v>
+        <v>-0.43893509681643</v>
       </c>
       <c r="AO3" s="1">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP3" s="1">
-        <f>(AK3*1.35*(AK3/3255000)^-0.0723-AK2*1.35*(AK2/3255000)^-0.0723)/(AK3-AK2)</f>
-        <v>1.9053060830494941</v>
+      <c r="AP3" s="2">
+        <f>AL3/AK3</f>
+        <v>1.3530789263599041</v>
       </c>
       <c r="AQ3" s="1">
         <f>(2*AP3+3)/(3-AP3)</f>
-        <v>6.221476214165274</v>
+        <v>3.464742751823445</v>
       </c>
       <c r="AR3" s="1">
         <f>(1+2*AM3)*(AK3-AK2)*(1-AP3/3)/(3*AN3*AO3*AM3)</f>
-        <v>-1.7954520719665367E-2</v>
+        <v>1.8915143640328775E-2</v>
       </c>
       <c r="AS3" s="1">
         <f>(AS2+AR3)</f>
-        <v>-1.7954520719665367E-2</v>
+        <v>1.8915143640328775E-2</v>
       </c>
       <c r="AT3" s="1">
         <f>2*(1-AM3)*(AK3-AK2)*(1-AP3/3)/(9*AN3*AO3*AM3)</f>
-        <v>0.57237542883510506</v>
+        <v>0.36803718647389322</v>
       </c>
       <c r="AU3" s="1">
         <f>AU2+AT3</f>
-        <v>0.57237542883510506</v>
+        <v>0.36803718647389322</v>
       </c>
       <c r="AV3" s="2">
-        <f t="shared" ref="AV3:AV18" si="12">(AQ3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
-        <v>61.573331518164267</v>
+        <f t="shared" ref="AV3:AV18" si="11">(AQ3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
+        <v>31.048885324486896</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
@@ -1088,15 +1092,15 @@
         <v>0.53723081921390747</v>
       </c>
       <c r="AC4" s="2">
+        <f t="shared" si="5"/>
+        <v>0.64894857499996228</v>
+      </c>
+      <c r="AD4" s="2">
         <f t="shared" si="6"/>
-        <v>0.64894857499996228</v>
-      </c>
-      <c r="AD4" s="2">
+        <v>-0.11171775578605481</v>
+      </c>
+      <c r="AE4" s="4">
         <f t="shared" si="7"/>
-        <v>-0.11171775578605481</v>
-      </c>
-      <c r="AE4" s="4">
-        <f t="shared" si="8"/>
         <v>1.8270880839220307</v>
       </c>
       <c r="AF4" s="2">
@@ -1104,20 +1108,20 @@
         <v>-0.46585169261609249</v>
       </c>
       <c r="AG4" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.15811955952796386</v>
+      </c>
+      <c r="AH4" s="3">
+        <f t="shared" si="8"/>
+        <v>0.96269263537165972</v>
+      </c>
+      <c r="AI4" s="2">
         <f t="shared" si="9"/>
-        <v>-0.15811955952796386</v>
-      </c>
-      <c r="AH4" s="3">
-        <f t="shared" si="9"/>
-        <v>0.96269263537165972</v>
-      </c>
-      <c r="AI4" s="2">
+        <v>0.16424718930868293</v>
+      </c>
+      <c r="AJ4" s="2">
         <f t="shared" si="10"/>
-        <v>0.16424718930868293</v>
-      </c>
-      <c r="AJ4" s="2">
-        <f t="shared" si="11"/>
-        <v>0.16912422089899823</v>
+        <v>0.47229178477375378</v>
       </c>
       <c r="AK4">
         <f t="shared" si="2"/>
@@ -1128,43 +1132,43 @@
         <v>72940.740784349997</v>
       </c>
       <c r="AM4" s="3">
+        <f t="shared" ref="AM4:AM18" si="12">(-2*AI4-3)/(-2*AI4+6)</f>
+        <v>-0.58688020445017652</v>
+      </c>
+      <c r="AN4">
         <f t="shared" si="4"/>
-        <v>-0.58961408099265322</v>
-      </c>
-      <c r="AN4">
-        <f t="shared" si="5"/>
-        <v>-0.21274075919304949</v>
+        <v>-0.34637286525300914</v>
       </c>
       <c r="AO4" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP4">
-        <f t="shared" ref="AP4:AP18" si="13">(AK4*1.35*(AK4/3255000)^-0.0723-AK3*1.35*(AK3/3255000)^-0.0723)/(AK4-AK3)</f>
-        <v>1.7404396115775711</v>
+      <c r="AP4" s="2">
+        <f t="shared" ref="AP4:AP18" si="13">AL4/AK4</f>
+        <v>1.421262848003912</v>
       </c>
       <c r="AQ4">
         <f t="shared" ref="AQ4:AQ18" si="14">(2*AP4+3)/(3-AP4)</f>
-        <v>5.1453501417842284</v>
+        <v>3.7007589823428071</v>
       </c>
       <c r="AR4" s="1">
         <f t="shared" ref="AR4:AR18" si="15">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
-        <v>-0.1537741601894102</v>
+        <v>-0.11530390241841393</v>
       </c>
       <c r="AS4">
         <f t="shared" ref="AS4:AS18" si="16">AS3+AR4</f>
-        <v>-0.17172868090907556</v>
+        <v>-9.6388758778085157E-2</v>
       </c>
       <c r="AT4" s="1">
         <f t="shared" ref="AT4:AT18" si="17">2*(1-AM4)*(AK4-AK3)*(1-AP4/3)/(9*AN4*AO4*AM4)</f>
-        <v>0.90923795167839838</v>
+        <v>0.70201446310118631</v>
       </c>
       <c r="AU4">
         <f>AU3+AT4</f>
-        <v>1.4816133805135034</v>
+        <v>1.0700516495750796</v>
       </c>
       <c r="AV4" s="2">
-        <f t="shared" si="12"/>
-        <v>123.63582364180566</v>
+        <f t="shared" si="11"/>
+        <v>83.878038367314915</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
@@ -1254,15 +1258,15 @@
         <v>0.57836850681094454</v>
       </c>
       <c r="AC5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.85304626901129565</v>
+      </c>
+      <c r="AD5" s="2">
         <f t="shared" si="6"/>
-        <v>0.85304626901129565</v>
-      </c>
-      <c r="AD5" s="2">
+        <v>-0.27467776220035112</v>
+      </c>
+      <c r="AE5" s="4">
         <f t="shared" si="7"/>
-        <v>-0.27467776220035112</v>
-      </c>
-      <c r="AE5" s="4">
-        <f t="shared" si="8"/>
         <v>2.8131835652496848</v>
       </c>
       <c r="AF5" s="2">
@@ -1270,20 +1274,20 @@
         <v>-0.92461802694905537</v>
       </c>
       <c r="AG5" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.16296000641429631</v>
+      </c>
+      <c r="AH5" s="3">
+        <f t="shared" si="8"/>
+        <v>0.98609548132765412</v>
+      </c>
+      <c r="AI5" s="2">
         <f t="shared" si="9"/>
-        <v>-0.16296000641429631</v>
-      </c>
-      <c r="AH5" s="3">
-        <f t="shared" si="9"/>
-        <v>0.98609548132765412</v>
-      </c>
-      <c r="AI5" s="2">
+        <v>0.16525783709594841</v>
+      </c>
+      <c r="AJ5" s="2">
         <f t="shared" si="10"/>
-        <v>0.16525783709594841</v>
-      </c>
-      <c r="AJ5" s="2">
-        <f t="shared" si="11"/>
-        <v>0.2465601787796606</v>
+        <v>0.44251031757577897</v>
       </c>
       <c r="AK5">
         <f t="shared" si="2"/>
@@ -1294,43 +1298,43 @@
         <v>131416.95121849998</v>
       </c>
       <c r="AM5" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.58744596206590272</v>
+      </c>
+      <c r="AN5">
         <f t="shared" si="4"/>
-        <v>-0.63431935767006364</v>
-      </c>
-      <c r="AN5">
-        <f t="shared" si="5"/>
-        <v>-0.23247936597521568</v>
+        <v>-0.33110852548566583</v>
       </c>
       <c r="AO5" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" s="2">
         <f t="shared" si="13"/>
-        <v>1.6531141584289157</v>
+        <v>1.4498992998035272</v>
       </c>
       <c r="AQ5">
         <f t="shared" si="14"/>
-        <v>4.6820807838486802</v>
+        <v>3.8060744046236894</v>
       </c>
       <c r="AR5" s="1">
         <f t="shared" si="15"/>
-        <v>-0.26272807087725686</v>
+        <v>-0.14924192667254385</v>
       </c>
       <c r="AS5">
         <f t="shared" si="16"/>
-        <v>-0.43445675178633242</v>
+        <v>-0.24563068545062899</v>
       </c>
       <c r="AT5" s="1">
         <f t="shared" si="17"/>
-        <v>1.065573817222305</v>
+        <v>0.90308531985623286</v>
       </c>
       <c r="AU5">
         <f>AU4+AT5</f>
-        <v>2.5471871977358083</v>
+        <v>1.9731369694313123</v>
       </c>
       <c r="AV5" s="2">
-        <f t="shared" si="12"/>
-        <v>193.61859757528433</v>
+        <f t="shared" si="11"/>
+        <v>151.60234099951631</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
@@ -1420,15 +1424,15 @@
         <v>0.35070042781746302</v>
       </c>
       <c r="AC6" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0207434038263898</v>
+      </c>
+      <c r="AD6" s="2">
         <f t="shared" si="6"/>
-        <v>1.0207434038263898</v>
-      </c>
-      <c r="AD6" s="2">
+        <v>-0.67004297600892682</v>
+      </c>
+      <c r="AE6" s="4">
         <f t="shared" si="7"/>
-        <v>-0.67004297600892682</v>
-      </c>
-      <c r="AE6" s="4">
-        <f t="shared" si="8"/>
         <v>3.8888826306841788</v>
       </c>
       <c r="AF6" s="2">
@@ -1436,20 +1440,20 @@
         <v>-1.652190958827537</v>
       </c>
       <c r="AG6" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.3953652138085757</v>
+      </c>
+      <c r="AH6" s="3">
+        <f t="shared" si="8"/>
+        <v>1.075699065434494</v>
+      </c>
+      <c r="AI6" s="2">
         <f t="shared" si="9"/>
-        <v>-0.3953652138085757</v>
-      </c>
-      <c r="AH6" s="3">
-        <f t="shared" si="9"/>
-        <v>1.075699065434494</v>
-      </c>
-      <c r="AI6" s="2">
+        <v>0.36754258371404336</v>
+      </c>
+      <c r="AJ6" s="2">
         <f t="shared" si="10"/>
-        <v>0.36754258371404336</v>
-      </c>
-      <c r="AJ6" s="2">
-        <f t="shared" si="11"/>
-        <v>0.29783972053186508</v>
+        <v>0.42224854292958564</v>
       </c>
       <c r="AK6">
         <f t="shared" si="2"/>
@@ -1460,43 +1464,43 @@
         <v>199552.3578074</v>
       </c>
       <c r="AM6" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.70942936138693358</v>
+      </c>
+      <c r="AN6">
         <f t="shared" si="4"/>
-        <v>-0.66533422691185917</v>
-      </c>
-      <c r="AN6">
-        <f t="shared" si="5"/>
-        <v>-0.24541223655052344</v>
+        <v>-0.28515064788020883</v>
       </c>
       <c r="AO6" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" s="2">
         <f t="shared" si="13"/>
-        <v>1.5974582636996595</v>
+        <v>1.4697214087143282</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="14"/>
-        <v>4.4169213414927846</v>
+        <v>3.8812820431857453</v>
       </c>
       <c r="AR6" s="1">
         <f t="shared" si="15"/>
-        <v>-0.34915420953330917</v>
+        <v>-0.38949272303242916</v>
       </c>
       <c r="AS6">
         <f t="shared" si="16"/>
-        <v>-0.78361096131964159</v>
+        <v>-0.63512340848305815</v>
       </c>
       <c r="AT6" s="1">
         <f t="shared" si="17"/>
-        <v>1.1722889375191792</v>
+        <v>1.059721350099295</v>
       </c>
       <c r="AU6">
         <f t="shared" ref="AU6:AU18" si="18">AU5+AT6</f>
-        <v>3.7194761352549874</v>
+        <v>3.0328583195306074</v>
       </c>
       <c r="AV6" s="2">
-        <f t="shared" si="12"/>
-        <v>268.73281207978994</v>
+        <f t="shared" si="11"/>
+        <v>230.65721129774403</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -1586,15 +1590,15 @@
         <v>0.19999993483033052</v>
       </c>
       <c r="AC7" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1561091253948397</v>
+      </c>
+      <c r="AD7" s="2">
         <f t="shared" si="6"/>
-        <v>1.1561091253948397</v>
-      </c>
-      <c r="AD7" s="2">
+        <v>-0.95610919056450916</v>
+      </c>
+      <c r="AE7" s="4">
         <f t="shared" si="7"/>
-        <v>-0.95610919056450916</v>
-      </c>
-      <c r="AE7" s="4">
-        <f t="shared" si="8"/>
         <v>4.9384663104565565</v>
       </c>
       <c r="AF7" s="2">
@@ -1602,20 +1606,20 @@
         <v>-2.3025665428696693</v>
       </c>
       <c r="AG7" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.28606621455558234</v>
+      </c>
+      <c r="AH7" s="3">
+        <f t="shared" si="8"/>
+        <v>1.0495836797723777</v>
+      </c>
+      <c r="AI7" s="2">
         <f t="shared" si="9"/>
-        <v>-0.28606621455558234</v>
-      </c>
-      <c r="AH7" s="3">
-        <f t="shared" si="9"/>
-        <v>1.0495836797723777</v>
-      </c>
-      <c r="AI7" s="2">
+        <v>0.27255207952320798</v>
+      </c>
+      <c r="AJ7" s="2">
         <f t="shared" si="10"/>
-        <v>0.27255207952320798</v>
-      </c>
-      <c r="AJ7" s="2">
-        <f t="shared" si="11"/>
-        <v>0.33487633629698077</v>
+        <v>0.40967713528617822</v>
       </c>
       <c r="AK7">
         <f t="shared" si="2"/>
@@ -1626,43 +1630,43 @@
         <v>269986.16568114999</v>
       </c>
       <c r="AM7" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.64989401491975829</v>
+      </c>
+      <c r="AN7">
         <f t="shared" si="4"/>
-        <v>-0.68847699687883801</v>
-      </c>
-      <c r="AN7">
-        <f t="shared" si="5"/>
-        <v>-0.25464876034754208</v>
+        <v>-0.29601020053209681</v>
       </c>
       <c r="AO7" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" s="2">
         <f t="shared" si="13"/>
-        <v>1.5583485062903495</v>
+        <v>1.4821583066755686</v>
       </c>
       <c r="AQ7">
         <f t="shared" si="14"/>
-        <v>4.2428402698361198</v>
+        <v>3.9294721179307417</v>
       </c>
       <c r="AR7" s="1">
         <f t="shared" si="15"/>
-        <v>-0.39154149141951317</v>
+        <v>-0.29878012725482339</v>
       </c>
       <c r="AS7">
         <f t="shared" si="16"/>
-        <v>-1.1751524527391548</v>
+        <v>-0.93390353573788154</v>
       </c>
       <c r="AT7" s="1">
         <f t="shared" si="17"/>
-        <v>1.1692121806787794</v>
+        <v>1.096231324954474</v>
       </c>
       <c r="AU7">
         <f t="shared" si="18"/>
-        <v>4.8886883159337664</v>
+        <v>4.1290896444850809</v>
       </c>
       <c r="AV7" s="2">
-        <f t="shared" si="12"/>
-        <v>341.68565419548128</v>
+        <f t="shared" si="11"/>
+        <v>312.06306622211565</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
@@ -1752,15 +1756,15 @@
         <v>-0.10677972586135009</v>
       </c>
       <c r="AC8" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2739837410670807</v>
+      </c>
+      <c r="AD8" s="2">
         <f t="shared" si="6"/>
-        <v>1.2739837410670807</v>
-      </c>
-      <c r="AD8" s="2">
+        <v>-1.3807634669284308</v>
+      </c>
+      <c r="AE8" s="4">
         <f t="shared" si="7"/>
-        <v>-1.3807634669284308</v>
-      </c>
-      <c r="AE8" s="4">
-        <f t="shared" si="8"/>
         <v>6.0396844916037837</v>
       </c>
       <c r="AF8" s="2">
@@ -1768,20 +1772,20 @@
         <v>-3.1088253506863501</v>
       </c>
       <c r="AG8" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.42465427636392161</v>
+      </c>
+      <c r="AH8" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1012181811472272</v>
+      </c>
+      <c r="AI8" s="2">
         <f t="shared" si="9"/>
-        <v>-0.42465427636392161</v>
-      </c>
-      <c r="AH8" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1012181811472272</v>
-      </c>
-      <c r="AI8" s="2">
+        <v>0.38562228960070855</v>
+      </c>
+      <c r="AJ8" s="2">
         <f t="shared" si="10"/>
-        <v>0.38562228960070855</v>
-      </c>
-      <c r="AJ8" s="2">
-        <f t="shared" si="11"/>
-        <v>0.36322412530515052</v>
+        <v>0.40457569788824999</v>
       </c>
       <c r="AK8">
         <f t="shared" si="2"/>
@@ -1792,43 +1796,43 @@
         <v>343143.63679850003</v>
       </c>
       <c r="AM8" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.7212509049859972</v>
+      </c>
+      <c r="AN8">
         <f t="shared" si="4"/>
-        <v>-0.70662969241584817</v>
-      </c>
-      <c r="AN8">
-        <f t="shared" si="5"/>
-        <v>-0.2616440755961088</v>
+        <v>-0.27479710670582819</v>
       </c>
       <c r="AO8" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP8">
+      <c r="AP8" s="2">
         <f t="shared" si="13"/>
-        <v>1.5290331594502045</v>
+        <v>1.4872353745860825</v>
       </c>
       <c r="AQ8">
         <f t="shared" si="14"/>
-        <v>4.1184248019051992</v>
+        <v>3.9493723271969357</v>
       </c>
       <c r="AR8" s="1">
         <f t="shared" si="15"/>
-        <v>-0.43489971954479406</v>
+        <v>-0.4467393344404133</v>
       </c>
       <c r="AS8">
         <f t="shared" si="16"/>
-        <v>-1.6100521722839489</v>
+        <v>-1.3806428701782949</v>
       </c>
       <c r="AT8" s="1">
         <f t="shared" si="17"/>
-        <v>1.1973315901839605</v>
+        <v>1.1584893987922444</v>
       </c>
       <c r="AU8">
         <f t="shared" si="18"/>
-        <v>6.0860199061177269</v>
+        <v>5.2875790432773258</v>
       </c>
       <c r="AV8" s="2">
-        <f t="shared" si="12"/>
-        <v>416.42950066425135</v>
+        <f t="shared" si="11"/>
+        <v>396.30829648304172</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
@@ -1918,15 +1922,15 @@
         <v>-0.34012835873640235</v>
       </c>
       <c r="AC9" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3767389866898236</v>
+      </c>
+      <c r="AD9" s="2">
         <f t="shared" si="6"/>
-        <v>1.3767389866898236</v>
-      </c>
-      <c r="AD9" s="2">
+        <v>-1.716867345426226</v>
+      </c>
+      <c r="AE9" s="4">
         <f t="shared" si="7"/>
-        <v>-1.716867345426226</v>
-      </c>
-      <c r="AE9" s="4">
-        <f t="shared" si="8"/>
         <v>7.1192576157988006</v>
       </c>
       <c r="AF9" s="2">
@@ -1934,20 +1938,20 @@
         <v>-3.8430691068464022</v>
       </c>
       <c r="AG9" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.33610387849779522</v>
+      </c>
+      <c r="AH9" s="3">
+        <f t="shared" si="8"/>
+        <v>1.0795731241950168</v>
+      </c>
+      <c r="AI9" s="2">
         <f t="shared" si="9"/>
-        <v>-0.33610387849779522</v>
-      </c>
-      <c r="AH9" s="3">
-        <f t="shared" si="9"/>
-        <v>1.0795731241950168</v>
-      </c>
-      <c r="AI9" s="2">
+        <v>0.31133034989955954</v>
+      </c>
+      <c r="AJ9" s="2">
         <f t="shared" si="10"/>
-        <v>0.31133034989955954</v>
-      </c>
-      <c r="AJ9" s="2">
-        <f t="shared" si="11"/>
-        <v>0.38623271525634967</v>
+        <v>0.40424344843035476</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
@@ -1958,43 +1962,43 @@
         <v>416368.13751550001</v>
       </c>
       <c r="AM9" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.673690183482338</v>
+      </c>
+      <c r="AN9">
         <f t="shared" si="4"/>
-        <v>-0.72165289016590672</v>
-      </c>
-      <c r="AN9">
-        <f t="shared" si="5"/>
-        <v>-0.2672667846072983</v>
+        <v>-0.28699827519653104</v>
       </c>
       <c r="AO9" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" s="2">
         <f t="shared" si="13"/>
-        <v>1.5056348650184768</v>
+        <v>1.4875666419633369</v>
       </c>
       <c r="AQ9">
         <f t="shared" si="14"/>
-        <v>4.0226244505572453</v>
+        <v>3.950675414672935</v>
       </c>
       <c r="AR9" s="1">
         <f t="shared" si="15"/>
-        <v>-0.45996597226871672</v>
+        <v>-0.36389906440701658</v>
       </c>
       <c r="AS9">
         <f t="shared" si="16"/>
-        <v>-2.0700181445526655</v>
+        <v>-1.7445419345853115</v>
       </c>
       <c r="AT9" s="1">
         <f t="shared" si="17"/>
-        <v>1.1909037067546928</v>
+        <v>1.16885187879825</v>
       </c>
       <c r="AU9">
         <f t="shared" si="18"/>
-        <v>7.2769236128724195</v>
+        <v>6.456430922075576</v>
       </c>
       <c r="AV9" s="2">
-        <f t="shared" si="12"/>
-        <v>490.76000851941723</v>
+        <f t="shared" si="11"/>
+        <v>480.40795615833036</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
@@ -2084,15 +2088,15 @@
         <v>-0.69687079219256098</v>
       </c>
       <c r="AC10" s="2">
+        <f t="shared" si="5"/>
+        <v>1.467011534629955</v>
+      </c>
+      <c r="AD10" s="2">
         <f t="shared" si="6"/>
-        <v>1.467011534629955</v>
-      </c>
-      <c r="AD10" s="2">
+        <v>-2.1638823268225158</v>
+      </c>
+      <c r="AE10" s="4">
         <f t="shared" si="7"/>
-        <v>-2.1638823268225158</v>
-      </c>
-      <c r="AE10" s="4">
-        <f t="shared" si="8"/>
         <v>8.2334755863341869</v>
       </c>
       <c r="AF10" s="2">
@@ -2100,20 +2104,20 @@
         <v>-4.6974634533275612</v>
       </c>
       <c r="AG10" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.44701498139628981</v>
+      </c>
+      <c r="AH10" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1142179705353863</v>
+      </c>
+      <c r="AI10" s="2">
         <f t="shared" si="9"/>
-        <v>-0.44701498139628981</v>
-      </c>
-      <c r="AH10" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1142179705353863</v>
-      </c>
-      <c r="AI10" s="2">
+        <v>0.40119168171511116</v>
+      </c>
+      <c r="AJ10" s="2">
         <f t="shared" si="10"/>
-        <v>0.40119168171511116</v>
-      </c>
-      <c r="AJ10" s="2">
-        <f t="shared" si="11"/>
-        <v>0.40523305542392607</v>
+        <v>0.40507075527034625</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
@@ -2124,43 +2128,43 @@
         <v>488807.77019649994</v>
       </c>
       <c r="AM10" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.73156287377509355</v>
+      </c>
+      <c r="AN10">
         <f t="shared" si="4"/>
-        <v>-0.73425979909544348</v>
-      </c>
-      <c r="AN10">
-        <f t="shared" si="5"/>
-        <v>-0.27186852623002888</v>
+        <v>-0.27245961270850599</v>
       </c>
       <c r="AO10" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP10">
+      <c r="AP10" s="2">
         <f t="shared" si="13"/>
-        <v>1.4865801781327825</v>
+        <v>1.4867419177904724</v>
       </c>
       <c r="AQ10">
         <f t="shared" si="14"/>
-        <v>3.946796698417784</v>
+        <v>3.9474323023994584</v>
       </c>
       <c r="AR10" s="1">
         <f t="shared" si="15"/>
-        <v>-0.47283910294282233</v>
+        <v>-0.46805083579045414</v>
       </c>
       <c r="AS10">
         <f t="shared" si="16"/>
-        <v>-2.5428572474954878</v>
+        <v>-2.2125927703757657</v>
       </c>
       <c r="AT10" s="1">
         <f t="shared" si="17"/>
-        <v>1.1668325093770344</v>
+        <v>1.1666513966329444</v>
       </c>
       <c r="AU10">
         <f t="shared" si="18"/>
-        <v>8.4437561222494537</v>
+        <v>7.6230823187085202</v>
       </c>
       <c r="AV10" s="2">
-        <f t="shared" si="12"/>
-        <v>564.22397859727892</v>
+        <f t="shared" si="11"/>
+        <v>564.33125013541826</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2250,15 +2254,15 @@
         <v>-1.0567213372539408</v>
       </c>
       <c r="AC11" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5443363891529516</v>
+      </c>
+      <c r="AD11" s="2">
         <f t="shared" si="6"/>
-        <v>1.5443363891529516</v>
-      </c>
-      <c r="AD11" s="2">
+        <v>-2.6010577264068924</v>
+      </c>
+      <c r="AE11" s="4">
         <f t="shared" si="7"/>
-        <v>-2.6010577264068924</v>
-      </c>
-      <c r="AE11" s="4">
-        <f t="shared" si="8"/>
         <v>9.3529214808213137</v>
       </c>
       <c r="AF11" s="2">
@@ -2266,20 +2270,20 @@
         <v>-5.557061854788941</v>
       </c>
       <c r="AG11" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.43717539958437657</v>
+      </c>
+      <c r="AH11" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1194458944871268</v>
+      </c>
+      <c r="AI11" s="2">
         <f t="shared" si="9"/>
-        <v>-0.43717539958437657</v>
-      </c>
-      <c r="AH11" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1194458944871268</v>
-      </c>
-      <c r="AI11" s="2">
+        <v>0.39052838706837911</v>
+      </c>
+      <c r="AJ11" s="2">
         <f t="shared" si="10"/>
-        <v>0.39052838706837911</v>
-      </c>
-      <c r="AJ11" s="2">
-        <f t="shared" si="11"/>
-        <v>0.42095593773000084</v>
+        <v>0.41190691709578892</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
@@ -2290,43 +2294,43 @@
         <v>555202.86013150006</v>
       </c>
       <c r="AM11" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.72448704852721413</v>
+      </c>
+      <c r="AN11">
         <f t="shared" si="4"/>
-        <v>-0.74483253924682147</v>
-      </c>
-      <c r="AN11">
-        <f t="shared" si="5"/>
-        <v>-0.27564569709270981</v>
+        <v>-0.2769939879259114</v>
       </c>
       <c r="AO11" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP11">
+      <c r="AP11" s="2">
         <f t="shared" si="13"/>
-        <v>1.470995298159429</v>
+        <v>1.4799446551527975</v>
       </c>
       <c r="AQ11">
         <f t="shared" si="14"/>
-        <v>3.8861820301573067</v>
+        <v>3.9208370474857208</v>
       </c>
       <c r="AR11" s="1">
         <f t="shared" si="15"/>
-        <v>-0.46055165618769789</v>
+        <v>-0.42949683827302865</v>
       </c>
       <c r="AS11">
         <f t="shared" si="16"/>
-        <v>-3.0034089036831855</v>
+        <v>-2.6420896086487944</v>
       </c>
       <c r="AT11" s="1">
         <f t="shared" si="17"/>
-        <v>1.0940614323466165</v>
+        <v>1.0997839145501775</v>
       </c>
       <c r="AU11">
         <f t="shared" si="18"/>
-        <v>9.5378175545960708</v>
+        <v>8.7228662332586975</v>
       </c>
       <c r="AV11" s="2">
-        <f t="shared" si="12"/>
-        <v>635.17882804811688</v>
+        <f t="shared" si="11"/>
+        <v>641.86882088350251</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
@@ -2416,15 +2420,15 @@
         <v>-1.3573824484509611</v>
       </c>
       <c r="AC12" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6086676769888566</v>
+      </c>
+      <c r="AD12" s="2">
         <f t="shared" si="6"/>
-        <v>1.6086676769888566</v>
-      </c>
-      <c r="AD12" s="2">
+        <v>-2.9660501254398177</v>
+      </c>
+      <c r="AE12" s="4">
         <f t="shared" si="7"/>
-        <v>-2.9660501254398177</v>
-      </c>
-      <c r="AE12" s="4">
-        <f t="shared" si="8"/>
         <v>10.457959603650322</v>
       </c>
       <c r="AF12" s="2">
@@ -2432,20 +2436,20 @@
         <v>-6.3601318422009614</v>
       </c>
       <c r="AG12" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.36499239903292535</v>
+      </c>
+      <c r="AH12" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1050381228290078</v>
+      </c>
+      <c r="AI12" s="2">
         <f t="shared" si="9"/>
-        <v>-0.36499239903292535</v>
-      </c>
-      <c r="AH12" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1050381228290078</v>
-      </c>
-      <c r="AI12" s="2">
+        <v>0.330298467982723</v>
+      </c>
+      <c r="AJ12" s="2">
         <f t="shared" si="10"/>
-        <v>0.330298467982723</v>
-      </c>
-      <c r="AJ12" s="2">
-        <f t="shared" si="11"/>
-        <v>0.4337328660539343</v>
+        <v>0.42536557513271239</v>
       </c>
       <c r="AK12">
         <f t="shared" si="2"/>
@@ -2456,43 +2460,43 @@
         <v>611699.82950849994</v>
       </c>
       <c r="AM12" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.68558168245860607</v>
+      </c>
+      <c r="AN12">
         <f t="shared" si="4"/>
-        <v>-0.75351970980530625</v>
-      </c>
-      <c r="AN12">
-        <f t="shared" si="5"/>
-        <v>-0.27869324964626974</v>
+        <v>-0.29288859123013355</v>
       </c>
       <c r="AO12" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP12">
+      <c r="AP12" s="2">
         <f t="shared" si="13"/>
-        <v>1.4584525263146098</v>
+        <v>1.4666541135268127</v>
       </c>
       <c r="AQ12">
         <f t="shared" si="14"/>
-        <v>3.8382892214688829</v>
+        <v>3.869517164650103</v>
       </c>
       <c r="AR12" s="1">
         <f t="shared" si="15"/>
-        <v>-0.42492952929842154</v>
+        <v>-0.32358093460233733</v>
       </c>
       <c r="AS12">
         <f t="shared" si="16"/>
-        <v>-3.4283384329816071</v>
+        <v>-2.9656705432511319</v>
       </c>
       <c r="AT12" s="1">
         <f t="shared" si="17"/>
-        <v>0.97970332099661983</v>
+        <v>0.97966223270300812</v>
       </c>
       <c r="AU12">
         <f t="shared" si="18"/>
-        <v>10.517520875592691</v>
+        <v>9.7025284659617057</v>
       </c>
       <c r="AV12" s="2">
-        <f t="shared" si="12"/>
-        <v>701.86092936402974</v>
+        <f t="shared" si="11"/>
+        <v>708.60531781783538</v>
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
@@ -2582,15 +2586,15 @@
         <v>-2.0595318912459915</v>
       </c>
       <c r="AC13" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6363649598467622</v>
+      </c>
+      <c r="AD13" s="2">
         <f t="shared" si="6"/>
-        <v>1.6363649598467622</v>
-      </c>
-      <c r="AD13" s="2">
+        <v>-3.6958968510927539</v>
+      </c>
+      <c r="AE13" s="4">
         <f t="shared" si="7"/>
-        <v>-3.6958968510927539</v>
-      </c>
-      <c r="AE13" s="4">
-        <f t="shared" si="8"/>
         <v>11.68986396061533</v>
       </c>
       <c r="AF13" s="2">
@@ -2598,20 +2602,20 @@
         <v>-7.5612085563459912</v>
       </c>
       <c r="AG13" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.72984672565293618</v>
+      </c>
+      <c r="AH13" s="3">
+        <f t="shared" si="8"/>
+        <v>1.2319043569650088</v>
+      </c>
+      <c r="AI13" s="2">
         <f t="shared" si="9"/>
-        <v>-0.72984672565293618</v>
-      </c>
-      <c r="AH13" s="3">
-        <f t="shared" si="9"/>
-        <v>1.2319043569650088</v>
-      </c>
-      <c r="AI13" s="2">
+        <v>0.59245405012693442</v>
+      </c>
+      <c r="AJ13" s="2">
         <f t="shared" si="10"/>
-        <v>0.59245405012693442</v>
-      </c>
-      <c r="AJ13" s="2">
-        <f t="shared" si="11"/>
-        <v>0.44177279741358977</v>
+        <v>0.45511912099003649</v>
       </c>
       <c r="AK13">
         <f t="shared" si="2"/>
@@ -2622,43 +2626,43 @@
         <v>626967.5865185</v>
       </c>
       <c r="AM13" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.8691232041644964</v>
+      </c>
+      <c r="AN13">
         <f t="shared" si="4"/>
-        <v>-0.75903062693197265</v>
-      </c>
-      <c r="AN13">
-        <f t="shared" si="5"/>
-        <v>-0.28060038175465879</v>
+        <v>-0.26061853912273791</v>
       </c>
       <c r="AO13" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" s="2">
         <f t="shared" si="13"/>
-        <v>1.4506159942722798</v>
+        <v>1.4377028564890491</v>
       </c>
       <c r="AQ13">
         <f t="shared" si="14"/>
-        <v>3.8087601051314892</v>
+        <v>3.7607479072606491</v>
       </c>
       <c r="AR13" s="1">
         <f t="shared" si="15"/>
-        <v>-0.19519751473798011</v>
+        <v>-0.26373027711361469</v>
       </c>
       <c r="AS13">
         <f t="shared" si="16"/>
-        <v>-3.6235359477195872</v>
+        <v>-3.2294008203647464</v>
       </c>
       <c r="AT13" s="1">
         <f t="shared" si="17"/>
-        <v>0.44185046223032903</v>
+        <v>0.44514891417673641</v>
       </c>
       <c r="AU13">
         <f t="shared" si="18"/>
-        <v>10.95937133782302</v>
+        <v>10.147677380138441</v>
       </c>
       <c r="AV13" s="2">
-        <f t="shared" si="12"/>
-        <v>737.06366727525415</v>
+        <f t="shared" si="11"/>
+        <v>726.10196678091063</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
@@ -2748,15 +2752,15 @@
         <v>-3.1772879905688667</v>
       </c>
       <c r="AC14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6399324512181561</v>
+      </c>
+      <c r="AD14" s="2">
         <f t="shared" si="6"/>
-        <v>1.6399324512181561</v>
-      </c>
-      <c r="AD14" s="2">
+        <v>-4.8172204417870228</v>
+      </c>
+      <c r="AE14" s="4">
         <f t="shared" si="7"/>
-        <v>-4.8172204417870228</v>
-      </c>
-      <c r="AE14" s="4">
-        <f t="shared" si="8"/>
         <v>13.062964914256289</v>
       </c>
       <c r="AF14" s="2">
@@ -2764,20 +2768,20 @@
         <v>-9.1792224492688668</v>
       </c>
       <c r="AG14" s="3">
+        <f t="shared" si="8"/>
+        <v>-1.1213235906942689</v>
+      </c>
+      <c r="AH14" s="3">
+        <f t="shared" si="8"/>
+        <v>1.3731009536409591</v>
+      </c>
+      <c r="AI14" s="2">
         <f t="shared" si="9"/>
-        <v>-1.1213235906942689</v>
-      </c>
-      <c r="AH14" s="3">
-        <f t="shared" si="9"/>
-        <v>1.3731009536409591</v>
-      </c>
-      <c r="AI14" s="2">
+        <v>0.81663594196838252</v>
+      </c>
+      <c r="AJ14" s="2">
         <f t="shared" si="10"/>
-        <v>0.81663594196838252</v>
-      </c>
-      <c r="AJ14" s="2">
-        <f t="shared" si="11"/>
-        <v>0.44446908167319388</v>
+        <v>0.49536469757931656</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
@@ -2788,43 +2792,43 @@
         <v>613789.68986549997</v>
       </c>
       <c r="AM14" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.0610396985544017</v>
+      </c>
+      <c r="AN14">
         <f t="shared" si="4"/>
-        <v>-0.76088654131655131</v>
-      </c>
-      <c r="AN14">
-        <f t="shared" si="5"/>
-        <v>-0.28123808099769321</v>
+        <v>-0.23835834391504512</v>
       </c>
       <c r="AO14" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" s="2">
         <f t="shared" si="13"/>
-        <v>1.4479976141598188</v>
+        <v>1.3994843799165515</v>
       </c>
       <c r="AQ14">
         <f t="shared" si="14"/>
-        <v>3.7989601576081489</v>
+        <v>3.623187857129913</v>
       </c>
       <c r="AR14" s="1">
         <f t="shared" si="15"/>
-        <v>-2.5692097122298814E-2</v>
+        <v>-4.8210433931383655E-2</v>
       </c>
       <c r="AS14">
         <f t="shared" si="16"/>
-        <v>-3.6492280448418861</v>
+        <v>-3.2776112542961302</v>
       </c>
       <c r="AT14" s="1">
         <f t="shared" si="17"/>
-        <v>5.7804014231049541E-2</v>
+        <v>5.9035405440494577E-2</v>
       </c>
       <c r="AU14">
         <f t="shared" si="18"/>
-        <v>11.017175352054069</v>
+        <v>10.206712785578937</v>
       </c>
       <c r="AV14" s="2">
-        <f t="shared" si="12"/>
-        <v>753.96217613891213</v>
+        <f t="shared" si="11"/>
+        <v>712.89688778342315</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
@@ -2914,15 +2918,15 @@
         <v>-5.3026998397139868</v>
       </c>
       <c r="AC15" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6078256260480841</v>
+      </c>
+      <c r="AD15" s="2">
         <f t="shared" si="6"/>
-        <v>1.6078256260480841</v>
-      </c>
-      <c r="AD15" s="2">
+        <v>-6.9105254657620705</v>
+      </c>
+      <c r="AE15" s="4">
         <f t="shared" si="7"/>
-        <v>-6.9105254657620705</v>
-      </c>
-      <c r="AE15" s="4">
-        <f t="shared" si="8"/>
         <v>14.772471457237996</v>
       </c>
       <c r="AF15" s="2">
@@ -2930,20 +2934,20 @@
         <v>-11.805152261713987</v>
       </c>
       <c r="AG15" s="3">
+        <f t="shared" si="8"/>
+        <v>-2.0933050239750477</v>
+      </c>
+      <c r="AH15" s="3">
+        <f t="shared" si="8"/>
+        <v>1.7095065429817069</v>
+      </c>
+      <c r="AI15" s="2">
         <f t="shared" si="9"/>
-        <v>-2.0933050239750477</v>
-      </c>
-      <c r="AH15" s="3">
-        <f t="shared" si="9"/>
-        <v>1.7095065429817069</v>
-      </c>
-      <c r="AI15" s="2">
+        <v>1.2245083428133143</v>
+      </c>
+      <c r="AJ15" s="2">
         <f t="shared" si="10"/>
-        <v>1.2245083428133143</v>
-      </c>
-      <c r="AJ15" s="2">
-        <f t="shared" si="11"/>
-        <v>0.44201257516055953</v>
+        <v>0.56076249307108816</v>
       </c>
       <c r="AK15">
         <f t="shared" si="2"/>
@@ -2954,43 +2958,43 @@
         <v>557979.83421200002</v>
       </c>
       <c r="AM15" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.5345092339833188</v>
+      </c>
+      <c r="AN15">
         <f t="shared" si="4"/>
-        <v>-0.75919551296561028</v>
-      </c>
-      <c r="AN15">
-        <f t="shared" si="5"/>
-        <v>-0.28065713032120482</v>
+        <v>-0.19402989565662734</v>
       </c>
       <c r="AO15" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP15">
+      <c r="AP15" s="2">
         <f t="shared" si="13"/>
-        <v>1.4503829472856433</v>
+        <v>1.3396787480724246</v>
       </c>
       <c r="AQ15">
         <f t="shared" si="14"/>
-        <v>3.807886525406599</v>
+        <v>3.4206377166776081</v>
       </c>
       <c r="AR15" s="1">
         <f t="shared" si="15"/>
-        <v>0.22670660316641431</v>
+        <v>0.69379371110170596</v>
       </c>
       <c r="AS15">
         <f t="shared" si="16"/>
-        <v>-3.4225214416754719</v>
+        <v>-2.5838175431944244</v>
       </c>
       <c r="AT15" s="1">
         <f t="shared" si="17"/>
-        <v>-0.51289627469097221</v>
+        <v>-0.56658961547596431</v>
       </c>
       <c r="AU15">
         <f t="shared" si="18"/>
-        <v>10.504279077363098</v>
+        <v>9.6401231701029726</v>
       </c>
       <c r="AV15" s="2">
-        <f t="shared" si="12"/>
-        <v>735.40119360157871</v>
+        <f t="shared" si="11"/>
+        <v>647.67332194384869</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -3080,15 +3084,15 @@
         <v>-6.403433079926435</v>
       </c>
       <c r="AC16" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5546984421060532</v>
+      </c>
+      <c r="AD16" s="2">
         <f t="shared" si="6"/>
-        <v>1.5546984421060532</v>
-      </c>
-      <c r="AD16" s="2">
+        <v>-7.9581315220324882</v>
+      </c>
+      <c r="AE16" s="4">
         <f t="shared" si="7"/>
-        <v>-7.9581315220324882</v>
-      </c>
-      <c r="AE16" s="4">
-        <f t="shared" si="8"/>
         <v>16.13500808720881</v>
       </c>
       <c r="AF16" s="2">
@@ -3096,20 +3100,20 @@
         <v>-13.403698276876435</v>
       </c>
       <c r="AG16" s="3">
+        <f t="shared" si="8"/>
+        <v>-1.0476060562704177</v>
+      </c>
+      <c r="AH16" s="3">
+        <f t="shared" si="8"/>
+        <v>1.3625366299708137</v>
+      </c>
+      <c r="AI16" s="2">
         <f t="shared" si="9"/>
-        <v>-1.0476060562704177</v>
-      </c>
-      <c r="AH16" s="3">
-        <f t="shared" si="9"/>
-        <v>1.3625366299708137</v>
-      </c>
-      <c r="AI16" s="2">
+        <v>0.76886450846672505</v>
+      </c>
+      <c r="AJ16" s="2">
         <f t="shared" si="10"/>
-        <v>0.76886450846672505</v>
-      </c>
-      <c r="AJ16" s="2">
-        <f t="shared" si="11"/>
-        <v>0.43456075696068175</v>
+        <v>0.65041534995876793</v>
       </c>
       <c r="AK16">
         <f t="shared" si="2"/>
@@ -3120,43 +3124,43 @@
         <v>481797.63894000003</v>
       </c>
       <c r="AM16" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.0169102311700138</v>
+      </c>
+      <c r="AN16">
         <f t="shared" si="4"/>
-        <v>-0.75408558678972093</v>
-      </c>
-      <c r="AN16">
-        <f t="shared" si="5"/>
-        <v>-0.27889001452943801</v>
+        <v>-0.30120721151377106</v>
       </c>
       <c r="AO16" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP16">
+      <c r="AP16" s="2">
         <f t="shared" si="13"/>
-        <v>1.4576435805439203</v>
+        <v>1.2622601560374207</v>
       </c>
       <c r="AQ16">
         <f t="shared" si="14"/>
-        <v>3.8352271151267998</v>
+        <v>3.179141188060258</v>
       </c>
       <c r="AR16" s="1">
         <f t="shared" si="15"/>
-        <v>0.35329426396972924</v>
+        <v>0.5560032378663774</v>
       </c>
       <c r="AS16">
         <f t="shared" si="16"/>
-        <v>-3.0692271777057427</v>
+        <v>-2.0278143053280471</v>
       </c>
       <c r="AT16" s="1">
         <f t="shared" si="17"/>
-        <v>-0.81299164342558139</v>
+        <v>-0.72314852843859712</v>
       </c>
       <c r="AU16">
         <f t="shared" si="18"/>
-        <v>9.6912874339375161</v>
+        <v>8.9169746416643747</v>
       </c>
       <c r="AV16" s="2">
-        <f t="shared" si="12"/>
-        <v>708.58070636773732</v>
+        <f t="shared" si="11"/>
+        <v>566.88055710714389</v>
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.25">
@@ -3246,15 +3250,15 @@
         <v>-6.8663253380735645</v>
       </c>
       <c r="AC17" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5649448192025073</v>
+      </c>
+      <c r="AD17" s="2">
         <f t="shared" si="6"/>
-        <v>1.5649448192025073</v>
-      </c>
-      <c r="AD17" s="2">
+        <v>-8.4312701572760709</v>
+      </c>
+      <c r="AE17" s="4">
         <f t="shared" si="7"/>
-        <v>-8.4312701572760709</v>
-      </c>
-      <c r="AE17" s="4">
-        <f t="shared" si="8"/>
         <v>17.289686448891189</v>
       </c>
       <c r="AF17" s="2">
@@ -3262,20 +3266,20 @@
         <v>-14.366781006173564</v>
       </c>
       <c r="AG17" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.47313863524358268</v>
+      </c>
+      <c r="AH17" s="3">
+        <f t="shared" si="8"/>
+        <v>1.1546783616823788</v>
+      </c>
+      <c r="AI17" s="2">
         <f t="shared" si="9"/>
-        <v>-0.47313863524358268</v>
-      </c>
-      <c r="AH17" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1546783616823788</v>
-      </c>
-      <c r="AI17" s="2">
+        <v>0.40975794727305237</v>
+      </c>
+      <c r="AJ17" s="2">
         <f t="shared" si="10"/>
-        <v>0.40975794727305237</v>
-      </c>
-      <c r="AJ17" s="2">
-        <f t="shared" si="11"/>
-        <v>0.43070722447720716</v>
+        <v>0.65527386653846997</v>
       </c>
       <c r="AK17">
         <f t="shared" si="2"/>
@@ -3286,43 +3290,43 @@
         <v>488492.35904600006</v>
       </c>
       <c r="AM17" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.73728937620424428</v>
+      </c>
+      <c r="AN17">
         <f t="shared" si="4"/>
-        <v>-0.75145473605449731</v>
-      </c>
-      <c r="AN17">
-        <f t="shared" si="5"/>
-        <v>-0.27797340777508867</v>
+        <v>-0.38479944977878094</v>
       </c>
       <c r="AO17" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP17">
+      <c r="AP17" s="2">
         <f t="shared" si="13"/>
-        <v>1.461412835230103</v>
+        <v>1.2582135255079103</v>
       </c>
       <c r="AQ17">
         <f t="shared" si="14"/>
-        <v>3.8495223449663918</v>
+        <v>3.1671086736532548</v>
       </c>
       <c r="AR17" s="1">
         <f t="shared" si="15"/>
-        <v>-6.606236409583767E-2</v>
+        <v>-5.1961185798771473E-2</v>
       </c>
       <c r="AS17">
         <f t="shared" si="16"/>
-        <v>-3.1352895418015803</v>
+        <v>-2.0797754911268185</v>
       </c>
       <c r="AT17" s="1">
         <f t="shared" si="17"/>
-        <v>0.15338113767658354</v>
+        <v>0.12680946433028142</v>
       </c>
       <c r="AU17">
         <f t="shared" si="18"/>
-        <v>9.8446685716141005</v>
+        <v>9.0437841059946553</v>
       </c>
       <c r="AV17" s="2">
-        <f t="shared" si="12"/>
-        <v>729.31752827366404</v>
+        <f t="shared" si="11"/>
+        <v>578.54192788211469</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
@@ -3412,15 +3416,15 @@
         <v>-7.8129003470491121</v>
       </c>
       <c r="AC18" s="2">
+        <f t="shared" si="5"/>
+        <v>1.530243126630487</v>
+      </c>
+      <c r="AD18" s="2">
         <f t="shared" si="6"/>
-        <v>1.530243126630487</v>
-      </c>
-      <c r="AD18" s="2">
+        <v>-9.3431434736796</v>
+      </c>
+      <c r="AE18" s="4">
         <f t="shared" si="7"/>
-        <v>-9.3431434736796</v>
-      </c>
-      <c r="AE18" s="4">
-        <f t="shared" si="8"/>
         <v>18.607424828283037</v>
       </c>
       <c r="AF18" s="2">
@@ -3428,20 +3432,20 @@
         <v>-15.814462703349111</v>
       </c>
       <c r="AG18" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.91187331640352909</v>
+      </c>
+      <c r="AH18" s="3">
+        <f t="shared" si="8"/>
+        <v>1.317738379391848</v>
+      </c>
+      <c r="AI18" s="2">
         <f t="shared" si="9"/>
-        <v>-0.91187331640352909</v>
-      </c>
-      <c r="AH18" s="3">
-        <f t="shared" si="9"/>
-        <v>1.317738379391848</v>
-      </c>
-      <c r="AI18" s="2">
+        <v>0.69199875382271969</v>
+      </c>
+      <c r="AJ18" s="2">
         <f t="shared" si="10"/>
-        <v>0.69199875382271969</v>
-      </c>
-      <c r="AJ18" s="2">
-        <f t="shared" si="11"/>
-        <v>0.42852479015426859</v>
+        <v>0.71602881115130135</v>
       </c>
       <c r="AK18">
         <f t="shared" si="2"/>
@@ -3452,43 +3456,43 @@
         <v>442908.0974035</v>
       </c>
       <c r="AM18" s="3">
+        <f t="shared" si="12"/>
+        <v>-0.94973898192356077</v>
+      </c>
+      <c r="AN18">
         <f t="shared" si="4"/>
-        <v>-0.74996826054176313</v>
-      </c>
-      <c r="AN18">
-        <f t="shared" si="5"/>
-        <v>-0.27745346311550806</v>
+        <v>-0.34455398161993511</v>
       </c>
       <c r="AO18" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP18">
+      <c r="AP18" s="2">
         <f t="shared" si="13"/>
-        <v>1.4635519513705091</v>
+        <v>1.2088821857346015</v>
       </c>
       <c r="AQ18">
         <f t="shared" si="14"/>
-        <v>3.8576663285348212</v>
+        <v>3.0247950907077668</v>
       </c>
       <c r="AR18" s="1">
         <f t="shared" si="15"/>
-        <v>0.21981316973443407</v>
+        <v>0.29316164062004629</v>
       </c>
       <c r="AS18">
         <f t="shared" si="16"/>
-        <v>-2.9154763720671464</v>
+        <v>-1.7866138505067721</v>
       </c>
       <c r="AT18" s="1">
         <f t="shared" si="17"/>
-        <v>-0.51295321714130371</v>
+        <v>-0.42364475224929393</v>
       </c>
       <c r="AU18">
         <f t="shared" si="18"/>
-        <v>9.3317153544727969</v>
+        <v>8.6201393537453619</v>
       </c>
       <c r="AV18" s="2">
-        <f t="shared" si="12"/>
-        <v>708.70349050179982</v>
+        <f t="shared" si="11"/>
+        <v>530.66581098199913</v>
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Analytical solution using numSolve2.py
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t># avgT</t>
   </si>
@@ -141,10 +141,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>dev/deq_pred</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>s_n_real_pred</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -190,6 +186,14 @@
   </si>
   <si>
     <t>dratio_pred</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq-ratioF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dev/deq_pred</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -522,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX22"/>
+  <dimension ref="A1:AY22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AR1" sqref="AR1:AR1048576"/>
+      <selection activeCell="AN1" sqref="AN1:AN1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -550,18 +554,18 @@
     <col min="31" max="31" width="13.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.109375" style="2" customWidth="1"/>
     <col min="33" max="35" width="8.88671875" style="2"/>
-    <col min="36" max="36" width="12.88671875" customWidth="1"/>
-    <col min="39" max="39" width="8.88671875" style="2"/>
-    <col min="41" max="41" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.77734375" style="2" customWidth="1"/>
-    <col min="43" max="44" width="10.44140625" style="2" customWidth="1"/>
-    <col min="46" max="46" width="12.44140625" customWidth="1"/>
-    <col min="47" max="47" width="11.21875" customWidth="1"/>
-    <col min="50" max="50" width="13.33203125" style="2" customWidth="1"/>
-    <col min="51" max="1029" width="11.5546875"/>
+    <col min="36" max="37" width="12.88671875" style="2" customWidth="1"/>
+    <col min="40" max="40" width="8.88671875" style="2"/>
+    <col min="42" max="42" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.77734375" style="2" customWidth="1"/>
+    <col min="44" max="45" width="10.44140625" style="2" customWidth="1"/>
+    <col min="47" max="47" width="12.44140625" customWidth="1"/>
+    <col min="48" max="48" width="11.21875" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" style="2" customWidth="1"/>
+    <col min="52" max="1030" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,73 +651,76 @@
         <v>27</v>
       </c>
       <c r="AC1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AR1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.17366852143</v>
       </c>
@@ -800,7 +807,7 @@
         <v>-2.8766988791062431E-9</v>
       </c>
       <c r="AC2" s="2">
-        <f>1.34 *((AK2/100000)^0.3-(2594/100000)^0.3)</f>
+        <f>1.34 *((AL2/100000)^0.3-(2594/100000)^0.3)</f>
         <v>-1.9765021816098051E-3</v>
       </c>
       <c r="AD2" s="2">
@@ -815,54 +822,50 @@
         <f t="shared" ref="AF2:AF18" si="1">AB2-P2/2</f>
         <v>-2.8766988791062431E-9</v>
       </c>
-      <c r="AJ2" s="2">
-        <f>(( 1.588*EXP(-0.0005387*0.5*232))^2-AP2^2)/(2*AP2)+0.4</f>
-        <v>0.56109386188935539</v>
-      </c>
-      <c r="AK2">
-        <f t="shared" ref="AK2:AK18" si="2">(X2+Y2+Z2)/3</f>
+      <c r="AL2">
+        <f t="shared" ref="AL2:AL18" si="2">(X2+Y2+Z2)/3</f>
         <v>2556.0498433166663</v>
       </c>
-      <c r="AL2">
-        <f t="shared" ref="AL2:AL18" si="3">Z2-(Y2+X2)/2</f>
+      <c r="AM2">
+        <f t="shared" ref="AM2:AM18" si="3">Z2-(Y2+X2)/2</f>
         <v>3423.5295013549999</v>
       </c>
-      <c r="AM2" s="3">
-        <f>(-2*AI2-3)/(-2*AI2+6)</f>
+      <c r="AN2" s="3">
+        <f>(-2*AJ2-3)/(-2*AJ2+6)</f>
         <v>-0.5</v>
       </c>
-      <c r="AN2">
-        <f t="shared" ref="AN2:AN18" si="4">1/(2+AM2*AS2-2*0.33*(1+AM2+AS2))</f>
+      <c r="AO2">
+        <f t="shared" ref="AO2:AO18" si="4">1/(2+AN2*AT2-2*0.33*(1+AN2+AT2))</f>
         <v>0.5988023952095809</v>
       </c>
-      <c r="AO2" s="1" t="e">
-        <f>3*(1-2*0.33)*(AK2-AK1)/(AC2-AC1)</f>
+      <c r="AP2" s="1" t="e">
+        <f>3*(1-2*0.33)*(AL2-AL1)/(AC2-AC1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AP2" s="2">
-        <f>AL2/AK2</f>
+      <c r="AQ2" s="2">
+        <f>AM2/AL2</f>
         <v>1.3393829194319284</v>
       </c>
-      <c r="AQ2" s="2">
-        <f>AL2/AK2-(1.35*(AK2/3255000)^-0.0723)</f>
-        <v>-0.92434352155457233</v>
-      </c>
       <c r="AR2" s="2">
-        <f>1.35*(AK2/3255000)^-0.0723-1.386/(AE2+1.27)+0.03463</f>
+        <f>-1.386/(AE2+1.27)+0.03463</f>
+        <v>-1.0567085818531621</v>
+      </c>
+      <c r="AS2" s="2">
+        <f>1.35*(AL2/3255000)^-0.0723-1.386/(AE2+1.27)+0.03463</f>
         <v>1.2070178591333387</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>0</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>0</v>
       </c>
-      <c r="AX2" s="2">
-        <f>(AS2*X2-4*X2*(1-0.01*P2-2*0.01*AF2)*(0.08/0.4)/(-0.08/0.4*0.01*P2-(2*0.08/0.4+3)*0.01*AF2+0.08/0.4+1))/1000</f>
+      <c r="AY2" s="2">
+        <f>(AT2*X2-4*X2*(1-0.01*P2-2*0.01*AF2)*(0.08/0.4)/(-0.08/0.4*0.01*P2-(2*0.08/0.4+3)*0.01*AF2+0.08/0.4+1))/1000</f>
         <v>-0.95579557395708714</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.3863060409200001</v>
       </c>
@@ -949,7 +952,7 @@
         <v>0.42455699990888718</v>
       </c>
       <c r="AC3" s="2">
-        <f t="shared" ref="AC3:AC18" si="5">1.34 *((AK3/100000)^0.3-(2594/100000)^0.3)</f>
+        <f t="shared" ref="AC3:AC18" si="5">1.34 *((AL3/100000)^0.3-(2594/100000)^0.3)</f>
         <v>0.37815519616697812</v>
       </c>
       <c r="AD3" s="2">
@@ -977,66 +980,70 @@
         <v>-5.1394653408672643E-2</v>
       </c>
       <c r="AJ3" s="2">
-        <f t="shared" ref="AJ3:AJ18" si="10">(( 1.588*EXP(-0.0005387*0.5*232))^2-AP3^2)/(2*AP3)+0.4</f>
-        <v>0.54583656219090648</v>
-      </c>
-      <c r="AK3" s="1">
+        <f>-(1.35-(1.35*(AL3/3255000)^-0.0723))+0.2354+1.382*AR3</f>
+        <v>-1.2928989089855514E-2</v>
+      </c>
+      <c r="AK3" s="2">
+        <f>AI3+(1.35-(1.35*(AL3/3255000)^-0.0723))</f>
+        <v>-0.65262833329556669</v>
+      </c>
+      <c r="AL3" s="1">
         <f t="shared" si="2"/>
         <v>19947.490459600001</v>
       </c>
-      <c r="AL3" s="1">
+      <c r="AM3" s="1">
         <f t="shared" si="3"/>
         <v>26990.528974650002</v>
       </c>
-      <c r="AM3" s="3">
-        <f>(-2*AI3-3)/(-2*AI3+6)</f>
-        <v>-0.47473549348102495</v>
-      </c>
-      <c r="AN3" s="1">
+      <c r="AN3" s="3">
+        <f>(-2*AJ3-3)/(-2*AJ3+6)</f>
+        <v>-0.49356324569712429</v>
+      </c>
+      <c r="AO3" s="1">
         <f t="shared" si="4"/>
-        <v>-0.43893509681643</v>
-      </c>
-      <c r="AO3" s="1">
+        <v>-0.42899156719796372</v>
+      </c>
+      <c r="AP3" s="1">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP3" s="2">
-        <f>AL3/AK3</f>
+      <c r="AQ3" s="2">
+        <f>AM3/AL3</f>
         <v>1.3530789263599041</v>
       </c>
-      <c r="AQ3" s="2">
-        <f t="shared" ref="AQ3:AQ18" si="11">AL3/AK3-(1.35*(AK3/3255000)^-0.0723)</f>
-        <v>-0.59815475352698999</v>
-      </c>
       <c r="AR3" s="2">
-        <f t="shared" ref="AR3:AR18" si="12">1.35*(AK3/3255000)^-0.0723-1.386/(AE3+1.27)+0.03463</f>
+        <f t="shared" ref="AR3:AR18" si="10">-1.386/(AE3+1.27)+0.03463</f>
+        <v>-0.61473420331168571</v>
+      </c>
+      <c r="AS3" s="2">
+        <f t="shared" ref="AS3:AS18" si="11">1.35*(AL3/3255000)^-0.0723-1.386/(AE3+1.27)+0.03463</f>
         <v>1.3364994765752083</v>
       </c>
-      <c r="AS3" s="1">
-        <f>(2*AP3+3)/(3-AP3)</f>
+      <c r="AT3" s="1">
+        <f>(2*AQ3+3)/(3-AQ3)</f>
         <v>3.464742751823445</v>
       </c>
-      <c r="AT3" s="1">
-        <f>(1+2*AM3)*(AK3-AK2)*(1-AP3/3)/(3*AN3*AO3*AM3)</f>
-        <v>1.8915143640328775E-2</v>
-      </c>
       <c r="AU3" s="1">
-        <f>(AU2+AT3)</f>
-        <v>1.8915143640328775E-2</v>
+        <f>(1+2*AN3)*(AL3-AL2)*(1-AQ3/3)/(3*AO3*AP3*AN3)</f>
+        <v>4.7427059605727592E-3</v>
       </c>
       <c r="AV3" s="1">
-        <f>2*(1-AM3)*(AK3-AK2)*(1-AP3/3)/(9*AN3*AO3*AM3)</f>
-        <v>0.36803718647389322</v>
+        <f>(AV2+AU3)</f>
+        <v>4.7427059605727592E-3</v>
       </c>
       <c r="AW3" s="1">
-        <f>AW2+AV3</f>
-        <v>0.36803718647389322</v>
-      </c>
-      <c r="AX3" s="2">
-        <f t="shared" ref="AX3:AX18" si="13">(AS3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
+        <f>2*(1-AN3)*(AL3-AL2)*(1-AQ3/3)/(9*AO3*AP3*AN3)</f>
+        <v>0.36682728460913289</v>
+      </c>
+      <c r="AX3" s="1">
+        <f>AX2+AW3</f>
+        <v>0.36682728460913289</v>
+      </c>
+      <c r="AY3" s="2">
+        <f t="shared" ref="AY3:AY18" si="12">(AT3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
         <v>31.048885324486896</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.4615371024499999</v>
       </c>
@@ -1151,66 +1158,70 @@
         <v>0.16424718930868293</v>
       </c>
       <c r="AJ4" s="2">
-        <f t="shared" si="10"/>
-        <v>0.47229178477375378</v>
-      </c>
-      <c r="AK4">
+        <f t="shared" ref="AJ4:AJ22" si="13">-(1.35-(1.35*(AL4/3255000)^-0.0723))+0.2354+1.382*AR4</f>
+        <v>0.13716108102294489</v>
+      </c>
+      <c r="AK4" s="2">
+        <f t="shared" ref="AK4:AK18" si="14">AI4+(1.35-(1.35*(AL4/3255000)^-0.0723))</f>
+        <v>-0.30812391846028003</v>
+      </c>
+      <c r="AL4">
         <f t="shared" si="2"/>
         <v>51321.077509900002</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <f t="shared" si="3"/>
         <v>72940.740784349997</v>
       </c>
-      <c r="AM4" s="3">
-        <f t="shared" ref="AM4:AM18" si="14">(-2*AI4-3)/(-2*AI4+6)</f>
-        <v>-0.58688020445017652</v>
-      </c>
-      <c r="AN4">
+      <c r="AN4" s="3">
+        <f t="shared" ref="AN4:AN18" si="15">(-2*AJ4-3)/(-2*AJ4+6)</f>
+        <v>-0.5718662933393166</v>
+      </c>
+      <c r="AO4">
         <f t="shared" si="4"/>
-        <v>-0.34637286525300914</v>
-      </c>
-      <c r="AO4" s="3">
+        <v>-0.3519381325233058</v>
+      </c>
+      <c r="AP4" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP4" s="2">
-        <f t="shared" ref="AP4:AP18" si="15">AL4/AK4</f>
+      <c r="AQ4" s="2">
+        <f t="shared" ref="AQ4:AQ18" si="16">AM4/AL4</f>
         <v>1.421262848003912</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="AR4" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.41288713946889882</v>
+      </c>
+      <c r="AS4" s="2">
         <f t="shared" si="11"/>
-        <v>-0.40110825976505105</v>
-      </c>
-      <c r="AR4" s="2">
+        <v>1.4094839683000642</v>
+      </c>
+      <c r="AT4">
+        <f t="shared" ref="AT4:AT18" si="17">(2*AQ4+3)/(3-AQ4)</f>
+        <v>3.7007589823428071</v>
+      </c>
+      <c r="AU4" s="1">
+        <f t="shared" ref="AU4:AU18" si="18">(1+2*AN4)*(AL4-AL3)*(1-AQ4/3)/(3*AO4*AP4*AN4)</f>
+        <v>-9.633429338296641E-2</v>
+      </c>
+      <c r="AV4">
+        <f t="shared" ref="AV4:AV18" si="19">AV3+AU4</f>
+        <v>-9.159158742239365E-2</v>
+      </c>
+      <c r="AW4" s="1">
+        <f t="shared" ref="AW4:AW18" si="20">2*(1-AN4)*(AL4-AL3)*(1-AQ4/3)/(9*AO4*AP4*AN4)</f>
+        <v>0.70234422668957619</v>
+      </c>
+      <c r="AX4">
+        <f>AX3+AW4</f>
+        <v>1.069171511298709</v>
+      </c>
+      <c r="AY4" s="2">
         <f t="shared" si="12"/>
-        <v>1.4094839683000642</v>
-      </c>
-      <c r="AS4">
-        <f t="shared" ref="AS4:AS18" si="16">(2*AP4+3)/(3-AP4)</f>
-        <v>3.7007589823428071</v>
-      </c>
-      <c r="AT4" s="1">
-        <f t="shared" ref="AT4:AT18" si="17">(1+2*AM4)*(AK4-AK3)*(1-AP4/3)/(3*AN4*AO4*AM4)</f>
-        <v>-0.11530390241841393</v>
-      </c>
-      <c r="AU4">
-        <f t="shared" ref="AU4:AU18" si="18">AU3+AT4</f>
-        <v>-9.6388758778085157E-2</v>
-      </c>
-      <c r="AV4" s="1">
-        <f t="shared" ref="AV4:AV18" si="19">2*(1-AM4)*(AK4-AK3)*(1-AP4/3)/(9*AN4*AO4*AM4)</f>
-        <v>0.70201446310118631</v>
-      </c>
-      <c r="AW4">
-        <f>AW3+AV4</f>
-        <v>1.0700516495750796</v>
-      </c>
-      <c r="AX4" s="2">
-        <f t="shared" si="13"/>
         <v>83.878038367314915</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.0730406484000001</v>
       </c>
@@ -1325,66 +1336,70 @@
         <v>0.16525783709594841</v>
       </c>
       <c r="AJ5" s="2">
-        <f t="shared" si="10"/>
-        <v>0.44251031757577897</v>
-      </c>
-      <c r="AK5">
+        <f t="shared" si="13"/>
+        <v>0.21310133756212912</v>
+      </c>
+      <c r="AK5" s="2">
+        <f t="shared" si="14"/>
+        <v>-0.23369233205721099</v>
+      </c>
+      <c r="AL5">
         <f t="shared" si="2"/>
         <v>90638.674862666681</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <f t="shared" si="3"/>
         <v>131416.95121849998</v>
       </c>
-      <c r="AM5" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.58744596206590272</v>
-      </c>
-      <c r="AN5">
+      <c r="AN5" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.6146981089235497</v>
+      </c>
+      <c r="AO5">
         <f t="shared" si="4"/>
-        <v>-0.33110852548566583</v>
-      </c>
-      <c r="AO5" s="3">
+        <v>-0.32196837616875357</v>
+      </c>
+      <c r="AP5" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP5" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ5" s="2">
+        <f t="shared" si="16"/>
         <v>1.4498992998035272</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="AR5" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.3048110214117441</v>
+      </c>
+      <c r="AS5" s="2">
         <f t="shared" si="11"/>
-        <v>-0.29905086934963232</v>
-      </c>
-      <c r="AR5" s="2">
+        <v>1.4441391477414154</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" si="17"/>
+        <v>3.8060744046236894</v>
+      </c>
+      <c r="AU5" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.19238470260591006</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" si="19"/>
+        <v>-0.28397629002830371</v>
+      </c>
+      <c r="AW5" s="1">
+        <f t="shared" si="20"/>
+        <v>0.90278505431633316</v>
+      </c>
+      <c r="AX5">
+        <f>AX4+AW5</f>
+        <v>1.9719565656150422</v>
+      </c>
+      <c r="AY5" s="2">
         <f t="shared" si="12"/>
-        <v>1.4441391477414154</v>
-      </c>
-      <c r="AS5">
-        <f t="shared" si="16"/>
-        <v>3.8060744046236894</v>
-      </c>
-      <c r="AT5" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.14924192667254385</v>
-      </c>
-      <c r="AU5">
-        <f t="shared" si="18"/>
-        <v>-0.24563068545062899</v>
-      </c>
-      <c r="AV5" s="1">
-        <f t="shared" si="19"/>
-        <v>0.90308531985623286</v>
-      </c>
-      <c r="AW5">
-        <f>AW4+AV5</f>
-        <v>1.9731369694313123</v>
-      </c>
-      <c r="AX5" s="2">
-        <f t="shared" si="13"/>
         <v>151.60234099951631</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.0101377271699992</v>
       </c>
@@ -1499,66 +1514,70 @@
         <v>0.36754258371404336</v>
       </c>
       <c r="AJ6" s="2">
-        <f t="shared" si="10"/>
-        <v>0.42224854292958564</v>
-      </c>
-      <c r="AK6">
+        <f t="shared" si="13"/>
+        <v>0.26055515659463535</v>
+      </c>
+      <c r="AK6" s="2">
+        <f t="shared" si="14"/>
+        <v>1.8954057987516482E-2</v>
+      </c>
+      <c r="AL6">
         <f t="shared" si="2"/>
         <v>135775.63518106667</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <f t="shared" si="3"/>
         <v>199552.3578074</v>
       </c>
-      <c r="AM6" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.70942936138693358</v>
-      </c>
-      <c r="AN6">
+      <c r="AN6" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.64266859062076032</v>
+      </c>
+      <c r="AO6">
         <f t="shared" si="4"/>
-        <v>-0.28515064788020883</v>
-      </c>
-      <c r="AO6" s="3">
+        <v>-0.30377935487388319</v>
+      </c>
+      <c r="AP6" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP6" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ6" s="2">
+        <f t="shared" si="16"/>
         <v>1.4697214087143282</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="AR6" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.23403282860484198</v>
+      </c>
+      <c r="AS6" s="2">
         <f t="shared" si="11"/>
-        <v>-0.22886711701219875</v>
-      </c>
-      <c r="AR6" s="2">
+        <v>1.4645556971216849</v>
+      </c>
+      <c r="AT6">
+        <f t="shared" si="17"/>
+        <v>3.8812820431857453</v>
+      </c>
+      <c r="AU6" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.27493393099282515</v>
+      </c>
+      <c r="AV6">
+        <f t="shared" si="19"/>
+        <v>-0.55891022102112886</v>
+      </c>
+      <c r="AW6" s="1">
+        <f t="shared" si="20"/>
+        <v>1.0551851461552919</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" ref="AX6:AX18" si="21">AX5+AW6</f>
+        <v>3.0271417117703341</v>
+      </c>
+      <c r="AY6" s="2">
         <f t="shared" si="12"/>
-        <v>1.4645556971216849</v>
-      </c>
-      <c r="AS6">
-        <f t="shared" si="16"/>
-        <v>3.8812820431857453</v>
-      </c>
-      <c r="AT6" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.38949272303242916</v>
-      </c>
-      <c r="AU6">
-        <f t="shared" si="18"/>
-        <v>-0.63512340848305815</v>
-      </c>
-      <c r="AV6" s="1">
-        <f t="shared" si="19"/>
-        <v>1.059721350099295</v>
-      </c>
-      <c r="AW6">
-        <f t="shared" ref="AW6:AW18" si="20">AW5+AV6</f>
-        <v>3.0328583195306074</v>
-      </c>
-      <c r="AX6" s="2">
-        <f t="shared" si="13"/>
         <v>230.65721129774403</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12.176646483900001</v>
       </c>
@@ -1673,66 +1692,70 @@
         <v>0.27255207952320798</v>
       </c>
       <c r="AJ7" s="2">
-        <f t="shared" si="10"/>
-        <v>0.40967713528617822</v>
-      </c>
-      <c r="AK7">
+        <f t="shared" si="13"/>
+        <v>0.28761602241634676</v>
+      </c>
+      <c r="AK7" s="2">
+        <f t="shared" si="14"/>
+        <v>-4.032785581487891E-2</v>
+      </c>
+      <c r="AL7">
         <f t="shared" si="2"/>
         <v>182157.4419312333</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <f t="shared" si="3"/>
         <v>269986.16568114999</v>
       </c>
-      <c r="AM7" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.64989401491975829</v>
-      </c>
-      <c r="AN7">
+      <c r="AN7" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.65905713836610169</v>
+      </c>
+      <c r="AO7">
         <f t="shared" si="4"/>
-        <v>-0.29601020053209681</v>
-      </c>
-      <c r="AO7" s="3">
+        <v>-0.29340824324090536</v>
+      </c>
+      <c r="AP7" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP7" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ7" s="2">
+        <f t="shared" si="16"/>
         <v>1.4821583066755686</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="AR7" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.18861354046435613</v>
+      </c>
+      <c r="AS7" s="2">
         <f t="shared" si="11"/>
-        <v>-0.1807216286625184</v>
-      </c>
-      <c r="AR7" s="2">
+        <v>1.4742663948737307</v>
+      </c>
+      <c r="AT7">
+        <f t="shared" si="17"/>
+        <v>3.9294721179307417</v>
+      </c>
+      <c r="AU7" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.31540924250029956</v>
+      </c>
+      <c r="AV7">
+        <f t="shared" si="19"/>
+        <v>-0.87431946352142842</v>
+      </c>
+      <c r="AW7" s="1">
+        <f t="shared" si="20"/>
+        <v>1.0966330729785276</v>
+      </c>
+      <c r="AX7">
+        <f t="shared" si="21"/>
+        <v>4.1237747847488615</v>
+      </c>
+      <c r="AY7" s="2">
         <f t="shared" si="12"/>
-        <v>1.4742663948737307</v>
-      </c>
-      <c r="AS7">
-        <f t="shared" si="16"/>
-        <v>3.9294721179307417</v>
-      </c>
-      <c r="AT7" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.29878012725482339</v>
-      </c>
-      <c r="AU7">
-        <f t="shared" si="18"/>
-        <v>-0.93390353573788154</v>
-      </c>
-      <c r="AV7" s="1">
-        <f t="shared" si="19"/>
-        <v>1.096231324954474</v>
-      </c>
-      <c r="AW7">
-        <f t="shared" si="20"/>
-        <v>4.1290896444850809</v>
-      </c>
-      <c r="AX7" s="2">
-        <f t="shared" si="13"/>
         <v>312.06306622211565</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15.449823501799999</v>
       </c>
@@ -1847,66 +1870,70 @@
         <v>0.38562228960070855</v>
       </c>
       <c r="AJ8" s="2">
-        <f t="shared" si="10"/>
-        <v>0.40457569788824999</v>
-      </c>
-      <c r="AK8">
+        <f t="shared" si="13"/>
+        <v>0.30592044667071117</v>
+      </c>
+      <c r="AK8" s="2">
+        <f t="shared" si="14"/>
+        <v>0.10091745549064901</v>
+      </c>
+      <c r="AL8">
         <f t="shared" si="2"/>
         <v>230725.84384566665</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <f t="shared" si="3"/>
         <v>343143.63679850003</v>
       </c>
-      <c r="AM8" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.7212509049859972</v>
-      </c>
-      <c r="AN8">
+      <c r="AN8" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.67032929463385416</v>
+      </c>
+      <c r="AO8">
         <f t="shared" si="4"/>
-        <v>-0.27479710670582819</v>
-      </c>
-      <c r="AO8" s="3">
+        <v>-0.28805590302797707</v>
+      </c>
+      <c r="AP8" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP8" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ8" s="2">
+        <f t="shared" si="16"/>
         <v>1.4872353745860825</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="AR8" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.15498146703281362</v>
+      </c>
+      <c r="AS8" s="2">
         <f t="shared" si="11"/>
-        <v>-0.14746945952397716</v>
-      </c>
-      <c r="AR8" s="2">
+        <v>1.4797233670772458</v>
+      </c>
+      <c r="AT8">
+        <f t="shared" si="17"/>
+        <v>3.9493723271969357</v>
+      </c>
+      <c r="AU8" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.35301408447238236</v>
+      </c>
+      <c r="AV8">
+        <f t="shared" si="19"/>
+        <v>-1.2273335479938108</v>
+      </c>
+      <c r="AW8" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1539407983813592</v>
+      </c>
+      <c r="AX8">
+        <f t="shared" si="21"/>
+        <v>5.2777155831302203</v>
+      </c>
+      <c r="AY8" s="2">
         <f t="shared" si="12"/>
-        <v>1.4797233670772458</v>
-      </c>
-      <c r="AS8">
-        <f t="shared" si="16"/>
-        <v>3.9493723271969357</v>
-      </c>
-      <c r="AT8" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.4467393344404133</v>
-      </c>
-      <c r="AU8">
-        <f t="shared" si="18"/>
-        <v>-1.3806428701782949</v>
-      </c>
-      <c r="AV8" s="1">
-        <f t="shared" si="19"/>
-        <v>1.1584893987922444</v>
-      </c>
-      <c r="AW8">
-        <f t="shared" si="20"/>
-        <v>5.2875790432773258</v>
-      </c>
-      <c r="AX8" s="2">
-        <f t="shared" si="13"/>
         <v>396.30829648304172</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>18.810443319000001</v>
       </c>
@@ -2021,66 +2048,70 @@
         <v>0.31133034989955954</v>
       </c>
       <c r="AJ9" s="2">
-        <f t="shared" si="10"/>
-        <v>0.40424344843035476</v>
-      </c>
-      <c r="AK9">
+        <f t="shared" si="13"/>
+        <v>0.3169663317101642</v>
+      </c>
+      <c r="AK9" s="2">
+        <f t="shared" si="14"/>
+        <v>4.9300687410046007E-2</v>
+      </c>
+      <c r="AL9">
         <f t="shared" si="2"/>
         <v>279898.81311533332</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <f t="shared" si="3"/>
         <v>416368.13751550001</v>
       </c>
-      <c r="AM9" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.673690183482338</v>
-      </c>
-      <c r="AN9">
+      <c r="AN9" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.67720593788459515</v>
+      </c>
+      <c r="AO9">
         <f t="shared" si="4"/>
-        <v>-0.28699827519653104</v>
-      </c>
-      <c r="AO9" s="3">
+        <v>-0.28604849626521334</v>
+      </c>
+      <c r="AP9" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP9" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ9" s="2">
+        <f t="shared" si="16"/>
         <v>1.4875666419633369</v>
       </c>
-      <c r="AQ9" s="2">
+      <c r="AR9" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.13058128131646116</v>
+      </c>
+      <c r="AS9" s="2">
         <f t="shared" si="11"/>
-        <v>-0.12446302052617675</v>
-      </c>
-      <c r="AR9" s="2">
+        <v>1.4814483811730523</v>
+      </c>
+      <c r="AT9">
+        <f t="shared" si="17"/>
+        <v>3.950675414672935</v>
+      </c>
+      <c r="AU9" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.3705638200463337</v>
+      </c>
+      <c r="AV9">
+        <f t="shared" si="19"/>
+        <v>-1.5978973680401445</v>
+      </c>
+      <c r="AW9" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1690952097246072</v>
+      </c>
+      <c r="AX9">
+        <f t="shared" si="21"/>
+        <v>6.4468107928548273</v>
+      </c>
+      <c r="AY9" s="2">
         <f t="shared" si="12"/>
-        <v>1.4814483811730523</v>
-      </c>
-      <c r="AS9">
-        <f t="shared" si="16"/>
-        <v>3.950675414672935</v>
-      </c>
-      <c r="AT9" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.36389906440701658</v>
-      </c>
-      <c r="AU9">
-        <f t="shared" si="18"/>
-        <v>-1.7445419345853115</v>
-      </c>
-      <c r="AV9" s="1">
-        <f t="shared" si="19"/>
-        <v>1.16885187879825</v>
-      </c>
-      <c r="AW9">
-        <f t="shared" si="20"/>
-        <v>6.456430922075576</v>
-      </c>
-      <c r="AX9" s="2">
-        <f t="shared" si="13"/>
         <v>480.40795615833036</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22.1821845652</v>
       </c>
@@ -2195,66 +2226,70 @@
         <v>0.40119168171511116</v>
       </c>
       <c r="AJ10" s="2">
-        <f t="shared" si="10"/>
-        <v>0.40507075527034625</v>
-      </c>
-      <c r="AK10">
+        <f t="shared" si="13"/>
+        <v>0.32508510830967652</v>
+      </c>
+      <c r="AK10" s="2">
+        <f t="shared" si="14"/>
+        <v>0.15781244541759759</v>
+      </c>
+      <c r="AL10">
         <f t="shared" si="2"/>
         <v>328777.82239633333</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <f t="shared" si="3"/>
         <v>488807.77019649994</v>
       </c>
-      <c r="AM10" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.73156287377509355</v>
-      </c>
-      <c r="AN10">
+      <c r="AN10" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.68229651492065768</v>
+      </c>
+      <c r="AO10">
         <f t="shared" si="4"/>
-        <v>-0.27245961270850599</v>
-      </c>
-      <c r="AO10" s="3">
+        <v>-0.28503761272927297</v>
+      </c>
+      <c r="AP10" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP10" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ10" s="2">
+        <f t="shared" si="16"/>
         <v>1.4867419177904724</v>
       </c>
-      <c r="AQ10" s="2">
+      <c r="AR10" s="2">
+        <f t="shared" si="10"/>
+        <v>-0.11121138059901381</v>
+      </c>
+      <c r="AS10" s="2">
         <f t="shared" si="11"/>
-        <v>-0.10663731850704128</v>
-      </c>
-      <c r="AR10" s="2">
+        <v>1.4821678556984998</v>
+      </c>
+      <c r="AT10">
+        <f t="shared" si="17"/>
+        <v>3.9474323023994584</v>
+      </c>
+      <c r="AU10" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.3776425553857754</v>
+      </c>
+      <c r="AV10">
+        <f t="shared" si="19"/>
+        <v>-1.9755399234259199</v>
+      </c>
+      <c r="AW10" s="1">
+        <f t="shared" si="20"/>
+        <v>1.1616728842160089</v>
+      </c>
+      <c r="AX10">
+        <f t="shared" si="21"/>
+        <v>7.6084836770708364</v>
+      </c>
+      <c r="AY10" s="2">
         <f t="shared" si="12"/>
-        <v>1.4821678556984998</v>
-      </c>
-      <c r="AS10">
-        <f t="shared" si="16"/>
-        <v>3.9474323023994584</v>
-      </c>
-      <c r="AT10" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.46805083579045414</v>
-      </c>
-      <c r="AU10">
-        <f t="shared" si="18"/>
-        <v>-2.2125927703757657</v>
-      </c>
-      <c r="AV10" s="1">
-        <f t="shared" si="19"/>
-        <v>1.1666513966329444</v>
-      </c>
-      <c r="AW10">
-        <f t="shared" si="20"/>
-        <v>7.6230823187085202</v>
-      </c>
-      <c r="AX10" s="2">
-        <f t="shared" si="13"/>
         <v>564.33125013541826</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25.4604440606</v>
       </c>
@@ -2369,66 +2404,70 @@
         <v>0.39052838706837911</v>
       </c>
       <c r="AJ11" s="2">
-        <f t="shared" si="10"/>
-        <v>0.41190691709578892</v>
-      </c>
-      <c r="AK11">
+        <f t="shared" si="13"/>
+        <v>0.33119663226499868</v>
+      </c>
+      <c r="AK11" s="2">
+        <f t="shared" si="14"/>
+        <v>0.16227730569698551</v>
+      </c>
+      <c r="AL11">
         <f t="shared" si="2"/>
         <v>375151.09649433335</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <f t="shared" si="3"/>
         <v>555202.86013150006</v>
       </c>
-      <c r="AM11" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.72448704852721413</v>
-      </c>
-      <c r="AN11">
+      <c r="AN11" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.6861489514003144</v>
+      </c>
+      <c r="AO11">
         <f t="shared" si="4"/>
-        <v>-0.2769939879259114</v>
-      </c>
-      <c r="AO11" s="3">
+        <v>-0.28692985402617949</v>
+      </c>
+      <c r="AP11" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP11" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ11" s="2">
+        <f t="shared" si="16"/>
         <v>1.4799446551527975</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="AR11" s="2">
+        <f t="shared" si="10"/>
+        <v>-9.5842582566132373E-2</v>
+      </c>
+      <c r="AS11" s="2">
         <f t="shared" si="11"/>
-        <v>-9.8306426218596199E-2</v>
-      </c>
-      <c r="AR11" s="2">
+        <v>1.4824084988052613</v>
+      </c>
+      <c r="AT11">
+        <f t="shared" si="17"/>
+        <v>3.9208370474857208</v>
+      </c>
+      <c r="AU11" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.3630246395685261</v>
+      </c>
+      <c r="AV11">
+        <f t="shared" si="19"/>
+        <v>-2.338564562994446</v>
+      </c>
+      <c r="AW11" s="1">
+        <f t="shared" si="20"/>
+        <v>1.096100033040375</v>
+      </c>
+      <c r="AX11">
+        <f t="shared" si="21"/>
+        <v>8.704583710111212</v>
+      </c>
+      <c r="AY11" s="2">
         <f t="shared" si="12"/>
-        <v>1.4824084988052613</v>
-      </c>
-      <c r="AS11">
-        <f t="shared" si="16"/>
-        <v>3.9208370474857208</v>
-      </c>
-      <c r="AT11" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.42949683827302865</v>
-      </c>
-      <c r="AU11">
-        <f t="shared" si="18"/>
-        <v>-2.6420896086487944</v>
-      </c>
-      <c r="AV11" s="1">
-        <f t="shared" si="19"/>
-        <v>1.0997839145501775</v>
-      </c>
-      <c r="AW11">
-        <f t="shared" si="20"/>
-        <v>8.7228662332586975</v>
-      </c>
-      <c r="AX11" s="2">
-        <f t="shared" si="13"/>
         <v>641.86882088350251</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28.5971191999</v>
       </c>
@@ -2543,66 +2582,70 @@
         <v>0.330298467982723</v>
       </c>
       <c r="AJ12" s="2">
-        <f t="shared" si="10"/>
-        <v>0.42536557513271239</v>
-      </c>
-      <c r="AK12">
+        <f t="shared" si="13"/>
+        <v>0.33614504624275532</v>
+      </c>
+      <c r="AK12" s="2">
+        <f t="shared" si="14"/>
+        <v>0.1140885314607003</v>
+      </c>
+      <c r="AL12">
         <f t="shared" si="2"/>
         <v>417071.63527299999</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <f t="shared" si="3"/>
         <v>611699.82950849994</v>
       </c>
-      <c r="AM12" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.68558168245860607</v>
-      </c>
-      <c r="AN12">
+      <c r="AN12" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.68928116512235682</v>
+      </c>
+      <c r="AO12">
         <f t="shared" si="4"/>
-        <v>-0.29288859123013355</v>
-      </c>
-      <c r="AO12" s="3">
+        <v>-0.29187356348233073</v>
+      </c>
+      <c r="AP12" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP12" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ12" s="2">
+        <f t="shared" si="16"/>
         <v>1.4666541135268127</v>
       </c>
-      <c r="AQ12" s="2">
+      <c r="AR12" s="2">
+        <f t="shared" si="10"/>
+        <v>-8.3549124659383051E-2</v>
+      </c>
+      <c r="AS12" s="2">
         <f t="shared" si="11"/>
-        <v>-9.9555822995210042E-2</v>
-      </c>
-      <c r="AR12" s="2">
+        <v>1.4826608118626396</v>
+      </c>
+      <c r="AT12">
+        <f t="shared" si="17"/>
+        <v>3.869517164650103</v>
+      </c>
+      <c r="AU12" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.3294016018343443</v>
+      </c>
+      <c r="AV12">
+        <f t="shared" si="19"/>
+        <v>-2.6679661648287905</v>
+      </c>
+      <c r="AW12" s="1">
+        <f t="shared" si="20"/>
+        <v>0.97993888506230964</v>
+      </c>
+      <c r="AX12">
+        <f t="shared" si="21"/>
+        <v>9.6845225951735223</v>
+      </c>
+      <c r="AY12" s="2">
         <f t="shared" si="12"/>
-        <v>1.4826608118626396</v>
-      </c>
-      <c r="AS12">
-        <f t="shared" si="16"/>
-        <v>3.869517164650103</v>
-      </c>
-      <c r="AT12" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.32358093460233733</v>
-      </c>
-      <c r="AU12">
-        <f t="shared" si="18"/>
-        <v>-2.9656705432511319</v>
-      </c>
-      <c r="AV12" s="1">
-        <f t="shared" si="19"/>
-        <v>0.97966223270300812</v>
-      </c>
-      <c r="AW12">
-        <f t="shared" si="20"/>
-        <v>9.7025284659617057</v>
-      </c>
-      <c r="AX12" s="2">
-        <f t="shared" si="13"/>
         <v>708.60531781783538</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>30.854626388900002</v>
       </c>
@@ -2717,66 +2760,70 @@
         <v>0.59245405012693442</v>
       </c>
       <c r="AJ13" s="2">
-        <f t="shared" si="10"/>
-        <v>0.45511912099003649</v>
-      </c>
-      <c r="AK13">
+        <f t="shared" si="13"/>
+        <v>0.34662868833166355</v>
+      </c>
+      <c r="AK13" s="2">
+        <f t="shared" si="14"/>
+        <v>0.3812852481491118</v>
+      </c>
+      <c r="AL13">
         <f t="shared" si="2"/>
         <v>436089.82460366673</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <f t="shared" si="3"/>
         <v>626967.5865185</v>
       </c>
-      <c r="AM13" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.8691232041644964</v>
-      </c>
-      <c r="AN13">
+      <c r="AN13" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.69595562453359594</v>
+      </c>
+      <c r="AO13">
         <f t="shared" si="4"/>
-        <v>-0.26061853912273791</v>
-      </c>
-      <c r="AO13" s="3">
+        <v>-0.30302327242107752</v>
+      </c>
+      <c r="AP13" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP13" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ13" s="2">
+        <f t="shared" si="16"/>
         <v>1.4377028564890491</v>
       </c>
-      <c r="AQ13" s="2">
+      <c r="AR13" s="2">
+        <f t="shared" si="10"/>
+        <v>-7.2315567037741724E-2</v>
+      </c>
+      <c r="AS13" s="2">
         <f t="shared" si="11"/>
-        <v>-0.12346594548877365</v>
-      </c>
-      <c r="AR13" s="2">
+        <v>1.4888532349400809</v>
+      </c>
+      <c r="AT13">
+        <f t="shared" si="17"/>
+        <v>3.7607479072606491</v>
+      </c>
+      <c r="AU13" s="1">
+        <f t="shared" si="18"/>
+        <v>-0.15037494992411293</v>
+      </c>
+      <c r="AV13">
+        <f t="shared" si="19"/>
+        <v>-2.8183411147529034</v>
+      </c>
+      <c r="AW13" s="1">
+        <f t="shared" si="20"/>
+        <v>0.43382142040196658</v>
+      </c>
+      <c r="AX13">
+        <f t="shared" si="21"/>
+        <v>10.118344015575488</v>
+      </c>
+      <c r="AY13" s="2">
         <f t="shared" si="12"/>
-        <v>1.4888532349400809</v>
-      </c>
-      <c r="AS13">
-        <f t="shared" si="16"/>
-        <v>3.7607479072606491</v>
-      </c>
-      <c r="AT13" s="1">
-        <f t="shared" si="17"/>
-        <v>-0.26373027711361469</v>
-      </c>
-      <c r="AU13">
-        <f t="shared" si="18"/>
-        <v>-3.2294008203647464</v>
-      </c>
-      <c r="AV13" s="1">
-        <f t="shared" si="19"/>
-        <v>0.44514891417673641</v>
-      </c>
-      <c r="AW13">
-        <f t="shared" si="20"/>
-        <v>10.147677380138441</v>
-      </c>
-      <c r="AX13" s="2">
-        <f t="shared" si="13"/>
         <v>726.10196678091063</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32.080066029599998</v>
       </c>
@@ -2891,66 +2938,70 @@
         <v>0.81663594196838252</v>
       </c>
       <c r="AJ14" s="2">
-        <f t="shared" si="10"/>
-        <v>0.49536469757931656</v>
-      </c>
-      <c r="AK14">
+        <f t="shared" si="13"/>
+        <v>0.36014457375338738</v>
+      </c>
+      <c r="AK14" s="2">
+        <f t="shared" si="14"/>
+        <v>0.60611040714156361</v>
+      </c>
+      <c r="AL14">
         <f t="shared" si="2"/>
         <v>438582.73709499999</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <f t="shared" si="3"/>
         <v>613789.68986549997</v>
       </c>
-      <c r="AM14" s="3">
-        <f t="shared" si="14"/>
-        <v>-1.0610396985544017</v>
-      </c>
-      <c r="AN14">
+      <c r="AN14" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.7046388053144903</v>
+      </c>
+      <c r="AO14">
         <f t="shared" si="4"/>
-        <v>-0.23835834391504512</v>
-      </c>
-      <c r="AO14" s="3">
+        <v>-0.3185442642030018</v>
+      </c>
+      <c r="AP14" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP14" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ14" s="2">
+        <f t="shared" si="16"/>
         <v>1.3994843799165515</v>
       </c>
-      <c r="AQ14" s="2">
+      <c r="AR14" s="2">
+        <f t="shared" si="10"/>
+        <v>-6.2070159966303586E-2</v>
+      </c>
+      <c r="AS14" s="2">
         <f t="shared" si="11"/>
-        <v>-0.16104115491026749</v>
-      </c>
-      <c r="AR14" s="2">
+        <v>1.4984553748605154</v>
+      </c>
+      <c r="AT14">
+        <f t="shared" si="17"/>
+        <v>3.623187857129913</v>
+      </c>
+      <c r="AU14" s="1">
+        <f t="shared" si="18"/>
+        <v>-1.9813494840667002E-2</v>
+      </c>
+      <c r="AV14">
+        <f t="shared" si="19"/>
+        <v>-2.8381546095935706</v>
+      </c>
+      <c r="AW14" s="1">
+        <f t="shared" si="20"/>
+        <v>5.5015391830488841E-2</v>
+      </c>
+      <c r="AX14">
+        <f t="shared" si="21"/>
+        <v>10.173359407405977</v>
+      </c>
+      <c r="AY14" s="2">
         <f t="shared" si="12"/>
-        <v>1.4984553748605154</v>
-      </c>
-      <c r="AS14">
-        <f t="shared" si="16"/>
-        <v>3.623187857129913</v>
-      </c>
-      <c r="AT14" s="1">
-        <f t="shared" si="17"/>
-        <v>-4.8210433931383655E-2</v>
-      </c>
-      <c r="AU14">
-        <f t="shared" si="18"/>
-        <v>-3.2776112542961302</v>
-      </c>
-      <c r="AV14" s="1">
-        <f t="shared" si="19"/>
-        <v>5.9035405440494577E-2</v>
-      </c>
-      <c r="AW14">
-        <f t="shared" si="20"/>
-        <v>10.206712785578937</v>
-      </c>
-      <c r="AX14" s="2">
-        <f t="shared" si="13"/>
         <v>712.89688778342315</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>32.297219829100001</v>
       </c>
@@ -3065,66 +3116,70 @@
         <v>1.2245083428133143</v>
       </c>
       <c r="AJ15" s="2">
-        <f t="shared" si="10"/>
-        <v>0.56076249307108816</v>
-      </c>
-      <c r="AK15">
+        <f t="shared" si="13"/>
+        <v>0.38022436463206377</v>
+      </c>
+      <c r="AK15" s="2">
+        <f t="shared" si="14"/>
+        <v>1.008143828271834</v>
+      </c>
+      <c r="AL15">
         <f t="shared" si="2"/>
         <v>416502.71381466667</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <f t="shared" si="3"/>
         <v>557979.83421200002</v>
       </c>
-      <c r="AM15" s="3">
-        <f t="shared" si="14"/>
-        <v>-1.5345092339833188</v>
-      </c>
-      <c r="AN15">
+      <c r="AN15" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.71770434813132167</v>
+      </c>
+      <c r="AO15">
         <f t="shared" si="4"/>
-        <v>-0.19402989565662734</v>
-      </c>
-      <c r="AO15" s="3">
+        <v>-0.34495336502006951</v>
+      </c>
+      <c r="AP15" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP15" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ15" s="2">
+        <f t="shared" si="16"/>
         <v>1.3396787480724246</v>
       </c>
-      <c r="AQ15" s="2">
+      <c r="AR15" s="2">
+        <f t="shared" si="10"/>
+        <v>-5.1765665636336118E-2</v>
+      </c>
+      <c r="AS15" s="2">
         <f t="shared" si="11"/>
-        <v>-0.2266857664690558</v>
-      </c>
-      <c r="AR15" s="2">
+        <v>1.5145988489051443</v>
+      </c>
+      <c r="AT15">
+        <f t="shared" si="17"/>
+        <v>3.4206377166776081</v>
+      </c>
+      <c r="AU15" s="1">
+        <f t="shared" si="18"/>
+        <v>0.17558818252270267</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="19"/>
+        <v>-2.662566427070868</v>
+      </c>
+      <c r="AW15" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.46180150157556626</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="21"/>
+        <v>9.7115579058304107</v>
+      </c>
+      <c r="AY15" s="2">
         <f t="shared" si="12"/>
-        <v>1.5145988489051443</v>
-      </c>
-      <c r="AS15">
-        <f t="shared" si="16"/>
-        <v>3.4206377166776081</v>
-      </c>
-      <c r="AT15" s="1">
-        <f t="shared" si="17"/>
-        <v>0.69379371110170596</v>
-      </c>
-      <c r="AU15">
-        <f t="shared" si="18"/>
-        <v>-2.5838175431944244</v>
-      </c>
-      <c r="AV15" s="1">
-        <f t="shared" si="19"/>
-        <v>-0.56658961547596431</v>
-      </c>
-      <c r="AW15">
-        <f t="shared" si="20"/>
-        <v>9.6401231701029726</v>
-      </c>
-      <c r="AX15" s="2">
-        <f t="shared" si="13"/>
         <v>647.67332194384869</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>31.505757123799999</v>
       </c>
@@ -3239,66 +3294,70 @@
         <v>0.76886450846672505</v>
       </c>
       <c r="AJ16" s="2">
-        <f t="shared" si="10"/>
-        <v>0.65041534995876793</v>
-      </c>
-      <c r="AK16">
+        <f t="shared" si="13"/>
+        <v>0.39948611813446039</v>
+      </c>
+      <c r="AK16" s="2">
+        <f t="shared" si="14"/>
+        <v>0.54258527727921491</v>
+      </c>
+      <c r="AL16">
         <f t="shared" si="2"/>
         <v>381694.40478300001</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <f t="shared" si="3"/>
         <v>481797.63894000003</v>
       </c>
-      <c r="AM16" s="3">
-        <f t="shared" si="14"/>
-        <v>-1.0169102311700138</v>
-      </c>
-      <c r="AN16">
+      <c r="AN16" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.73042721724362403</v>
+      </c>
+      <c r="AO16">
         <f t="shared" si="4"/>
-        <v>-0.30120721151377106</v>
-      </c>
-      <c r="AO16" s="3">
+        <v>-0.38486962475879805</v>
+      </c>
+      <c r="AP16" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP16" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ16" s="2">
+        <f t="shared" si="16"/>
         <v>1.2622601560374207</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="AR16" s="2">
+        <f t="shared" si="10"/>
+        <v>-4.5002252570947733E-2</v>
+      </c>
+      <c r="AS16" s="2">
         <f t="shared" si="11"/>
-        <v>-0.31401907515008953</v>
-      </c>
-      <c r="AR16" s="2">
+        <v>1.5312769786165625</v>
+      </c>
+      <c r="AT16">
+        <f t="shared" si="17"/>
+        <v>3.179141188060258</v>
+      </c>
+      <c r="AU16" s="1">
+        <f t="shared" si="18"/>
+        <v>0.27005571100398773</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" si="19"/>
+        <v>-2.3925107160668801</v>
+      </c>
+      <c r="AW16" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.67600774781638684</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" si="21"/>
+        <v>9.0355501580140238</v>
+      </c>
+      <c r="AY16" s="2">
         <f t="shared" si="12"/>
-        <v>1.5312769786165625</v>
-      </c>
-      <c r="AS16">
-        <f t="shared" si="16"/>
-        <v>3.179141188060258</v>
-      </c>
-      <c r="AT16" s="1">
-        <f t="shared" si="17"/>
-        <v>0.5560032378663774</v>
-      </c>
-      <c r="AU16">
-        <f t="shared" si="18"/>
-        <v>-2.0278143053280471</v>
-      </c>
-      <c r="AV16" s="1">
-        <f t="shared" si="19"/>
-        <v>-0.72314852843859712</v>
-      </c>
-      <c r="AW16">
-        <f t="shared" si="20"/>
-        <v>8.9169746416643747</v>
-      </c>
-      <c r="AX16" s="2">
-        <f t="shared" si="13"/>
         <v>566.88055710714389</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>32.253108226000002</v>
       </c>
@@ -3413,66 +3472,70 @@
         <v>0.40975794727305237</v>
       </c>
       <c r="AJ17" s="2">
-        <f t="shared" si="10"/>
-        <v>0.65527386653846997</v>
-      </c>
-      <c r="AK17">
+        <f t="shared" si="13"/>
+        <v>0.40439548791344437</v>
+      </c>
+      <c r="AK17" s="2">
+        <f t="shared" si="14"/>
+        <v>0.18541614306463217</v>
+      </c>
+      <c r="AL17">
         <f t="shared" si="2"/>
         <v>388242.81343566667</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <f t="shared" si="3"/>
         <v>488492.35904600006</v>
       </c>
-      <c r="AM17" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.73728937620424428</v>
-      </c>
-      <c r="AN17">
+      <c r="AN17" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.73370017621927242</v>
+      </c>
+      <c r="AO17">
         <f t="shared" si="4"/>
-        <v>-0.38479944977878094</v>
-      </c>
-      <c r="AO17" s="3">
+        <v>-0.38613649504026959</v>
+      </c>
+      <c r="AP17" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP17" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ17" s="2">
+        <f t="shared" si="16"/>
         <v>1.2582135255079103</v>
       </c>
-      <c r="AQ17" s="2">
+      <c r="AR17" s="2">
+        <f t="shared" si="10"/>
+        <v>-4.0047985741661261E-2</v>
+      </c>
+      <c r="AS17" s="2">
         <f t="shared" si="11"/>
-        <v>-0.31612827870050997</v>
-      </c>
-      <c r="AR17" s="2">
+        <v>1.5342938184667589</v>
+      </c>
+      <c r="AT17">
+        <f t="shared" si="17"/>
+        <v>3.1671086736532548</v>
+      </c>
+      <c r="AU17" s="1">
+        <f t="shared" si="18"/>
+        <v>-5.1247507020115123E-2</v>
+      </c>
+      <c r="AV17">
+        <f t="shared" si="19"/>
+        <v>-2.4437582230869954</v>
+      </c>
+      <c r="AW17" s="1">
+        <f t="shared" si="20"/>
+        <v>0.12672620875306101</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" si="21"/>
+        <v>9.1622763667670846</v>
+      </c>
+      <c r="AY17" s="2">
         <f t="shared" si="12"/>
-        <v>1.5342938184667589</v>
-      </c>
-      <c r="AS17">
-        <f t="shared" si="16"/>
-        <v>3.1671086736532548</v>
-      </c>
-      <c r="AT17" s="1">
-        <f t="shared" si="17"/>
-        <v>-5.1961185798771473E-2</v>
-      </c>
-      <c r="AU17">
-        <f t="shared" si="18"/>
-        <v>-2.0797754911268185</v>
-      </c>
-      <c r="AV17" s="1">
-        <f t="shared" si="19"/>
-        <v>0.12680946433028142</v>
-      </c>
-      <c r="AW17">
-        <f t="shared" si="20"/>
-        <v>9.0437841059946553</v>
-      </c>
-      <c r="AX17" s="2">
-        <f t="shared" si="13"/>
         <v>578.54192788211469</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31.807406181800001</v>
       </c>
@@ -3587,66 +3650,70 @@
         <v>0.69199875382271969</v>
       </c>
       <c r="AJ18" s="2">
-        <f t="shared" si="10"/>
-        <v>0.71602881115130135</v>
-      </c>
-      <c r="AK18">
+        <f t="shared" si="13"/>
+        <v>0.4178489578328618</v>
+      </c>
+      <c r="AK18" s="2">
+        <f t="shared" si="14"/>
+        <v>0.46104526928196221</v>
+      </c>
+      <c r="AL18">
         <f t="shared" si="2"/>
         <v>366378.21504033334</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <f t="shared" si="3"/>
         <v>442908.0974035</v>
       </c>
-      <c r="AM18" s="3">
-        <f t="shared" si="14"/>
-        <v>-0.94973898192356077</v>
-      </c>
-      <c r="AN18">
+      <c r="AN18" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.74273306499656055</v>
+      </c>
+      <c r="AO18">
         <f t="shared" si="4"/>
-        <v>-0.34455398161993511</v>
-      </c>
-      <c r="AO18" s="3">
+        <v>-0.4144603104006726</v>
+      </c>
+      <c r="AP18" s="3">
         <v>40798.57518375088</v>
       </c>
-      <c r="AP18" s="2">
-        <f t="shared" si="15"/>
+      <c r="AQ18" s="2">
+        <f t="shared" si="16"/>
         <v>1.2088821857346015</v>
       </c>
-      <c r="AQ18" s="2">
+      <c r="AR18" s="2">
+        <f t="shared" si="10"/>
+        <v>-3.5097342046234221E-2</v>
+      </c>
+      <c r="AS18" s="2">
         <f t="shared" si="11"/>
-        <v>-0.37207129880615608</v>
-      </c>
-      <c r="AR18" s="2">
+        <v>1.5458561424945232</v>
+      </c>
+      <c r="AT18">
+        <f t="shared" si="17"/>
+        <v>3.0247950907077668</v>
+      </c>
+      <c r="AU18" s="1">
+        <f t="shared" si="18"/>
+        <v>0.16819821458626852</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" si="19"/>
+        <v>-2.2755600085007268</v>
+      </c>
+      <c r="AW18" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.40253352660878777</v>
+      </c>
+      <c r="AX18">
+        <f t="shared" si="21"/>
+        <v>8.759742840158296</v>
+      </c>
+      <c r="AY18" s="2">
         <f t="shared" si="12"/>
-        <v>1.5458561424945232</v>
-      </c>
-      <c r="AS18">
-        <f t="shared" si="16"/>
-        <v>3.0247950907077668</v>
-      </c>
-      <c r="AT18" s="1">
-        <f t="shared" si="17"/>
-        <v>0.29316164062004629</v>
-      </c>
-      <c r="AU18">
-        <f t="shared" si="18"/>
-        <v>-1.7866138505067721</v>
-      </c>
-      <c r="AV18" s="1">
-        <f t="shared" si="19"/>
-        <v>-0.42364475224929393</v>
-      </c>
-      <c r="AW18">
-        <f t="shared" si="20"/>
-        <v>8.6201393537453619</v>
-      </c>
-      <c r="AX18" s="2">
-        <f t="shared" si="13"/>
         <v>530.66581098199913</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>31.567336453999999</v>
       </c>
@@ -3733,7 +3800,7 @@
         <v>-8.4108845215175485</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31.4068883148</v>
       </c>
@@ -3820,7 +3887,7 @@
         <v>-8.9525746769235415</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31.270712094699999</v>
       </c>
@@ -3907,7 +3974,7 @@
         <v>-9.3346573756835518</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>31.137649633700001</v>
       </c>

</xml_diff>

<commit_message>
Analytical solution succeed, but volumetric strain prediction is not so good.
</commit_message>
<xml_diff>
--- a/SMP_0.5PP.xlsx
+++ b/SMP_0.5PP.xlsx
@@ -240,12 +240,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY22"/>
+  <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1:AN1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1003,8 +1004,8 @@
         <f t="shared" si="4"/>
         <v>-0.42899156719796372</v>
       </c>
-      <c r="AP3" s="1">
-        <v>40798.57518375088</v>
+      <c r="AP3" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ3" s="2">
         <f>AM3/AL3</f>
@@ -1024,19 +1025,19 @@
       </c>
       <c r="AU3" s="1">
         <f>(1+2*AN3)*(AL3-AL2)*(1-AQ3/3)/(3*AO3*AP3*AN3)</f>
-        <v>4.7427059605727592E-3</v>
+        <v>5.0092908674774219E-3</v>
       </c>
       <c r="AV3" s="1">
         <f>(AV2+AU3)</f>
-        <v>4.7427059605727592E-3</v>
+        <v>5.0092908674774219E-3</v>
       </c>
       <c r="AW3" s="1">
         <f>2*(1-AN3)*(AL3-AL2)*(1-AQ3/3)/(9*AO3*AP3*AN3)</f>
-        <v>0.36682728460913289</v>
+        <v>0.38744644555450292</v>
       </c>
       <c r="AX3" s="1">
         <f>AX2+AW3</f>
-        <v>0.36682728460913289</v>
+        <v>0.38744644555450292</v>
       </c>
       <c r="AY3" s="2">
         <f t="shared" ref="AY3:AY18" si="12">(AT3*X3-4*X3*(1-0.01*P3-2*0.01*AF3)*(0.08/0.4)/(-0.08/0.4*0.01*P3-(2*0.08/0.4+3)*0.01*AF3+0.08/0.4+1))/1000</f>
@@ -1158,7 +1159,7 @@
         <v>0.16424718930868293</v>
       </c>
       <c r="AJ4" s="2">
-        <f t="shared" ref="AJ4:AJ22" si="13">-(1.35-(1.35*(AL4/3255000)^-0.0723))+0.2354+1.382*AR4</f>
+        <f t="shared" ref="AJ4:AJ18" si="13">-(1.35-(1.35*(AL4/3255000)^-0.0723))+0.2354+1.382*AR4</f>
         <v>0.13716108102294489</v>
       </c>
       <c r="AK4" s="2">
@@ -1181,8 +1182,8 @@
         <f t="shared" si="4"/>
         <v>-0.3519381325233058</v>
       </c>
-      <c r="AP4" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP4" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ4" s="2">
         <f t="shared" ref="AQ4:AQ18" si="16">AM4/AL4</f>
@@ -1202,19 +1203,19 @@
       </c>
       <c r="AU4" s="1">
         <f t="shared" ref="AU4:AU18" si="18">(1+2*AN4)*(AL4-AL3)*(1-AQ4/3)/(3*AO4*AP4*AN4)</f>
-        <v>-9.633429338296641E-2</v>
+        <v>-0.10174919130131072</v>
       </c>
       <c r="AV4">
         <f t="shared" ref="AV4:AV18" si="19">AV3+AU4</f>
-        <v>-9.159158742239365E-2</v>
+        <v>-9.6739900433833292E-2</v>
       </c>
       <c r="AW4" s="1">
         <f t="shared" ref="AW4:AW18" si="20">2*(1-AN4)*(AL4-AL3)*(1-AQ4/3)/(9*AO4*AP4*AN4)</f>
-        <v>0.70234422668957619</v>
+        <v>0.74182261135933891</v>
       </c>
       <c r="AX4">
         <f>AX3+AW4</f>
-        <v>1.069171511298709</v>
+        <v>1.1292690569138419</v>
       </c>
       <c r="AY4" s="2">
         <f t="shared" si="12"/>
@@ -1359,8 +1360,8 @@
         <f t="shared" si="4"/>
         <v>-0.32196837616875357</v>
       </c>
-      <c r="AP5" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP5" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ5" s="2">
         <f t="shared" si="16"/>
@@ -1380,19 +1381,19 @@
       </c>
       <c r="AU5" s="1">
         <f t="shared" si="18"/>
-        <v>-0.19238470260591006</v>
+        <v>-0.20319854146930103</v>
       </c>
       <c r="AV5">
         <f t="shared" si="19"/>
-        <v>-0.28397629002830371</v>
+        <v>-0.29993844190313435</v>
       </c>
       <c r="AW5" s="1">
         <f t="shared" si="20"/>
-        <v>0.90278505431633316</v>
+        <v>0.95353010822871531</v>
       </c>
       <c r="AX5">
         <f>AX4+AW5</f>
-        <v>1.9719565656150422</v>
+        <v>2.082799165142557</v>
       </c>
       <c r="AY5" s="2">
         <f t="shared" si="12"/>
@@ -1537,8 +1538,8 @@
         <f t="shared" si="4"/>
         <v>-0.30377935487388319</v>
       </c>
-      <c r="AP6" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP6" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ6" s="2">
         <f t="shared" si="16"/>
@@ -1558,19 +1559,19 @@
       </c>
       <c r="AU6" s="1">
         <f t="shared" si="18"/>
-        <v>-0.27493393099282515</v>
+        <v>-0.29038781681411774</v>
       </c>
       <c r="AV6">
         <f t="shared" si="19"/>
-        <v>-0.55891022102112886</v>
+        <v>-0.59032625871725208</v>
       </c>
       <c r="AW6" s="1">
         <f t="shared" si="20"/>
-        <v>1.0551851461552919</v>
+        <v>1.1144965258388471</v>
       </c>
       <c r="AX6">
         <f t="shared" ref="AX6:AX18" si="21">AX5+AW6</f>
-        <v>3.0271417117703341</v>
+        <v>3.1972956909814041</v>
       </c>
       <c r="AY6" s="2">
         <f t="shared" si="12"/>
@@ -1715,8 +1716,8 @@
         <f t="shared" si="4"/>
         <v>-0.29340824324090536</v>
       </c>
-      <c r="AP7" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP7" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ7" s="2">
         <f t="shared" si="16"/>
@@ -1736,19 +1737,19 @@
       </c>
       <c r="AU7" s="1">
         <f t="shared" si="18"/>
-        <v>-0.31540924250029956</v>
+        <v>-0.33313822343393051</v>
       </c>
       <c r="AV7">
         <f t="shared" si="19"/>
-        <v>-0.87431946352142842</v>
+        <v>-0.9234644821511826</v>
       </c>
       <c r="AW7" s="1">
         <f t="shared" si="20"/>
-        <v>1.0966330729785276</v>
+        <v>1.1582742179491192</v>
       </c>
       <c r="AX7">
         <f t="shared" si="21"/>
-        <v>4.1237747847488615</v>
+        <v>4.3555699089305229</v>
       </c>
       <c r="AY7" s="2">
         <f t="shared" si="12"/>
@@ -1893,8 +1894,8 @@
         <f t="shared" si="4"/>
         <v>-0.28805590302797707</v>
       </c>
-      <c r="AP8" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP8" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ8" s="2">
         <f t="shared" si="16"/>
@@ -1914,19 +1915,19 @@
       </c>
       <c r="AU8" s="1">
         <f t="shared" si="18"/>
-        <v>-0.35301408447238236</v>
+        <v>-0.37285681299644619</v>
       </c>
       <c r="AV8">
         <f t="shared" si="19"/>
-        <v>-1.2273335479938108</v>
+        <v>-1.2963212951476288</v>
       </c>
       <c r="AW8" s="1">
         <f t="shared" si="20"/>
-        <v>1.1539407983813592</v>
+        <v>1.2188031792388974</v>
       </c>
       <c r="AX8">
         <f t="shared" si="21"/>
-        <v>5.2777155831302203</v>
+        <v>5.5743730881694198</v>
       </c>
       <c r="AY8" s="2">
         <f t="shared" si="12"/>
@@ -2071,8 +2072,8 @@
         <f t="shared" si="4"/>
         <v>-0.28604849626521334</v>
       </c>
-      <c r="AP9" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP9" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ9" s="2">
         <f t="shared" si="16"/>
@@ -2092,19 +2093,19 @@
       </c>
       <c r="AU9" s="1">
         <f t="shared" si="18"/>
-        <v>-0.3705638200463337</v>
+        <v>-0.39139300960405143</v>
       </c>
       <c r="AV9">
         <f t="shared" si="19"/>
-        <v>-1.5978973680401445</v>
+        <v>-1.6877143047516803</v>
       </c>
       <c r="AW9" s="1">
         <f t="shared" si="20"/>
-        <v>1.1690952097246072</v>
+        <v>1.2348094117514776</v>
       </c>
       <c r="AX9">
         <f t="shared" si="21"/>
-        <v>6.4468107928548273</v>
+        <v>6.8091824999208974</v>
       </c>
       <c r="AY9" s="2">
         <f t="shared" si="12"/>
@@ -2249,8 +2250,8 @@
         <f t="shared" si="4"/>
         <v>-0.28503761272927297</v>
       </c>
-      <c r="AP10" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP10" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ10" s="2">
         <f t="shared" si="16"/>
@@ -2270,19 +2271,19 @@
       </c>
       <c r="AU10" s="1">
         <f t="shared" si="18"/>
-        <v>-0.3776425553857754</v>
+        <v>-0.39886963678354292</v>
       </c>
       <c r="AV10">
         <f t="shared" si="19"/>
-        <v>-1.9755399234259199</v>
+        <v>-2.0865839415352232</v>
       </c>
       <c r="AW10" s="1">
         <f t="shared" si="20"/>
-        <v>1.1616728842160089</v>
+        <v>1.2269698813874286</v>
       </c>
       <c r="AX10">
         <f t="shared" si="21"/>
-        <v>7.6084836770708364</v>
+        <v>8.0361523813083267</v>
       </c>
       <c r="AY10" s="2">
         <f t="shared" si="12"/>
@@ -2427,8 +2428,8 @@
         <f t="shared" si="4"/>
         <v>-0.28692985402617949</v>
       </c>
-      <c r="AP11" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP11" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ11" s="2">
         <f t="shared" si="16"/>
@@ -2448,19 +2449,19 @@
       </c>
       <c r="AU11" s="1">
         <f t="shared" si="18"/>
-        <v>-0.3630246395685261</v>
+        <v>-0.38343005591691526</v>
       </c>
       <c r="AV11">
         <f t="shared" si="19"/>
-        <v>-2.338564562994446</v>
+        <v>-2.4700139974521385</v>
       </c>
       <c r="AW11" s="1">
         <f t="shared" si="20"/>
-        <v>1.096100033040375</v>
+        <v>1.1577112161277148</v>
       </c>
       <c r="AX11">
         <f t="shared" si="21"/>
-        <v>8.704583710111212</v>
+        <v>9.1938635974360423</v>
       </c>
       <c r="AY11" s="2">
         <f t="shared" si="12"/>
@@ -2605,8 +2606,8 @@
         <f t="shared" si="4"/>
         <v>-0.29187356348233073</v>
       </c>
-      <c r="AP12" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP12" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ12" s="2">
         <f t="shared" si="16"/>
@@ -2626,19 +2627,19 @@
       </c>
       <c r="AU12" s="1">
         <f t="shared" si="18"/>
-        <v>-0.3294016018343443</v>
+        <v>-0.34791708562972817</v>
       </c>
       <c r="AV12">
         <f t="shared" si="19"/>
-        <v>-2.6679661648287905</v>
+        <v>-2.8179310830818665</v>
       </c>
       <c r="AW12" s="1">
         <f t="shared" si="20"/>
-        <v>0.97993888506230964</v>
+        <v>1.0350207135834786</v>
       </c>
       <c r="AX12">
         <f t="shared" si="21"/>
-        <v>9.6845225951735223</v>
+        <v>10.22888431101952</v>
       </c>
       <c r="AY12" s="2">
         <f t="shared" si="12"/>
@@ -2783,8 +2784,8 @@
         <f t="shared" si="4"/>
         <v>-0.30302327242107752</v>
       </c>
-      <c r="AP13" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP13" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ13" s="2">
         <f t="shared" si="16"/>
@@ -2804,19 +2805,19 @@
       </c>
       <c r="AU13" s="1">
         <f t="shared" si="18"/>
-        <v>-0.15037494992411293</v>
+        <v>-0.15882744357638048</v>
       </c>
       <c r="AV13">
         <f t="shared" si="19"/>
-        <v>-2.8183411147529034</v>
+        <v>-2.976758526658247</v>
       </c>
       <c r="AW13" s="1">
         <f t="shared" si="20"/>
-        <v>0.43382142040196658</v>
+        <v>0.45820628506204347</v>
       </c>
       <c r="AX13">
         <f t="shared" si="21"/>
-        <v>10.118344015575488</v>
+        <v>10.687090596081564</v>
       </c>
       <c r="AY13" s="2">
         <f t="shared" si="12"/>
@@ -2961,8 +2962,8 @@
         <f t="shared" si="4"/>
         <v>-0.3185442642030018</v>
       </c>
-      <c r="AP14" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP14" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ14" s="2">
         <f t="shared" si="16"/>
@@ -2982,19 +2983,19 @@
       </c>
       <c r="AU14" s="1">
         <f t="shared" si="18"/>
-        <v>-1.9813494840667002E-2</v>
+        <v>-2.0927200544007159E-2</v>
       </c>
       <c r="AV14">
         <f t="shared" si="19"/>
-        <v>-2.8381546095935706</v>
+        <v>-2.9976857272022541</v>
       </c>
       <c r="AW14" s="1">
         <f t="shared" si="20"/>
-        <v>5.5015391830488841E-2</v>
+        <v>5.8107776901665215E-2</v>
       </c>
       <c r="AX14">
         <f t="shared" si="21"/>
-        <v>10.173359407405977</v>
+        <v>10.745198372983229</v>
       </c>
       <c r="AY14" s="2">
         <f t="shared" si="12"/>
@@ -3139,8 +3140,8 @@
         <f t="shared" si="4"/>
         <v>-0.34495336502006951</v>
       </c>
-      <c r="AP15" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP15" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ15" s="2">
         <f t="shared" si="16"/>
@@ -3160,19 +3161,19 @@
       </c>
       <c r="AU15" s="1">
         <f t="shared" si="18"/>
-        <v>0.17558818252270267</v>
+        <v>0.18545789818302597</v>
       </c>
       <c r="AV15">
         <f t="shared" si="19"/>
-        <v>-2.662566427070868</v>
+        <v>-2.812227829019228</v>
       </c>
       <c r="AW15" s="1">
         <f t="shared" si="20"/>
-        <v>-0.46180150157556626</v>
+        <v>-0.48775911128812122</v>
       </c>
       <c r="AX15">
         <f t="shared" si="21"/>
-        <v>9.7115579058304107</v>
+        <v>10.257439261695108</v>
       </c>
       <c r="AY15" s="2">
         <f t="shared" si="12"/>
@@ -3317,8 +3318,8 @@
         <f t="shared" si="4"/>
         <v>-0.38486962475879805</v>
       </c>
-      <c r="AP16" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP16" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ16" s="2">
         <f t="shared" si="16"/>
@@ -3338,19 +3339,19 @@
       </c>
       <c r="AU16" s="1">
         <f t="shared" si="18"/>
-        <v>0.27005571100398773</v>
+        <v>0.28523539474899817</v>
       </c>
       <c r="AV16">
         <f t="shared" si="19"/>
-        <v>-2.3925107160668801</v>
+        <v>-2.5269924342702299</v>
       </c>
       <c r="AW16" s="1">
         <f t="shared" si="20"/>
-        <v>-0.67600774781638684</v>
+        <v>-0.71400577341962246</v>
       </c>
       <c r="AX16">
         <f t="shared" si="21"/>
-        <v>9.0355501580140238</v>
+        <v>9.5434334882754861</v>
       </c>
       <c r="AY16" s="2">
         <f t="shared" si="12"/>
@@ -3495,8 +3496,8 @@
         <f t="shared" si="4"/>
         <v>-0.38613649504026959</v>
       </c>
-      <c r="AP17" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP17" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ17" s="2">
         <f t="shared" si="16"/>
@@ -3516,19 +3517,19 @@
       </c>
       <c r="AU17" s="1">
         <f t="shared" si="18"/>
-        <v>-5.1247507020115123E-2</v>
+        <v>-5.4128101347831671E-2</v>
       </c>
       <c r="AV17">
         <f t="shared" si="19"/>
-        <v>-2.4437582230869954</v>
+        <v>-2.5811205356180618</v>
       </c>
       <c r="AW17" s="1">
         <f t="shared" si="20"/>
-        <v>0.12672620875306101</v>
+        <v>0.13384941960434801</v>
       </c>
       <c r="AX17">
         <f t="shared" si="21"/>
-        <v>9.1622763667670846</v>
+        <v>9.6772829078798335</v>
       </c>
       <c r="AY17" s="2">
         <f t="shared" si="12"/>
@@ -3673,8 +3674,8 @@
         <f t="shared" si="4"/>
         <v>-0.4144603104006726</v>
       </c>
-      <c r="AP18" s="3">
-        <v>40798.57518375088</v>
+      <c r="AP18" s="5">
+        <v>38627.352818162799</v>
       </c>
       <c r="AQ18" s="2">
         <f t="shared" si="16"/>
@@ -3694,19 +3695,19 @@
       </c>
       <c r="AU18" s="1">
         <f t="shared" si="18"/>
-        <v>0.16819821458626852</v>
+        <v>0.1776525441925669</v>
       </c>
       <c r="AV18">
         <f t="shared" si="19"/>
-        <v>-2.2755600085007268</v>
+        <v>-2.4034679914254951</v>
       </c>
       <c r="AW18" s="1">
         <f t="shared" si="20"/>
-        <v>-0.40253352660878777</v>
+        <v>-0.42515971587902668</v>
       </c>
       <c r="AX18">
         <f t="shared" si="21"/>
-        <v>8.759742840158296</v>
+        <v>9.2521231920008074</v>
       </c>
       <c r="AY18" s="2">
         <f t="shared" si="12"/>
@@ -4059,6 +4060,12 @@
       <c r="AB22">
         <f t="shared" si="0"/>
         <v>-9.8293447096183151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="W23" s="2">
+        <f>MIN(W2:W22)</f>
+        <v>4.2173620645199996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>